<commit_message>
setup for functional forms
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDDE781-0B28-4B08-B31D-0157BA5D16BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2346EEB3-015B-45AD-BCB9-F557B0618006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -808,7 +808,7 @@
   <dimension ref="A1:AG18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bugfix and functional form range
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0B12F9-2A8D-461D-9148-B9DF636D3695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58E7D0D-AC6B-418E-8CFE-753DB4EBEEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="135">
   <si>
     <t>Poisson</t>
   </si>
@@ -198,12 +198,6 @@
     <t>$ \\tilde{E}(y) =\\tilde{\\lambda} = \\bar{Y}$</t>
   </si>
   <si>
-    <t>optimMethod</t>
-  </si>
-  <si>
-    <t>Nelder-Mead</t>
-  </si>
-  <si>
     <t>c(.3)</t>
   </si>
   <si>
@@ -324,9 +318,6 @@
     <t>sigmaScale</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>c(-2,2)</t>
   </si>
   <si>
@@ -336,9 +327,6 @@
     <t>c("Beta0", "Beta1", "Beta2","Gamma")</t>
   </si>
   <si>
-    <t>testParams</t>
-  </si>
-  <si>
     <t>c(-1,2)</t>
   </si>
   <si>
@@ -445,6 +433,12 @@
   </si>
   <si>
     <t>c(-1,-1.5,.25, 2,-1)</t>
+  </si>
+  <si>
+    <t>funcFormRange</t>
+  </si>
+  <si>
+    <t>c(-10,10)</t>
   </si>
 </sst>
 </file>
@@ -811,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:AG18"/>
+  <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="Q9" sqref="Q9:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,24 +823,22 @@
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="31.140625" customWidth="1"/>
     <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="17" width="9.42578125" customWidth="1"/>
     <col min="18" max="18" width="6.140625" customWidth="1"/>
     <col min="19" max="19" width="4.28515625" customWidth="1"/>
     <col min="20" max="21" width="7.140625" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6" customWidth="1"/>
-    <col min="24" max="25" width="4.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16" customWidth="1"/>
-    <col min="27" max="28" width="26" customWidth="1"/>
-    <col min="29" max="29" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="15.5703125" customWidth="1"/>
+    <col min="22" max="22" width="6" customWidth="1"/>
+    <col min="23" max="24" width="4.28515625" customWidth="1"/>
+    <col min="25" max="25" width="16" customWidth="1"/>
+    <col min="26" max="27" width="26" customWidth="1"/>
+    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -860,10 +852,10 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
@@ -890,64 +882,61 @@
         <v>41</v>
       </c>
       <c r="O1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="P1" t="s">
         <v>71</v>
       </c>
       <c r="Q1" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="R1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" t="s">
         <v>58</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>59</v>
       </c>
-      <c r="U1" t="s">
-        <v>95</v>
-      </c>
-      <c r="V1" t="s">
-        <v>100</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>60</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" t="s">
-        <v>62</v>
-      </c>
       <c r="Z1" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="AA1" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="AB1" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="AC1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AD1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AE1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AF1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AG1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -970,10 +959,10 @@
         <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>46</v>
@@ -991,13 +980,13 @@
         <v>44</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="R2" s="1">
         <v>0</v>
@@ -1006,59 +995,56 @@
         <v>1</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W2">
+        <v>70</v>
+      </c>
+      <c r="V2">
         <v>0.01</v>
       </c>
-      <c r="X2" t="str">
+      <c r="W2" t="str">
         <f>"""&amp;"&amp;RIGHT(L2,LEN(L2)-1)&amp;";"""</f>
         <v>"&amp;pi;"</v>
       </c>
+      <c r="X2" t="str">
+        <f>IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
       <c r="Y2" t="str">
-        <f t="shared" ref="Y2:Y18" si="0">IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
-        <v>"none"</v>
+        <f>"manyParamSliderMaker(minVal ="&amp;R2&amp;", maxVal = "&amp;S2&amp;", startVals = "&amp;T2&amp;", stepVal = "&amp;V2&amp;", paramHTML = "&amp;W2&amp;", multi = "&amp;X2&amp;", sigmaScale ="&amp;U2&amp;","</f>
+        <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z2" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;R2&amp;", maxVal = "&amp;S2&amp;", startVals = "&amp;T2&amp;", stepVal = "&amp;W2&amp;", paramHTML = "&amp;X2&amp;", multi = "&amp;Y2&amp;", sigmaScale ="&amp;U2&amp;","</f>
-        <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AA2" t="str">
         <f>$B2&amp;"ParamTransform"</f>
         <v>bernParamTransform</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AA2" t="str">
         <f>$B2&amp;"PDF"</f>
         <v>bernPDF</v>
       </c>
+      <c r="AB2" t="str">
+        <f>B2&amp;"PlotDistr"</f>
+        <v>bernPlotDistr</v>
+      </c>
       <c r="AC2" t="str">
-        <f t="shared" ref="AC2:AC18" si="1">B2&amp;"PlotDistr"</f>
-        <v>bernPlotDistr</v>
+        <f>B2&amp;"Draws"</f>
+        <v>bernDraws</v>
       </c>
       <c r="AD2" t="str">
-        <f t="shared" ref="AD2:AD18" si="2">B2&amp;"Draws"</f>
-        <v>bernDraws</v>
+        <f>B2&amp;"Latex"</f>
+        <v>bernLatex</v>
       </c>
       <c r="AE2" t="str">
-        <f t="shared" ref="AE2:AE18" si="3">B2&amp;"Latex"</f>
-        <v>bernLatex</v>
-      </c>
-      <c r="AF2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="AG2" t="str">
+      <c r="AF2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1066,7 +1052,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -1081,10 +1067,10 @@
         <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>47</v>
@@ -1102,13 +1088,13 @@
         <v>44</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="R3" s="1">
         <v>-2</v>
@@ -1117,59 +1103,56 @@
         <v>2</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W3">
+        <v>70</v>
+      </c>
+      <c r="V3">
         <v>0.01</v>
       </c>
+      <c r="W3" t="str">
+        <f>"""&amp;"&amp;RIGHT(L3,LEN(L3)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X3" t="str">
-        <f t="shared" ref="X3:X16" si="4">"""&amp;"&amp;RIGHT(L3,LEN(L3)-1)&amp;";"""</f>
-        <v>"&amp;beta;"</v>
+        <f>IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
       </c>
       <c r="Y3" t="str">
-        <f t="shared" si="0"/>
-        <v>"none"</v>
+        <f>"manyParamSliderMaker(minVal ="&amp;R3&amp;", maxVal = "&amp;S3&amp;", startVals = "&amp;T3&amp;", stepVal = "&amp;V3&amp;", paramHTML = "&amp;W3&amp;", multi = "&amp;X3&amp;", sigmaScale ="&amp;U3&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z3" t="str">
-        <f t="shared" ref="Z3:Z18" si="5">"manyParamSliderMaker(minVal ="&amp;R3&amp;", maxVal = "&amp;S3&amp;", startVals = "&amp;T3&amp;", stepVal = "&amp;W3&amp;", paramHTML = "&amp;X3&amp;", multi = "&amp;Y3&amp;", sigmaScale ="&amp;U3&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <f t="shared" ref="Z3:Z18" si="0">$B3&amp;"ParamTransform"</f>
+        <v>bernLogitParamTransform</v>
       </c>
       <c r="AA3" t="str">
-        <f t="shared" ref="AA3:AA18" si="6">$B3&amp;"ParamTransform"</f>
-        <v>bernLogitParamTransform</v>
+        <f t="shared" ref="AA3:AA18" si="1">$B3&amp;"PDF"</f>
+        <v>bernLogitPDF</v>
       </c>
       <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB18" si="7">$B3&amp;"PDF"</f>
-        <v>bernLogitPDF</v>
+        <f>B3&amp;"PlotDistr"</f>
+        <v>bernLogitPlotDistr</v>
       </c>
       <c r="AC3" t="str">
-        <f t="shared" si="1"/>
-        <v>bernLogitPlotDistr</v>
+        <f>B3&amp;"Draws"</f>
+        <v>bernLogitDraws</v>
       </c>
       <c r="AD3" t="str">
-        <f t="shared" si="2"/>
-        <v>bernLogitDraws</v>
+        <f>B3&amp;"Latex"</f>
+        <v>bernLogitLatex</v>
       </c>
       <c r="AE3" t="str">
-        <f t="shared" si="3"/>
-        <v>bernLogitLatex</v>
+        <f t="shared" ref="AE3:AE18" si="2">$B3&amp;"ChartDomain"</f>
+        <v>bernLogitChartDomain</v>
       </c>
       <c r="AF3" t="str">
-        <f t="shared" ref="AF3:AF18" si="8">$B3&amp;"ChartDomain"</f>
-        <v>bernLogitChartDomain</v>
-      </c>
-      <c r="AG3" t="str">
-        <f t="shared" ref="AG3:AG18" si="9">$B3&amp;"LikelihoodFun"</f>
+        <f t="shared" ref="AF3:AF18" si="3">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1177,7 +1160,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -1192,10 +1175,10 @@
         <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>47</v>
@@ -1213,13 +1196,13 @@
         <v>44</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="R4" s="1">
         <v>-4</v>
@@ -1228,59 +1211,56 @@
         <v>4</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W4">
+        <v>70</v>
+      </c>
+      <c r="V4">
         <v>0.01</v>
       </c>
+      <c r="W4" t="str">
+        <f>"""&amp;"&amp;RIGHT(L4,LEN(L4)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X4" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F4=1,"""none""",IF(E4=F4,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
       </c>
       <c r="Y4" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R4&amp;", maxVal = "&amp;S4&amp;", startVals = "&amp;T4&amp;", stepVal = "&amp;V4&amp;", paramHTML = "&amp;W4&amp;", multi = "&amp;X4&amp;", sigmaScale ="&amp;U4&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="Z4" t="str">
         <f t="shared" si="0"/>
-        <v>"betas"</v>
-      </c>
-      <c r="Z4" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>bernLogitXParamTransform</v>
       </c>
       <c r="AA4" t="str">
-        <f t="shared" si="6"/>
-        <v>bernLogitXParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>bernLogitXPDF</v>
       </c>
       <c r="AB4" t="str">
-        <f t="shared" si="7"/>
-        <v>bernLogitXPDF</v>
+        <f>B4&amp;"PlotDistr"</f>
+        <v>bernLogitXPlotDistr</v>
       </c>
       <c r="AC4" t="str">
-        <f t="shared" si="1"/>
-        <v>bernLogitXPlotDistr</v>
+        <f>B4&amp;"Draws"</f>
+        <v>bernLogitXDraws</v>
       </c>
       <c r="AD4" t="str">
+        <f>B4&amp;"Latex"</f>
+        <v>bernLogitXLatex</v>
+      </c>
+      <c r="AE4" t="str">
         <f t="shared" si="2"/>
-        <v>bernLogitXDraws</v>
-      </c>
-      <c r="AE4" t="str">
+        <v>bernLogitXChartDomain</v>
+      </c>
+      <c r="AF4" t="str">
         <f t="shared" si="3"/>
-        <v>bernLogitXLatex</v>
-      </c>
-      <c r="AF4" t="str">
-        <f t="shared" si="8"/>
-        <v>bernLogitXChartDomain</v>
-      </c>
-      <c r="AG4" t="str">
-        <f t="shared" si="9"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1288,7 +1268,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
@@ -1303,10 +1283,10 @@
         <v>24</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>52</v>
@@ -1324,13 +1304,13 @@
         <v>45</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="R5" s="1">
         <v>-4</v>
@@ -1339,59 +1319,56 @@
         <v>4</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W5">
+        <v>70</v>
+      </c>
+      <c r="V5">
         <v>0.01</v>
       </c>
+      <c r="W5" t="str">
+        <f>"""&amp;"&amp;RIGHT(L5,LEN(L5)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X5" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F5=1,"""none""",IF(E5=F5,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
       </c>
       <c r="Y5" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R5&amp;", maxVal = "&amp;S5&amp;", startVals = "&amp;T5&amp;", stepVal = "&amp;V5&amp;", paramHTML = "&amp;W5&amp;", multi = "&amp;X5&amp;", sigmaScale ="&amp;U5&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="Z5" t="str">
         <f t="shared" si="0"/>
-        <v>"none"</v>
-      </c>
-      <c r="Z5" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <v>styNormParamTransform</v>
       </c>
       <c r="AA5" t="str">
-        <f t="shared" si="6"/>
-        <v>styNormParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>styNormPDF</v>
       </c>
       <c r="AB5" t="str">
-        <f t="shared" si="7"/>
-        <v>styNormPDF</v>
+        <f>B5&amp;"PlotDistr"</f>
+        <v>styNormPlotDistr</v>
       </c>
       <c r="AC5" t="str">
-        <f t="shared" si="1"/>
-        <v>styNormPlotDistr</v>
+        <f>B5&amp;"Draws"</f>
+        <v>styNormDraws</v>
       </c>
       <c r="AD5" t="str">
+        <f>B5&amp;"Latex"</f>
+        <v>styNormLatex</v>
+      </c>
+      <c r="AE5" t="str">
         <f t="shared" si="2"/>
-        <v>styNormDraws</v>
-      </c>
-      <c r="AE5" t="str">
+        <v>styNormChartDomain</v>
+      </c>
+      <c r="AF5" t="str">
         <f t="shared" si="3"/>
-        <v>styNormLatex</v>
-      </c>
-      <c r="AF5" t="str">
-        <f t="shared" si="8"/>
-        <v>styNormChartDomain</v>
-      </c>
-      <c r="AG5" t="str">
-        <f t="shared" si="9"/>
         <v>styNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1399,7 +1376,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>3</v>
@@ -1414,10 +1391,10 @@
         <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>52</v>
@@ -1435,74 +1412,71 @@
         <v>45</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="R6" s="1">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="S6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W6">
+        <v>70</v>
+      </c>
+      <c r="V6">
         <v>0.01</v>
       </c>
+      <c r="W6" t="str">
+        <f>"""&amp;"&amp;RIGHT(L6,LEN(L6)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X6" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F6=1,"""none""",IF(E6=F6,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
       </c>
       <c r="Y6" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R6&amp;", maxVal = "&amp;S6&amp;", startVals = "&amp;T6&amp;", stepVal = "&amp;V6&amp;", paramHTML = "&amp;W6&amp;", multi = "&amp;X6&amp;", sigmaScale ="&amp;U6&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,3,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="Z6" t="str">
         <f t="shared" si="0"/>
-        <v>"betas"</v>
-      </c>
-      <c r="Z6" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(-1,3,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>styNormXParamTransform</v>
       </c>
       <c r="AA6" t="str">
-        <f t="shared" si="6"/>
-        <v>styNormXParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>styNormXPDF</v>
       </c>
       <c r="AB6" t="str">
-        <f t="shared" si="7"/>
-        <v>styNormXPDF</v>
+        <f>B6&amp;"PlotDistr"</f>
+        <v>styNormXPlotDistr</v>
       </c>
       <c r="AC6" t="str">
-        <f t="shared" si="1"/>
-        <v>styNormXPlotDistr</v>
+        <f>B6&amp;"Draws"</f>
+        <v>styNormXDraws</v>
       </c>
       <c r="AD6" t="str">
+        <f>B6&amp;"Latex"</f>
+        <v>styNormXLatex</v>
+      </c>
+      <c r="AE6" t="str">
         <f t="shared" si="2"/>
-        <v>styNormXDraws</v>
-      </c>
-      <c r="AE6" t="str">
+        <v>styNormXChartDomain</v>
+      </c>
+      <c r="AF6" t="str">
         <f t="shared" si="3"/>
-        <v>styNormXLatex</v>
-      </c>
-      <c r="AF6" t="str">
-        <f t="shared" si="8"/>
-        <v>styNormXChartDomain</v>
-      </c>
-      <c r="AG6" t="str">
-        <f t="shared" si="9"/>
         <v>styNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1510,7 +1484,7 @@
         <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
@@ -1525,16 +1499,16 @@
         <v>24</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>37</v>
@@ -1546,74 +1520,71 @@
         <v>45</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="R7" s="1">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="S7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W7">
+        <v>94</v>
+      </c>
+      <c r="V7">
         <v>0.01</v>
       </c>
+      <c r="W7" t="str">
+        <f>"""&amp;"&amp;RIGHT(L7,LEN(L7)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X7" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F7=1,"""none""",IF(E7=F7,"""betas""","""fullNorm"""))</f>
+        <v>"fullNorm"</v>
       </c>
       <c r="Y7" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R7&amp;", maxVal = "&amp;S7&amp;", startVals = "&amp;T7&amp;", stepVal = "&amp;V7&amp;", paramHTML = "&amp;W7&amp;", multi = "&amp;X7&amp;", sigmaScale ="&amp;U7&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,-1.5,.25, 2,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-2,2),</v>
+      </c>
+      <c r="Z7" t="str">
         <f t="shared" si="0"/>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="Z7" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(-1,-1.5,.25, 2,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-2,2),</v>
+        <v>fullNormXParamTransform</v>
       </c>
       <c r="AA7" t="str">
-        <f t="shared" si="6"/>
-        <v>fullNormXParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>fullNormXPDF</v>
       </c>
       <c r="AB7" t="str">
-        <f t="shared" si="7"/>
-        <v>fullNormXPDF</v>
+        <f>B7&amp;"PlotDistr"</f>
+        <v>fullNormXPlotDistr</v>
       </c>
       <c r="AC7" t="str">
-        <f t="shared" si="1"/>
-        <v>fullNormXPlotDistr</v>
+        <f>B7&amp;"Draws"</f>
+        <v>fullNormXDraws</v>
       </c>
       <c r="AD7" t="str">
+        <f>B7&amp;"Latex"</f>
+        <v>fullNormXLatex</v>
+      </c>
+      <c r="AE7" t="str">
         <f t="shared" si="2"/>
-        <v>fullNormXDraws</v>
-      </c>
-      <c r="AE7" t="str">
+        <v>fullNormXChartDomain</v>
+      </c>
+      <c r="AF7" t="str">
         <f t="shared" si="3"/>
-        <v>fullNormXLatex</v>
-      </c>
-      <c r="AF7" t="str">
-        <f t="shared" si="8"/>
-        <v>fullNormXChartDomain</v>
-      </c>
-      <c r="AG7" t="str">
-        <f t="shared" si="9"/>
         <v>fullNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1621,10 +1592,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1636,10 +1607,10 @@
         <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>48</v>
@@ -1657,13 +1628,13 @@
         <v>42</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="R8" s="1">
         <v>-0.5</v>
@@ -1672,59 +1643,56 @@
         <v>0.5</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W8">
+        <v>70</v>
+      </c>
+      <c r="V8">
         <v>0.01</v>
       </c>
+      <c r="W8" t="str">
+        <f>"""&amp;"&amp;RIGHT(L8,LEN(L8)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X8" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F8=1,"""none""",IF(E8=F8,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
       </c>
       <c r="Y8" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R8&amp;", maxVal = "&amp;S8&amp;", startVals = "&amp;T8&amp;", stepVal = "&amp;V8&amp;", paramHTML = "&amp;W8&amp;", multi = "&amp;X8&amp;", sigmaScale ="&amp;U8&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="Z8" t="str">
         <f t="shared" si="0"/>
-        <v>"none"</v>
-      </c>
-      <c r="Z8" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <v>logNormParamTransform</v>
       </c>
       <c r="AA8" t="str">
-        <f t="shared" si="6"/>
-        <v>logNormParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>logNormPDF</v>
       </c>
       <c r="AB8" t="str">
-        <f t="shared" si="7"/>
-        <v>logNormPDF</v>
+        <f>B8&amp;"PlotDistr"</f>
+        <v>logNormPlotDistr</v>
       </c>
       <c r="AC8" t="str">
-        <f t="shared" si="1"/>
-        <v>logNormPlotDistr</v>
+        <f>B8&amp;"Draws"</f>
+        <v>logNormDraws</v>
       </c>
       <c r="AD8" t="str">
+        <f>B8&amp;"Latex"</f>
+        <v>logNormLatex</v>
+      </c>
+      <c r="AE8" t="str">
         <f t="shared" si="2"/>
-        <v>logNormDraws</v>
-      </c>
-      <c r="AE8" t="str">
+        <v>logNormChartDomain</v>
+      </c>
+      <c r="AF8" t="str">
         <f t="shared" si="3"/>
-        <v>logNormLatex</v>
-      </c>
-      <c r="AF8" t="str">
-        <f t="shared" si="8"/>
-        <v>logNormChartDomain</v>
-      </c>
-      <c r="AG8" t="str">
-        <f t="shared" si="9"/>
         <v>logNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1732,10 +1700,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
@@ -1747,10 +1715,10 @@
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>48</v>
@@ -1768,13 +1736,13 @@
         <v>49</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="R9" s="1">
         <v>-0.5</v>
@@ -1783,59 +1751,56 @@
         <v>0.5</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W9">
+        <v>70</v>
+      </c>
+      <c r="V9">
         <v>0.01</v>
       </c>
+      <c r="W9" t="str">
+        <f>"""&amp;"&amp;RIGHT(L9,LEN(L9)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X9" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F9=1,"""none""",IF(E9=F9,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
       </c>
       <c r="Y9" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R9&amp;", maxVal = "&amp;S9&amp;", startVals = "&amp;T9&amp;", stepVal = "&amp;V9&amp;", paramHTML = "&amp;W9&amp;", multi = "&amp;X9&amp;", sigmaScale ="&amp;U9&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="Z9" t="str">
         <f t="shared" si="0"/>
-        <v>"betas"</v>
-      </c>
-      <c r="Z9" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>logNormXParamTransform</v>
       </c>
       <c r="AA9" t="str">
-        <f t="shared" si="6"/>
-        <v>logNormXParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>logNormXPDF</v>
       </c>
       <c r="AB9" t="str">
-        <f t="shared" si="7"/>
-        <v>logNormXPDF</v>
+        <f>B9&amp;"PlotDistr"</f>
+        <v>logNormXPlotDistr</v>
       </c>
       <c r="AC9" t="str">
-        <f t="shared" si="1"/>
-        <v>logNormXPlotDistr</v>
+        <f>B9&amp;"Draws"</f>
+        <v>logNormXDraws</v>
       </c>
       <c r="AD9" t="str">
+        <f>B9&amp;"Latex"</f>
+        <v>logNormXLatex</v>
+      </c>
+      <c r="AE9" t="str">
         <f t="shared" si="2"/>
-        <v>logNormXDraws</v>
-      </c>
-      <c r="AE9" t="str">
+        <v>logNormXChartDomain</v>
+      </c>
+      <c r="AF9" t="str">
         <f t="shared" si="3"/>
-        <v>logNormXLatex</v>
-      </c>
-      <c r="AF9" t="str">
-        <f t="shared" si="8"/>
-        <v>logNormXChartDomain</v>
-      </c>
-      <c r="AG9" t="str">
-        <f t="shared" si="9"/>
         <v>logNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1858,10 +1823,10 @@
         <v>23</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>53</v>
@@ -1879,13 +1844,13 @@
         <v>44</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="R10" s="1">
         <v>1</v>
@@ -1894,59 +1859,56 @@
         <v>10</v>
       </c>
       <c r="T10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="U10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W10">
+      <c r="V10">
         <v>0.01</v>
       </c>
+      <c r="W10" t="str">
+        <f>"""&amp;"&amp;RIGHT(L10,LEN(L10)-1)&amp;";"""</f>
+        <v>"&amp;lambda;"</v>
+      </c>
       <c r="X10" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;lambda;"</v>
+        <f>IF(F10=1,"""none""",IF(E10=F10,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
       </c>
       <c r="Y10" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R10&amp;", maxVal = "&amp;S10&amp;", startVals = "&amp;T10&amp;", stepVal = "&amp;V10&amp;", paramHTML = "&amp;W10&amp;", multi = "&amp;X10&amp;", sigmaScale ="&amp;U10&amp;","</f>
+        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="Z10" t="str">
         <f t="shared" si="0"/>
-        <v>"none"</v>
-      </c>
-      <c r="Z10" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+        <v>poisParamTransform</v>
       </c>
       <c r="AA10" t="str">
-        <f t="shared" si="6"/>
-        <v>poisParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>poisPDF</v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" si="7"/>
-        <v>poisPDF</v>
+        <f>B10&amp;"PlotDistr"</f>
+        <v>poisPlotDistr</v>
       </c>
       <c r="AC10" t="str">
-        <f t="shared" si="1"/>
-        <v>poisPlotDistr</v>
+        <f>B10&amp;"Draws"</f>
+        <v>poisDraws</v>
       </c>
       <c r="AD10" t="str">
+        <f>B10&amp;"Latex"</f>
+        <v>poisLatex</v>
+      </c>
+      <c r="AE10" t="str">
         <f t="shared" si="2"/>
-        <v>poisDraws</v>
-      </c>
-      <c r="AE10" t="str">
+        <v>poisChartDomain</v>
+      </c>
+      <c r="AF10" t="str">
         <f t="shared" si="3"/>
-        <v>poisLatex</v>
-      </c>
-      <c r="AF10" t="str">
-        <f t="shared" si="8"/>
-        <v>poisChartDomain</v>
-      </c>
-      <c r="AG10" t="str">
-        <f t="shared" si="9"/>
         <v>poisLikelihoodFun</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1954,7 +1916,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>0</v>
@@ -1969,10 +1931,10 @@
         <v>23</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>53</v>
@@ -1990,13 +1952,13 @@
         <v>45</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="R11" s="1">
         <v>-0.25</v>
@@ -2005,59 +1967,56 @@
         <v>3</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W11">
+        <v>70</v>
+      </c>
+      <c r="V11">
         <v>0.01</v>
       </c>
+      <c r="W11" t="str">
+        <f>"""&amp;"&amp;RIGHT(L11,LEN(L11)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X11" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F11=1,"""none""",IF(E11=F11,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
       </c>
       <c r="Y11" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R11&amp;", maxVal = "&amp;S11&amp;", startVals = "&amp;T11&amp;", stepVal = "&amp;V11&amp;", paramHTML = "&amp;W11&amp;", multi = "&amp;X11&amp;", sigmaScale ="&amp;U11&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="Z11" t="str">
         <f t="shared" si="0"/>
-        <v>"none"</v>
-      </c>
-      <c r="Z11" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <v>poisExpParamTransform</v>
       </c>
       <c r="AA11" t="str">
-        <f t="shared" si="6"/>
-        <v>poisExpParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>poisExpPDF</v>
       </c>
       <c r="AB11" t="str">
-        <f t="shared" si="7"/>
-        <v>poisExpPDF</v>
+        <f>B11&amp;"PlotDistr"</f>
+        <v>poisExpPlotDistr</v>
       </c>
       <c r="AC11" t="str">
-        <f t="shared" si="1"/>
-        <v>poisExpPlotDistr</v>
+        <f>B11&amp;"Draws"</f>
+        <v>poisExpDraws</v>
       </c>
       <c r="AD11" t="str">
+        <f>B11&amp;"Latex"</f>
+        <v>poisExpLatex</v>
+      </c>
+      <c r="AE11" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpDraws</v>
-      </c>
-      <c r="AE11" t="str">
+        <v>poisExpChartDomain</v>
+      </c>
+      <c r="AF11" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpLatex</v>
-      </c>
-      <c r="AF11" t="str">
-        <f t="shared" si="8"/>
-        <v>poisExpChartDomain</v>
-      </c>
-      <c r="AG11" t="str">
-        <f t="shared" si="9"/>
         <v>poisExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2065,7 +2024,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>0</v>
@@ -2080,10 +2039,10 @@
         <v>23</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>53</v>
@@ -2101,13 +2060,13 @@
         <v>45</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="R12" s="1">
         <v>-0.25</v>
@@ -2116,67 +2075,64 @@
         <v>3</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W12">
+        <v>70</v>
+      </c>
+      <c r="V12">
         <v>0.01</v>
       </c>
+      <c r="W12" t="str">
+        <f>"""&amp;"&amp;RIGHT(L12,LEN(L12)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X12" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F12=1,"""none""",IF(E12=F12,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
       </c>
       <c r="Y12" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R12&amp;", maxVal = "&amp;S12&amp;", startVals = "&amp;T12&amp;", stepVal = "&amp;V12&amp;", paramHTML = "&amp;W12&amp;", multi = "&amp;X12&amp;", sigmaScale ="&amp;U12&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="Z12" t="str">
         <f t="shared" si="0"/>
-        <v>"betas"</v>
-      </c>
-      <c r="Z12" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>poisExpXParamTransform</v>
       </c>
       <c r="AA12" t="str">
-        <f t="shared" si="6"/>
-        <v>poisExpXParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>poisExpXPDF</v>
       </c>
       <c r="AB12" t="str">
-        <f t="shared" si="7"/>
-        <v>poisExpXPDF</v>
+        <f>B12&amp;"PlotDistr"</f>
+        <v>poisExpXPlotDistr</v>
       </c>
       <c r="AC12" t="str">
-        <f t="shared" si="1"/>
-        <v>poisExpXPlotDistr</v>
+        <f>B12&amp;"Draws"</f>
+        <v>poisExpXDraws</v>
       </c>
       <c r="AD12" t="str">
+        <f>B12&amp;"Latex"</f>
+        <v>poisExpXLatex</v>
+      </c>
+      <c r="AE12" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpXDraws</v>
-      </c>
-      <c r="AE12" t="str">
+        <v>poisExpXChartDomain</v>
+      </c>
+      <c r="AF12" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpXLatex</v>
-      </c>
-      <c r="AF12" t="str">
-        <f t="shared" si="8"/>
-        <v>poisExpXChartDomain</v>
-      </c>
-      <c r="AG12" t="str">
-        <f t="shared" si="9"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
@@ -2191,16 +2147,16 @@
         <v>24</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>37</v>
@@ -2212,13 +2168,13 @@
         <v>45</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="R13" s="1">
         <v>-0.25</v>
@@ -2227,59 +2183,56 @@
         <v>2.5</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W13">
+        <v>97</v>
+      </c>
+      <c r="V13">
         <v>0.01</v>
       </c>
-      <c r="X13" t="str">
+      <c r="W13" t="str">
         <f>"""&amp;"&amp;RIGHT(L13,LEN(L13)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y13" t="str">
+      <c r="X13" t="str">
         <f>IF(F13=1,"""none""",IF(E13=F13,"""betas""","""fullNorm"""))</f>
         <v>"fullNorm"</v>
       </c>
+      <c r="Y13" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R13&amp;", maxVal = "&amp;S13&amp;", startVals = "&amp;T13&amp;", stepVal = "&amp;V13&amp;", paramHTML = "&amp;W13&amp;", multi = "&amp;X13&amp;", sigmaScale ="&amp;U13&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 2.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1,2),</v>
+      </c>
       <c r="Z13" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;R13&amp;", maxVal = "&amp;S13&amp;", startVals = "&amp;T13&amp;", stepVal = "&amp;W13&amp;", paramHTML = "&amp;X13&amp;", multi = "&amp;Y13&amp;", sigmaScale ="&amp;U13&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 2.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1,2),</v>
-      </c>
-      <c r="AA13" t="str">
         <f>$B13&amp;"ParamTransform"</f>
         <v>negBinomXParamTransform</v>
       </c>
-      <c r="AB13" t="str">
+      <c r="AA13" t="str">
         <f>$B13&amp;"PDF"</f>
         <v>negBinomXPDF</v>
       </c>
-      <c r="AC13" t="str">
+      <c r="AB13" t="str">
         <f>B13&amp;"PlotDistr"</f>
         <v>negBinomXPlotDistr</v>
       </c>
-      <c r="AD13" t="str">
+      <c r="AC13" t="str">
         <f>B13&amp;"Draws"</f>
         <v>negBinomXDraws</v>
       </c>
-      <c r="AE13" t="str">
+      <c r="AD13" t="str">
         <f>B13&amp;"Latex"</f>
         <v>negBinomXLatex</v>
       </c>
-      <c r="AF13" t="str">
+      <c r="AE13" t="str">
         <f>$B13&amp;"ChartDomain"</f>
         <v>negBinomXChartDomain</v>
       </c>
-      <c r="AG13" t="str">
+      <c r="AF13" t="str">
         <f>$B13&amp;"LikelihoodFun"</f>
         <v>negBinomXLikelihoodFun</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2302,10 +2255,10 @@
         <v>24</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>48</v>
@@ -2323,13 +2276,13 @@
         <v>45</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="R14" s="1">
         <v>0.25</v>
@@ -2338,59 +2291,56 @@
         <v>1.5</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W14">
+        <v>70</v>
+      </c>
+      <c r="V14">
         <v>0.01</v>
       </c>
+      <c r="W14" t="str">
+        <f>"""&amp;"&amp;RIGHT(L14,LEN(L14)-1)&amp;";"""</f>
+        <v>"&amp;lambda;"</v>
+      </c>
       <c r="X14" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;lambda;"</v>
+        <f>IF(F14=1,"""none""",IF(E14=F14,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
       </c>
       <c r="Y14" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R14&amp;", maxVal = "&amp;S14&amp;", startVals = "&amp;T14&amp;", stepVal = "&amp;V14&amp;", paramHTML = "&amp;W14&amp;", multi = "&amp;X14&amp;", sigmaScale ="&amp;U14&amp;","</f>
+        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="Z14" t="str">
         <f t="shared" si="0"/>
-        <v>"none"</v>
-      </c>
-      <c r="Z14" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+        <v>expParamTransform</v>
       </c>
       <c r="AA14" t="str">
-        <f t="shared" si="6"/>
-        <v>expParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>expPDF</v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" si="7"/>
-        <v>expPDF</v>
+        <f>B14&amp;"PlotDistr"</f>
+        <v>expPlotDistr</v>
       </c>
       <c r="AC14" t="str">
-        <f t="shared" si="1"/>
-        <v>expPlotDistr</v>
+        <f>B14&amp;"Draws"</f>
+        <v>expDraws</v>
       </c>
       <c r="AD14" t="str">
+        <f>B14&amp;"Latex"</f>
+        <v>expLatex</v>
+      </c>
+      <c r="AE14" t="str">
         <f t="shared" si="2"/>
-        <v>expDraws</v>
-      </c>
-      <c r="AE14" t="str">
+        <v>expChartDomain</v>
+      </c>
+      <c r="AF14" t="str">
         <f t="shared" si="3"/>
-        <v>expLatex</v>
-      </c>
-      <c r="AF14" t="str">
-        <f t="shared" si="8"/>
-        <v>expChartDomain</v>
-      </c>
-      <c r="AG14" t="str">
-        <f t="shared" si="9"/>
         <v>expLikelihoodFun</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2398,7 +2348,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -2413,10 +2363,10 @@
         <v>24</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>48</v>
@@ -2434,13 +2384,13 @@
         <v>45</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="R15" s="1">
         <v>-2</v>
@@ -2449,59 +2399,56 @@
         <v>2</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W15">
+        <v>70</v>
+      </c>
+      <c r="V15">
         <v>0.01</v>
       </c>
+      <c r="W15" t="str">
+        <f>"""&amp;"&amp;RIGHT(L15,LEN(L15)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X15" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F15=1,"""none""",IF(E15=F15,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
       </c>
       <c r="Y15" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R15&amp;", maxVal = "&amp;S15&amp;", startVals = "&amp;T15&amp;", stepVal = "&amp;V15&amp;", paramHTML = "&amp;W15&amp;", multi = "&amp;X15&amp;", sigmaScale ="&amp;U15&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="Z15" t="str">
         <f t="shared" si="0"/>
-        <v>"none"</v>
-      </c>
-      <c r="Z15" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <v>expExpParamTransform</v>
       </c>
       <c r="AA15" t="str">
-        <f t="shared" si="6"/>
-        <v>expExpParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>expExpPDF</v>
       </c>
       <c r="AB15" t="str">
-        <f t="shared" si="7"/>
-        <v>expExpPDF</v>
+        <f>B15&amp;"PlotDistr"</f>
+        <v>expExpPlotDistr</v>
       </c>
       <c r="AC15" t="str">
-        <f t="shared" si="1"/>
-        <v>expExpPlotDistr</v>
+        <f>B15&amp;"Draws"</f>
+        <v>expExpDraws</v>
       </c>
       <c r="AD15" t="str">
+        <f>B15&amp;"Latex"</f>
+        <v>expExpLatex</v>
+      </c>
+      <c r="AE15" t="str">
         <f t="shared" si="2"/>
-        <v>expExpDraws</v>
-      </c>
-      <c r="AE15" t="str">
+        <v>expExpChartDomain</v>
+      </c>
+      <c r="AF15" t="str">
         <f t="shared" si="3"/>
-        <v>expExpLatex</v>
-      </c>
-      <c r="AF15" t="str">
-        <f t="shared" si="8"/>
-        <v>expExpChartDomain</v>
-      </c>
-      <c r="AG15" t="str">
-        <f t="shared" si="9"/>
         <v>expExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2509,7 +2456,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
@@ -2524,10 +2471,10 @@
         <v>24</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>48</v>
@@ -2545,13 +2492,13 @@
         <v>45</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="R16" s="1">
         <v>-0.5</v>
@@ -2560,70 +2507,67 @@
         <v>0.5</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W16">
+        <v>70</v>
+      </c>
+      <c r="V16">
         <v>0.01</v>
       </c>
+      <c r="W16" t="str">
+        <f>"""&amp;"&amp;RIGHT(L16,LEN(L16)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X16" t="str">
-        <f t="shared" si="4"/>
-        <v>"&amp;beta;"</v>
+        <f>IF(F16=1,"""none""",IF(E16=F16,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
       </c>
       <c r="Y16" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R16&amp;", maxVal = "&amp;S16&amp;", startVals = "&amp;T16&amp;", stepVal = "&amp;V16&amp;", paramHTML = "&amp;W16&amp;", multi = "&amp;X16&amp;", sigmaScale ="&amp;U16&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="Z16" t="str">
         <f t="shared" si="0"/>
-        <v>"betas"</v>
-      </c>
-      <c r="Z16" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>expExpXParamTransform</v>
       </c>
       <c r="AA16" t="str">
-        <f t="shared" si="6"/>
-        <v>expExpXParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>expExpXPDF</v>
       </c>
       <c r="AB16" t="str">
-        <f t="shared" si="7"/>
-        <v>expExpXPDF</v>
+        <f>B16&amp;"PlotDistr"</f>
+        <v>expExpXPlotDistr</v>
       </c>
       <c r="AC16" t="str">
-        <f t="shared" si="1"/>
-        <v>expExpXPlotDistr</v>
+        <f>B16&amp;"Draws"</f>
+        <v>expExpXDraws</v>
       </c>
       <c r="AD16" t="str">
+        <f>B16&amp;"Latex"</f>
+        <v>expExpXLatex</v>
+      </c>
+      <c r="AE16" t="str">
         <f t="shared" si="2"/>
-        <v>expExpXDraws</v>
-      </c>
-      <c r="AE16" t="str">
+        <v>expExpXChartDomain</v>
+      </c>
+      <c r="AF16" t="str">
         <f t="shared" si="3"/>
-        <v>expExpXLatex</v>
-      </c>
-      <c r="AF16" t="str">
-        <f t="shared" si="8"/>
-        <v>expExpXChartDomain</v>
-      </c>
-      <c r="AG16" t="str">
-        <f t="shared" si="9"/>
         <v>expExpXLikelihoodFun</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E17" s="1">
         <v>3</v>
@@ -2635,10 +2579,10 @@
         <v>24</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>48</v>
@@ -2656,13 +2600,13 @@
         <v>45</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="R17" s="1">
         <v>-0.5</v>
@@ -2671,70 +2615,67 @@
         <v>0.5</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W17">
+        <v>70</v>
+      </c>
+      <c r="V17">
         <v>0.01</v>
       </c>
+      <c r="W17" t="str">
+        <f>"""&amp;"&amp;RIGHT(L17,LEN(L17)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
       <c r="X17" t="str">
-        <f t="shared" ref="X17" si="10">"""&amp;"&amp;RIGHT(L17,LEN(L17)-1)&amp;";"""</f>
-        <v>"&amp;beta;"</v>
+        <f>IF(F17=1,"""none""",IF(E17=F17,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
       </c>
       <c r="Y17" t="str">
-        <f t="shared" ref="Y17" si="11">IF(F17=1,"""none""",IF(E17=F17,"""betas""","""fullNorm"""))</f>
-        <v>"betas"</v>
+        <f>"manyParamSliderMaker(minVal ="&amp;R17&amp;", maxVal = "&amp;S17&amp;", startVals = "&amp;T17&amp;", stepVal = "&amp;V17&amp;", paramHTML = "&amp;W17&amp;", multi = "&amp;X17&amp;", sigmaScale ="&amp;U17&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="Z17" t="str">
-        <f t="shared" ref="Z17" si="12">"manyParamSliderMaker(minVal ="&amp;R17&amp;", maxVal = "&amp;S17&amp;", startVals = "&amp;T17&amp;", stepVal = "&amp;W17&amp;", paramHTML = "&amp;X17&amp;", multi = "&amp;Y17&amp;", sigmaScale ="&amp;U17&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <f t="shared" si="0"/>
+        <v>neumayerParamTransform</v>
       </c>
       <c r="AA17" t="str">
-        <f t="shared" si="6"/>
-        <v>neumayerParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>neumayerPDF</v>
       </c>
       <c r="AB17" t="str">
-        <f t="shared" si="7"/>
-        <v>neumayerPDF</v>
+        <f t="shared" ref="AB17" si="4">B17&amp;"PlotDistr"</f>
+        <v>neumayerPlotDistr</v>
       </c>
       <c r="AC17" t="str">
-        <f t="shared" ref="AC17" si="13">B17&amp;"PlotDistr"</f>
-        <v>neumayerPlotDistr</v>
+        <f t="shared" ref="AC17" si="5">B17&amp;"Draws"</f>
+        <v>neumayerDraws</v>
       </c>
       <c r="AD17" t="str">
-        <f t="shared" ref="AD17" si="14">B17&amp;"Draws"</f>
-        <v>neumayerDraws</v>
+        <f t="shared" ref="AD17" si="6">B17&amp;"Latex"</f>
+        <v>neumayerLatex</v>
       </c>
       <c r="AE17" t="str">
-        <f t="shared" ref="AE17" si="15">B17&amp;"Latex"</f>
-        <v>neumayerLatex</v>
+        <f t="shared" si="2"/>
+        <v>neumayerChartDomain</v>
       </c>
       <c r="AF17" t="str">
-        <f t="shared" si="8"/>
-        <v>neumayerChartDomain</v>
-      </c>
-      <c r="AG17" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>neumayerLikelihoodFun</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="E18" s="1">
         <v>3</v>
@@ -2746,10 +2687,10 @@
         <v>24</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>48</v>
@@ -2767,13 +2708,13 @@
         <v>45</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="R18" s="1">
         <v>-0.5</v>
@@ -2782,55 +2723,52 @@
         <v>0.5</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W18">
+        <v>70</v>
+      </c>
+      <c r="V18">
         <v>0.01</v>
       </c>
-      <c r="X18" t="str">
+      <c r="W18" t="str">
         <f>"""&amp;"&amp;RIGHT(L18,LEN(L18)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
+      <c r="X18" t="str">
+        <f>IF(F18=1,"""none""",IF(E18=F18,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
+      </c>
       <c r="Y18" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;R18&amp;", maxVal = "&amp;S18&amp;", startVals = "&amp;T18&amp;", stepVal = "&amp;V18&amp;", paramHTML = "&amp;W18&amp;", multi = "&amp;X18&amp;", sigmaScale ="&amp;U18&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="Z18" t="str">
         <f t="shared" si="0"/>
-        <v>"betas"</v>
-      </c>
-      <c r="Z18" t="str">
-        <f t="shared" si="5"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>drehJenParamTransform</v>
       </c>
       <c r="AA18" t="str">
-        <f t="shared" si="6"/>
-        <v>drehJenParamTransform</v>
+        <f t="shared" si="1"/>
+        <v>drehJenPDF</v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" si="7"/>
-        <v>drehJenPDF</v>
+        <f>B18&amp;"PlotDistr"</f>
+        <v>drehJenPlotDistr</v>
       </c>
       <c r="AC18" t="str">
-        <f t="shared" si="1"/>
-        <v>drehJenPlotDistr</v>
+        <f>B18&amp;"Draws"</f>
+        <v>drehJenDraws</v>
       </c>
       <c r="AD18" t="str">
+        <f>B18&amp;"Latex"</f>
+        <v>drehJenLatex</v>
+      </c>
+      <c r="AE18" t="str">
         <f t="shared" si="2"/>
-        <v>drehJenDraws</v>
-      </c>
-      <c r="AE18" t="str">
+        <v>drehJenChartDomain</v>
+      </c>
+      <c r="AF18" t="str">
         <f t="shared" si="3"/>
-        <v>drehJenLatex</v>
-      </c>
-      <c r="AF18" t="str">
-        <f t="shared" si="8"/>
-        <v>drehJenChartDomain</v>
-      </c>
-      <c r="AG18" t="str">
-        <f t="shared" si="9"/>
         <v>drehJenLikelihoodFun</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more config and bugfix for bern logitX
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58E7D0D-AC6B-418E-8CFE-753DB4EBEEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EFD29C-A05A-49AE-BD6C-AA2546B1C533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="136">
   <si>
     <t>Poisson</t>
   </si>
@@ -432,13 +432,16 @@
     <t>nCovar</t>
   </si>
   <si>
-    <t>c(-1,-1.5,.25, 2,-1)</t>
-  </si>
-  <si>
     <t>funcFormRange</t>
   </si>
   <si>
     <t>c(-10,10)</t>
+  </si>
+  <si>
+    <t>c(-1,.6,.25, 1,-1)</t>
+  </si>
+  <si>
+    <t>c(-6,6)</t>
   </si>
 </sst>
 </file>
@@ -808,7 +811,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9:Q18"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +891,7 @@
         <v>71</v>
       </c>
       <c r="Q1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R1" t="s">
         <v>55</v>
@@ -1310,7 +1313,7 @@
         <v>72</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="R5" s="1">
         <v>-4</v>
@@ -1418,7 +1421,7 @@
         <v>72</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="R6" s="1">
         <v>-3</v>
@@ -1526,7 +1529,7 @@
         <v>73</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>134</v>
+        <v>85</v>
       </c>
       <c r="R7" s="1">
         <v>-3</v>
@@ -1535,7 +1538,7 @@
         <v>3</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>94</v>
@@ -1553,7 +1556,7 @@
       </c>
       <c r="Y7" t="str">
         <f>"manyParamSliderMaker(minVal ="&amp;R7&amp;", maxVal = "&amp;S7&amp;", startVals = "&amp;T7&amp;", stepVal = "&amp;V7&amp;", paramHTML = "&amp;W7&amp;", multi = "&amp;X7&amp;", sigmaScale ="&amp;U7&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,-1.5,.25, 2,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-2,2),</v>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,.25, 1,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-2,2),</v>
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="0"/>
@@ -1634,7 +1637,7 @@
         <v>79</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="R8" s="1">
         <v>-0.5</v>
@@ -1742,7 +1745,7 @@
         <v>72</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="R9" s="1">
         <v>-0.5</v>
@@ -1850,7 +1853,7 @@
         <v>75</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="R10" s="1">
         <v>1</v>
@@ -1958,7 +1961,7 @@
         <v>72</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="R11" s="1">
         <v>-0.25</v>
@@ -2066,7 +2069,7 @@
         <v>72</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="R12" s="1">
         <v>-0.25</v>
@@ -2174,7 +2177,7 @@
         <v>72</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="R13" s="1">
         <v>-0.25</v>
@@ -2282,7 +2285,7 @@
         <v>80</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="R14" s="1">
         <v>0.25</v>
@@ -2390,7 +2393,7 @@
         <v>80</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="R15" s="1">
         <v>-2</v>
@@ -2498,7 +2501,7 @@
         <v>80</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="R16" s="1">
         <v>-0.5</v>
@@ -2606,7 +2609,7 @@
         <v>80</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R17" s="1">
         <v>-0.5</v>
@@ -2714,7 +2717,7 @@
         <v>80</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R18" s="1">
         <v>-0.5</v>

</xml_diff>

<commit_message>
ui labels and tex change
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EFD29C-A05A-49AE-BD6C-AA2546B1C533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BFEDDF-5A9D-4AB9-AADC-072F699DECE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -811,7 +811,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ordered probit first draft of first page
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37E8820-1CB9-4E72-ABCA-31D654061DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5426DAE-3501-467E-9DFF-5EA324ADA299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="145">
   <si>
     <t>Poisson</t>
   </si>
@@ -457,6 +457,18 @@
   </si>
   <si>
     <t>list("Bernoulli (Probit, X)","Bernoulli (Logit, X)","Bernoulli","Bernoulli (Logit)")</t>
+  </si>
+  <si>
+    <t>orderedProbitX</t>
+  </si>
+  <si>
+    <t>Ordered Probit (X)</t>
+  </si>
+  <si>
+    <t>list("Ordered Probit (X)")</t>
+  </si>
+  <si>
+    <t>c(1,3)</t>
   </si>
 </sst>
 </file>
@@ -823,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:AF19"/>
+  <dimension ref="A1:AF20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1034,7 @@
         <v>0.01</v>
       </c>
       <c r="W2" t="str">
-        <f t="shared" ref="W2:W19" si="0">"""&amp;"&amp;RIGHT(L2,LEN(L2)-1)&amp;";"""</f>
+        <f t="shared" ref="W2:W20" si="0">"""&amp;"&amp;RIGHT(L2,LEN(L2)-1)&amp;";"""</f>
         <v>"&amp;pi;"</v>
       </c>
       <c r="X2" t="str">
@@ -1030,7 +1042,7 @@
         <v>"none"</v>
       </c>
       <c r="Y2" t="str">
-        <f t="shared" ref="Y2:Y19" si="1">"manyParamSliderMaker(minVal ="&amp;R2&amp;", maxVal = "&amp;S2&amp;", startVals = "&amp;T2&amp;", stepVal = "&amp;V2&amp;", paramHTML = "&amp;W2&amp;", multi = "&amp;X2&amp;", sigmaScale ="&amp;U2&amp;","</f>
+        <f t="shared" ref="Y2:Y20" si="1">"manyParamSliderMaker(minVal ="&amp;R2&amp;", maxVal = "&amp;S2&amp;", startVals = "&amp;T2&amp;", stepVal = "&amp;V2&amp;", paramHTML = "&amp;W2&amp;", multi = "&amp;X2&amp;", sigmaScale ="&amp;U2&amp;","</f>
         <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z2" t="str">
@@ -1064,6 +1076,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1142,11 +1155,11 @@
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z3" t="str">
-        <f t="shared" ref="Z3:Z19" si="2">$B3&amp;"ParamTransform"</f>
+        <f t="shared" ref="Z3:Z20" si="2">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
       <c r="AA3" t="str">
-        <f t="shared" ref="AA3:AA19" si="3">$B3&amp;"PDF"</f>
+        <f t="shared" ref="AA3:AA20" si="3">$B3&amp;"PDF"</f>
         <v>bernLogitPDF</v>
       </c>
       <c r="AB3" t="str">
@@ -1162,16 +1175,17 @@
         <v>bernLogitLatex</v>
       </c>
       <c r="AE3" t="str">
-        <f t="shared" ref="AE3:AE19" si="4">$B3&amp;"ChartDomain"</f>
+        <f t="shared" ref="AE3:AE20" si="4">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
       <c r="AF3" t="str">
-        <f t="shared" ref="AF3:AF19" si="5">$B3&amp;"LikelihoodFun"</f>
+        <f t="shared" ref="AF3:AF20" si="5">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:A20" si="6">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1280,6 +1294,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1346,7 +1361,7 @@
         <v>0.01</v>
       </c>
       <c r="W5" t="str">
-        <f t="shared" ref="W5" si="6">"""&amp;"&amp;RIGHT(L5,LEN(L5)-1)&amp;";"""</f>
+        <f t="shared" ref="W5" si="7">"""&amp;"&amp;RIGHT(L5,LEN(L5)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="X5" t="str">
@@ -1354,7 +1369,7 @@
         <v>"betas"</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" ref="Y5" si="7">"manyParamSliderMaker(minVal ="&amp;R5&amp;", maxVal = "&amp;S5&amp;", startVals = "&amp;T5&amp;", stepVal = "&amp;V5&amp;", paramHTML = "&amp;W5&amp;", multi = "&amp;X5&amp;", sigmaScale ="&amp;U5&amp;","</f>
+        <f t="shared" ref="Y5" si="8">"manyParamSliderMaker(minVal ="&amp;R5&amp;", maxVal = "&amp;S5&amp;", startVals = "&amp;T5&amp;", stepVal = "&amp;V5&amp;", paramHTML = "&amp;W5&amp;", multi = "&amp;X5&amp;", sigmaScale ="&amp;U5&amp;","</f>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="Z5" t="str">
@@ -1366,15 +1381,15 @@
         <v>bernProbitXPDF</v>
       </c>
       <c r="AB5" t="str">
-        <f t="shared" ref="AB5" si="8">B5&amp;"PlotDistr"</f>
+        <f t="shared" ref="AB5:AB6" si="9">B5&amp;"PlotDistr"</f>
         <v>bernProbitXPlotDistr</v>
       </c>
       <c r="AC5" t="str">
-        <f t="shared" ref="AC5" si="9">B5&amp;"Draws"</f>
+        <f t="shared" ref="AC5:AC6" si="10">B5&amp;"Draws"</f>
         <v>bernProbitXDraws</v>
       </c>
       <c r="AD5" t="str">
-        <f t="shared" ref="AD5" si="10">B5&amp;"Latex"</f>
+        <f t="shared" ref="AD5:AD6" si="11">B5&amp;"Latex"</f>
         <v>bernProbitXLatex</v>
       </c>
       <c r="AE5" t="str">
@@ -1388,34 +1403,35 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>28</v>
@@ -1424,103 +1440,104 @@
         <v>37</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="R6" s="1">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="S6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="V6">
         <v>0.01</v>
       </c>
       <c r="W6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="W6" si="12">"""&amp;"&amp;RIGHT(L6,LEN(L6)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="X6" t="str">
         <f>IF(F6=1,"""none""",IF(E6=F6,"""betas""","""fullNorm"""))</f>
-        <v>"none"</v>
+        <v>"fullNorm"</v>
       </c>
       <c r="Y6" t="str">
-        <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <f t="shared" ref="Y6" si="13">"manyParamSliderMaker(minVal ="&amp;R6&amp;", maxVal = "&amp;S6&amp;", startVals = "&amp;T6&amp;", stepVal = "&amp;V6&amp;", paramHTML = "&amp;W6&amp;", multi = "&amp;X6&amp;", sigmaScale ="&amp;U6&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" si="2"/>
-        <v>styNormParamTransform</v>
+        <v>orderedProbitXParamTransform</v>
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="3"/>
-        <v>styNormPDF</v>
+        <v>orderedProbitXPDF</v>
       </c>
       <c r="AB6" t="str">
-        <f>B6&amp;"PlotDistr"</f>
-        <v>styNormPlotDistr</v>
+        <f t="shared" ref="AB6" si="14">B6&amp;"PlotDistr"</f>
+        <v>orderedProbitXPlotDistr</v>
       </c>
       <c r="AC6" t="str">
-        <f>B6&amp;"Draws"</f>
-        <v>styNormDraws</v>
+        <f t="shared" ref="AC6" si="15">B6&amp;"Draws"</f>
+        <v>orderedProbitXDraws</v>
       </c>
       <c r="AD6" t="str">
-        <f>B6&amp;"Latex"</f>
-        <v>styNormLatex</v>
+        <f t="shared" ref="AD6" si="16">B6&amp;"Latex"</f>
+        <v>orderedProbitXLatex</v>
       </c>
       <c r="AE6" t="str">
         <f t="shared" si="4"/>
-        <v>styNormChartDomain</v>
+        <v>orderedProbitXChartDomain</v>
       </c>
       <c r="AF6" t="str">
         <f t="shared" si="5"/>
-        <v>styNormLikelihoodFun</v>
+        <v>orderedProbitXLikelihoodFun</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>52</v>
@@ -1535,7 +1552,7 @@
         <v>40</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>84</v>
@@ -1547,13 +1564,13 @@
         <v>133</v>
       </c>
       <c r="R7" s="1">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="S7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>70</v>
@@ -1567,74 +1584,75 @@
       </c>
       <c r="X7" t="str">
         <f>IF(F7=1,"""none""",IF(E7=F7,"""betas""","""fullNorm"""))</f>
-        <v>"betas"</v>
+        <v>"none"</v>
       </c>
       <c r="Y7" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="2"/>
-        <v>styNormXParamTransform</v>
+        <v>styNormParamTransform</v>
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="3"/>
-        <v>styNormXPDF</v>
+        <v>styNormPDF</v>
       </c>
       <c r="AB7" t="str">
         <f>B7&amp;"PlotDistr"</f>
-        <v>styNormXPlotDistr</v>
+        <v>styNormPlotDistr</v>
       </c>
       <c r="AC7" t="str">
         <f>B7&amp;"Draws"</f>
-        <v>styNormXDraws</v>
+        <v>styNormDraws</v>
       </c>
       <c r="AD7" t="str">
         <f>B7&amp;"Latex"</f>
-        <v>styNormXLatex</v>
+        <v>styNormLatex</v>
       </c>
       <c r="AE7" t="str">
         <f t="shared" si="4"/>
-        <v>styNormXChartDomain</v>
+        <v>styNormChartDomain</v>
       </c>
       <c r="AF7" t="str">
         <f t="shared" si="5"/>
-        <v>styNormXLikelihoodFun</v>
+        <v>styNormLikelihoodFun</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8">
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>37</v>
@@ -1649,10 +1667,10 @@
         <v>84</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="R8" s="1">
         <v>-3</v>
@@ -1661,10 +1679,10 @@
         <v>3</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>137</v>
+        <v>70</v>
       </c>
       <c r="V8">
         <v>0.01</v>
@@ -1675,74 +1693,75 @@
       </c>
       <c r="X8" t="str">
         <f>IF(F8=1,"""none""",IF(E8=F8,"""betas""","""fullNorm"""))</f>
-        <v>"fullNorm"</v>
+        <v>"betas"</v>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="2"/>
-        <v>fullNormXParamTransform</v>
+        <v>styNormXParamTransform</v>
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="3"/>
-        <v>fullNormXPDF</v>
+        <v>styNormXPDF</v>
       </c>
       <c r="AB8" t="str">
         <f>B8&amp;"PlotDistr"</f>
-        <v>fullNormXPlotDistr</v>
+        <v>styNormXPlotDistr</v>
       </c>
       <c r="AC8" t="str">
         <f>B8&amp;"Draws"</f>
-        <v>fullNormXDraws</v>
+        <v>styNormXDraws</v>
       </c>
       <c r="AD8" t="str">
         <f>B8&amp;"Latex"</f>
-        <v>fullNormXLatex</v>
+        <v>styNormXLatex</v>
       </c>
       <c r="AE8" t="str">
         <f t="shared" si="4"/>
-        <v>fullNormXChartDomain</v>
+        <v>styNormXChartDomain</v>
       </c>
       <c r="AF8" t="str">
         <f t="shared" si="5"/>
-        <v>fullNormXLikelihoodFun</v>
+        <v>styNormXLikelihoodFun</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9">
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>37</v>
@@ -1751,28 +1770,28 @@
         <v>40</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="R9" s="1">
-        <v>-0.5</v>
+        <v>-3</v>
       </c>
       <c r="S9" s="1">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="V9">
         <v>0.01</v>
@@ -1783,68 +1802,69 @@
       </c>
       <c r="X9" t="str">
         <f>IF(F9=1,"""none""",IF(E9=F9,"""betas""","""fullNorm"""))</f>
-        <v>"none"</v>
+        <v>"fullNorm"</v>
       </c>
       <c r="Y9" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="2"/>
-        <v>logNormParamTransform</v>
+        <v>fullNormXParamTransform</v>
       </c>
       <c r="AA9" t="str">
         <f t="shared" si="3"/>
-        <v>logNormPDF</v>
+        <v>fullNormXPDF</v>
       </c>
       <c r="AB9" t="str">
         <f>B9&amp;"PlotDistr"</f>
-        <v>logNormPlotDistr</v>
+        <v>fullNormXPlotDistr</v>
       </c>
       <c r="AC9" t="str">
         <f>B9&amp;"Draws"</f>
-        <v>logNormDraws</v>
+        <v>fullNormXDraws</v>
       </c>
       <c r="AD9" t="str">
         <f>B9&amp;"Latex"</f>
-        <v>logNormLatex</v>
+        <v>fullNormXLatex</v>
       </c>
       <c r="AE9" t="str">
         <f t="shared" si="4"/>
-        <v>logNormChartDomain</v>
+        <v>fullNormXChartDomain</v>
       </c>
       <c r="AF9" t="str">
         <f t="shared" si="5"/>
-        <v>logNormLikelihoodFun</v>
+        <v>fullNormXLikelihoodFun</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10">
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>110</v>
       </c>
       <c r="E10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>48</v>
@@ -1859,13 +1879,13 @@
         <v>40</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>93</v>
@@ -1877,7 +1897,7 @@
         <v>0.5</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>70</v>
@@ -1891,101 +1911,102 @@
       </c>
       <c r="X10" t="str">
         <f>IF(F10=1,"""none""",IF(E10=F10,"""betas""","""fullNorm"""))</f>
-        <v>"betas"</v>
+        <v>"none"</v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="2"/>
-        <v>logNormXParamTransform</v>
+        <v>logNormParamTransform</v>
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="3"/>
-        <v>logNormXPDF</v>
+        <v>logNormPDF</v>
       </c>
       <c r="AB10" t="str">
         <f>B10&amp;"PlotDistr"</f>
-        <v>logNormXPlotDistr</v>
+        <v>logNormPlotDistr</v>
       </c>
       <c r="AC10" t="str">
         <f>B10&amp;"Draws"</f>
-        <v>logNormXDraws</v>
+        <v>logNormDraws</v>
       </c>
       <c r="AD10" t="str">
         <f>B10&amp;"Latex"</f>
-        <v>logNormXLatex</v>
+        <v>logNormLatex</v>
       </c>
       <c r="AE10" t="str">
         <f t="shared" si="4"/>
-        <v>logNormXChartDomain</v>
+        <v>logNormChartDomain</v>
       </c>
       <c r="AF10" t="str">
         <f t="shared" si="5"/>
-        <v>logNormXLikelihoodFun</v>
+        <v>logNormLikelihoodFun</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11">
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="R11" s="1">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="S11" s="1">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>70</v>
@@ -1995,54 +2016,55 @@
       </c>
       <c r="W11" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;lambda;"</v>
+        <v>"&amp;beta;"</v>
       </c>
       <c r="X11" t="str">
         <f>IF(F11=1,"""none""",IF(E11=F11,"""betas""","""fullNorm"""))</f>
-        <v>"none"</v>
+        <v>"betas"</v>
       </c>
       <c r="Y11" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="2"/>
-        <v>poisParamTransform</v>
+        <v>logNormXParamTransform</v>
       </c>
       <c r="AA11" t="str">
         <f t="shared" si="3"/>
-        <v>poisPDF</v>
+        <v>logNormXPDF</v>
       </c>
       <c r="AB11" t="str">
         <f>B11&amp;"PlotDistr"</f>
-        <v>poisPlotDistr</v>
+        <v>logNormXPlotDistr</v>
       </c>
       <c r="AC11" t="str">
         <f>B11&amp;"Draws"</f>
-        <v>poisDraws</v>
+        <v>logNormXDraws</v>
       </c>
       <c r="AD11" t="str">
         <f>B11&amp;"Latex"</f>
-        <v>poisLatex</v>
+        <v>logNormXLatex</v>
       </c>
       <c r="AE11" t="str">
         <f t="shared" si="4"/>
-        <v>poisChartDomain</v>
+        <v>logNormXChartDomain</v>
       </c>
       <c r="AF11" t="str">
         <f t="shared" si="5"/>
-        <v>poisLikelihoodFun</v>
+        <v>logNormXLikelihoodFun</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12">
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>0</v>
@@ -2057,7 +2079,7 @@
         <v>23</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>89</v>
@@ -2066,34 +2088,34 @@
         <v>53</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>38</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>77</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>78</v>
       </c>
       <c r="R12" s="1">
-        <v>-0.25</v>
+        <v>1</v>
       </c>
       <c r="S12" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>70</v>
@@ -2103,7 +2125,7 @@
       </c>
       <c r="W12" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
+        <v>"&amp;lambda;"</v>
       </c>
       <c r="X12" t="str">
         <f>IF(F12=1,"""none""",IF(E12=F12,"""betas""","""fullNorm"""))</f>
@@ -2111,64 +2133,65 @@
       </c>
       <c r="Y12" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpParamTransform</v>
+        <v>poisParamTransform</v>
       </c>
       <c r="AA12" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpPDF</v>
+        <v>poisPDF</v>
       </c>
       <c r="AB12" t="str">
         <f>B12&amp;"PlotDistr"</f>
-        <v>poisExpPlotDistr</v>
+        <v>poisPlotDistr</v>
       </c>
       <c r="AC12" t="str">
         <f>B12&amp;"Draws"</f>
-        <v>poisExpDraws</v>
+        <v>poisDraws</v>
       </c>
       <c r="AD12" t="str">
         <f>B12&amp;"Latex"</f>
-        <v>poisExpLatex</v>
+        <v>poisLatex</v>
       </c>
       <c r="AE12" t="str">
         <f t="shared" si="4"/>
-        <v>poisExpChartDomain</v>
+        <v>poisChartDomain</v>
       </c>
       <c r="AF12" t="str">
         <f t="shared" si="5"/>
-        <v>poisExpLikelihoodFun</v>
+        <v>poisLikelihoodFun</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13">
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>53</v>
@@ -2186,7 +2209,7 @@
         <v>45</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>72</v>
@@ -2201,7 +2224,7 @@
         <v>3</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>70</v>
@@ -2215,74 +2238,75 @@
       </c>
       <c r="X13" t="str">
         <f>IF(F13=1,"""none""",IF(E13=F13,"""betas""","""fullNorm"""))</f>
-        <v>"betas"</v>
+        <v>"none"</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpXParamTransform</v>
+        <v>poisExpParamTransform</v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpXPDF</v>
+        <v>poisExpPDF</v>
       </c>
       <c r="AB13" t="str">
         <f>B13&amp;"PlotDistr"</f>
-        <v>poisExpXPlotDistr</v>
+        <v>poisExpPlotDistr</v>
       </c>
       <c r="AC13" t="str">
         <f>B13&amp;"Draws"</f>
-        <v>poisExpXDraws</v>
+        <v>poisExpDraws</v>
       </c>
       <c r="AD13" t="str">
         <f>B13&amp;"Latex"</f>
-        <v>poisExpXLatex</v>
+        <v>poisExpLatex</v>
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="4"/>
-        <v>poisExpXChartDomain</v>
+        <v>poisExpChartDomain</v>
       </c>
       <c r="AF13" t="str">
         <f t="shared" si="5"/>
-        <v>poisExpXLikelihoodFun</v>
+        <v>poisExpLikelihoodFun</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14">
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1">
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>37</v>
@@ -2294,7 +2318,7 @@
         <v>45</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>72</v>
@@ -2306,13 +2330,13 @@
         <v>-0.25</v>
       </c>
       <c r="S14" s="1">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="V14">
         <v>0.01</v>
@@ -2323,77 +2347,78 @@
       </c>
       <c r="X14" t="str">
         <f>IF(F14=1,"""none""",IF(E14=F14,"""betas""","""fullNorm"""))</f>
-        <v>"fullNorm"</v>
+        <v>"betas"</v>
       </c>
       <c r="Y14" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 1.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1,2),</v>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="Z14" t="str">
-        <f>$B14&amp;"ParamTransform"</f>
-        <v>negBinomXParamTransform</v>
+        <f t="shared" si="2"/>
+        <v>poisExpXParamTransform</v>
       </c>
       <c r="AA14" t="str">
-        <f>$B14&amp;"PDF"</f>
-        <v>negBinomXPDF</v>
+        <f t="shared" si="3"/>
+        <v>poisExpXPDF</v>
       </c>
       <c r="AB14" t="str">
         <f>B14&amp;"PlotDistr"</f>
-        <v>negBinomXPlotDistr</v>
+        <v>poisExpXPlotDistr</v>
       </c>
       <c r="AC14" t="str">
         <f>B14&amp;"Draws"</f>
-        <v>negBinomXDraws</v>
+        <v>poisExpXDraws</v>
       </c>
       <c r="AD14" t="str">
         <f>B14&amp;"Latex"</f>
-        <v>negBinomXLatex</v>
+        <v>poisExpXLatex</v>
       </c>
       <c r="AE14" t="str">
-        <f>$B14&amp;"ChartDomain"</f>
-        <v>negBinomXChartDomain</v>
+        <f t="shared" si="4"/>
+        <v>poisExpXChartDomain</v>
       </c>
       <c r="AF14" t="str">
-        <f>$B14&amp;"LikelihoodFun"</f>
-        <v>negBinomXLikelihoodFun</v>
+        <f t="shared" si="5"/>
+        <v>poisExpXLikelihoodFun</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15">
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>38</v>
@@ -2402,79 +2427,80 @@
         <v>45</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>78</v>
       </c>
       <c r="R15" s="1">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="S15" s="1">
         <v>1.5</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="V15">
         <v>0.01</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;lambda;"</v>
+        <v>"&amp;beta;"</v>
       </c>
       <c r="X15" t="str">
         <f>IF(F15=1,"""none""",IF(E15=F15,"""betas""","""fullNorm"""))</f>
-        <v>"none"</v>
+        <v>"fullNorm"</v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 1.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1,2),</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="2"/>
-        <v>expParamTransform</v>
+        <f>$B15&amp;"ParamTransform"</f>
+        <v>negBinomXParamTransform</v>
       </c>
       <c r="AA15" t="str">
-        <f t="shared" si="3"/>
-        <v>expPDF</v>
+        <f>$B15&amp;"PDF"</f>
+        <v>negBinomXPDF</v>
       </c>
       <c r="AB15" t="str">
         <f>B15&amp;"PlotDistr"</f>
-        <v>expPlotDistr</v>
+        <v>negBinomXPlotDistr</v>
       </c>
       <c r="AC15" t="str">
         <f>B15&amp;"Draws"</f>
-        <v>expDraws</v>
+        <v>negBinomXDraws</v>
       </c>
       <c r="AD15" t="str">
         <f>B15&amp;"Latex"</f>
-        <v>expLatex</v>
+        <v>negBinomXLatex</v>
       </c>
       <c r="AE15" t="str">
-        <f t="shared" si="4"/>
-        <v>expChartDomain</v>
+        <f>$B15&amp;"ChartDomain"</f>
+        <v>negBinomXChartDomain</v>
       </c>
       <c r="AF15" t="str">
-        <f t="shared" si="5"/>
-        <v>expLikelihoodFun</v>
+        <f>$B15&amp;"LikelihoodFun"</f>
+        <v>negBinomXLikelihoodFun</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16">
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
@@ -2489,7 +2515,7 @@
         <v>24</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>89</v>
@@ -2498,10 +2524,10 @@
         <v>48</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>38</v>
@@ -2519,10 +2545,10 @@
         <v>78</v>
       </c>
       <c r="R16" s="1">
-        <v>-2</v>
+        <v>0.25</v>
       </c>
       <c r="S16" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>64</v>
@@ -2535,7 +2561,7 @@
       </c>
       <c r="W16" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
+        <v>"&amp;lambda;"</v>
       </c>
       <c r="X16" t="str">
         <f>IF(F16=1,"""none""",IF(E16=F16,"""betas""","""fullNorm"""))</f>
@@ -2543,64 +2569,65 @@
       </c>
       <c r="Y16" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="2"/>
-        <v>expExpParamTransform</v>
+        <v>expParamTransform</v>
       </c>
       <c r="AA16" t="str">
         <f t="shared" si="3"/>
-        <v>expExpPDF</v>
+        <v>expPDF</v>
       </c>
       <c r="AB16" t="str">
         <f>B16&amp;"PlotDistr"</f>
-        <v>expExpPlotDistr</v>
+        <v>expPlotDistr</v>
       </c>
       <c r="AC16" t="str">
         <f>B16&amp;"Draws"</f>
-        <v>expExpDraws</v>
+        <v>expDraws</v>
       </c>
       <c r="AD16" t="str">
         <f>B16&amp;"Latex"</f>
-        <v>expExpLatex</v>
+        <v>expLatex</v>
       </c>
       <c r="AE16" t="str">
         <f t="shared" si="4"/>
-        <v>expExpChartDomain</v>
+        <v>expChartDomain</v>
       </c>
       <c r="AF16" t="str">
         <f t="shared" si="5"/>
-        <v>expExpLikelihoodFun</v>
+        <v>expLikelihoodFun</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>48</v>
@@ -2627,13 +2654,13 @@
         <v>78</v>
       </c>
       <c r="R17" s="1">
-        <v>-0.5</v>
+        <v>-2</v>
       </c>
       <c r="S17" s="1">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>70</v>
@@ -2647,53 +2674,54 @@
       </c>
       <c r="X17" t="str">
         <f>IF(F17=1,"""none""",IF(E17=F17,"""betas""","""fullNorm"""))</f>
-        <v>"betas"</v>
+        <v>"none"</v>
       </c>
       <c r="Y17" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="2"/>
-        <v>expExpXParamTransform</v>
+        <v>expExpParamTransform</v>
       </c>
       <c r="AA17" t="str">
         <f t="shared" si="3"/>
-        <v>expExpXPDF</v>
+        <v>expExpPDF</v>
       </c>
       <c r="AB17" t="str">
         <f>B17&amp;"PlotDistr"</f>
-        <v>expExpXPlotDistr</v>
+        <v>expExpPlotDistr</v>
       </c>
       <c r="AC17" t="str">
         <f>B17&amp;"Draws"</f>
-        <v>expExpXDraws</v>
+        <v>expExpDraws</v>
       </c>
       <c r="AD17" t="str">
         <f>B17&amp;"Latex"</f>
-        <v>expExpXLatex</v>
+        <v>expExpLatex</v>
       </c>
       <c r="AE17" t="str">
         <f t="shared" si="4"/>
-        <v>expExpXChartDomain</v>
+        <v>expExpChartDomain</v>
       </c>
       <c r="AF17" t="str">
         <f t="shared" si="5"/>
-        <v>expExpXLikelihoodFun</v>
+        <v>expExpLikelihoodFun</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18">
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>124</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>87</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1">
         <v>3</v>
@@ -2705,7 +2733,7 @@
         <v>24</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>90</v>
@@ -2732,7 +2760,7 @@
         <v>80</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="R18" s="1">
         <v>-0.5</v>
@@ -2763,42 +2791,43 @@
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="2"/>
-        <v>neumayerParamTransform</v>
+        <v>expExpXParamTransform</v>
       </c>
       <c r="AA18" t="str">
         <f t="shared" si="3"/>
-        <v>neumayerPDF</v>
+        <v>expExpXPDF</v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" ref="AB18" si="11">B18&amp;"PlotDistr"</f>
-        <v>neumayerPlotDistr</v>
+        <f>B18&amp;"PlotDistr"</f>
+        <v>expExpXPlotDistr</v>
       </c>
       <c r="AC18" t="str">
-        <f t="shared" ref="AC18" si="12">B18&amp;"Draws"</f>
-        <v>neumayerDraws</v>
+        <f>B18&amp;"Draws"</f>
+        <v>expExpXDraws</v>
       </c>
       <c r="AD18" t="str">
-        <f t="shared" ref="AD18" si="13">B18&amp;"Latex"</f>
-        <v>neumayerLatex</v>
+        <f>B18&amp;"Latex"</f>
+        <v>expExpXLatex</v>
       </c>
       <c r="AE18" t="str">
         <f t="shared" si="4"/>
-        <v>neumayerChartDomain</v>
+        <v>expExpXChartDomain</v>
       </c>
       <c r="AF18" t="str">
         <f t="shared" si="5"/>
-        <v>neumayerLikelihoodFun</v>
+        <v>expExpXLikelihoodFun</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19">
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>87</v>
@@ -2813,7 +2842,7 @@
         <v>24</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>90</v>
@@ -2871,29 +2900,138 @@
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="2"/>
-        <v>drehJenParamTransform</v>
+        <v>neumayerParamTransform</v>
       </c>
       <c r="AA19" t="str">
         <f t="shared" si="3"/>
-        <v>drehJenPDF</v>
+        <v>neumayerPDF</v>
       </c>
       <c r="AB19" t="str">
-        <f>B19&amp;"PlotDistr"</f>
-        <v>drehJenPlotDistr</v>
+        <f t="shared" ref="AB19" si="17">B19&amp;"PlotDistr"</f>
+        <v>neumayerPlotDistr</v>
       </c>
       <c r="AC19" t="str">
-        <f>B19&amp;"Draws"</f>
-        <v>drehJenDraws</v>
+        <f t="shared" ref="AC19" si="18">B19&amp;"Draws"</f>
+        <v>neumayerDraws</v>
       </c>
       <c r="AD19" t="str">
-        <f>B19&amp;"Latex"</f>
-        <v>drehJenLatex</v>
+        <f t="shared" ref="AD19" si="19">B19&amp;"Latex"</f>
+        <v>neumayerLatex</v>
       </c>
       <c r="AE19" t="str">
         <f t="shared" si="4"/>
+        <v>neumayerChartDomain</v>
+      </c>
+      <c r="AF19" t="str">
+        <f t="shared" si="5"/>
+        <v>neumayerLikelihoodFun</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="R20" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V20">
+        <v>0.01</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="X20" t="str">
+        <f>IF(F20=1,"""none""",IF(E20=F20,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
+      </c>
+      <c r="Y20" t="str">
+        <f t="shared" si="1"/>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="Z20" t="str">
+        <f t="shared" si="2"/>
+        <v>drehJenParamTransform</v>
+      </c>
+      <c r="AA20" t="str">
+        <f t="shared" si="3"/>
+        <v>drehJenPDF</v>
+      </c>
+      <c r="AB20" t="str">
+        <f>B20&amp;"PlotDistr"</f>
+        <v>drehJenPlotDistr</v>
+      </c>
+      <c r="AC20" t="str">
+        <f>B20&amp;"Draws"</f>
+        <v>drehJenDraws</v>
+      </c>
+      <c r="AD20" t="str">
+        <f>B20&amp;"Latex"</f>
+        <v>drehJenLatex</v>
+      </c>
+      <c r="AE20" t="str">
+        <f t="shared" si="4"/>
         <v>drehJenChartDomain</v>
       </c>
-      <c r="AF19" t="str">
+      <c r="AF20" t="str">
         <f t="shared" si="5"/>
         <v>drehJenLikelihoodFun</v>
       </c>

</xml_diff>

<commit_message>
update for order probit; rework of guesstimate plot for discrete case
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC05DD00-A097-4180-9A12-B20CF784C4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382C030B-5C87-4AA7-A0B1-26886058394C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -838,7 +838,7 @@
   <dimension ref="A1:AF20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1010,7 @@
         <v>49</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>70</v>
@@ -1119,7 +1119,7 @@
         <v>49</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>70</v>
@@ -1228,7 +1228,7 @@
         <v>49</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>70</v>
@@ -1337,7 +1337,7 @@
         <v>49</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
a bunch of fixes for probit
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5494402E-A49A-462A-9B3F-5B0D9A02C77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A8ED63-685F-46F5-881E-05D487B03066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -847,7 +847,7 @@
   <dimension ref="A1:AG20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,10 +1482,10 @@
         <v>79</v>
       </c>
       <c r="S6" s="1">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="T6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>63</v>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="Z6" t="str">
         <f t="shared" ref="Z6" si="10">"manyParamSliderMaker(minVal ="&amp;S6&amp;", maxVal = "&amp;T6&amp;", startVals = "&amp;U6&amp;", stepVal = "&amp;W6&amp;", paramHTML = "&amp;X6&amp;", multi = "&amp;Y6&amp;", sigmaScale ="&amp;V6&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
math updates; first draft of ord. logit
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FACCFD-FB37-4A38-B9A3-FD984FB23BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DD2C95-6080-466C-AD38-5A6D8269E291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="156">
   <si>
     <t>Poisson</t>
   </si>
@@ -481,6 +481,27 @@
   </si>
   <si>
     <t>c(1,-1,1.25)</t>
+  </si>
+  <si>
+    <t>orderedLogitX</t>
+  </si>
+  <si>
+    <t>Ordered Logit (X)</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>list("Ordered Logit (X)")</t>
+  </si>
+  <si>
+    <t>yStarPDF</t>
+  </si>
+  <si>
+    <t>styNormPDF</t>
+  </si>
+  <si>
+    <t>styLogPDF</t>
   </si>
 </sst>
 </file>
@@ -847,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:AG20"/>
+  <dimension ref="A1:AH21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,18 +890,18 @@
     <col min="17" max="18" width="9.42578125" customWidth="1"/>
     <col min="19" max="19" width="6.140625" customWidth="1"/>
     <col min="20" max="20" width="4.28515625" customWidth="1"/>
-    <col min="21" max="22" width="7.140625" customWidth="1"/>
-    <col min="23" max="23" width="6" customWidth="1"/>
-    <col min="24" max="25" width="4.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16" customWidth="1"/>
-    <col min="27" max="28" width="26" customWidth="1"/>
-    <col min="29" max="29" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="15.5703125" customWidth="1"/>
+    <col min="21" max="23" width="7.140625" customWidth="1"/>
+    <col min="24" max="24" width="6" customWidth="1"/>
+    <col min="25" max="26" width="4.28515625" customWidth="1"/>
+    <col min="27" max="27" width="16" customWidth="1"/>
+    <col min="28" max="29" width="26" customWidth="1"/>
+    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -948,40 +969,43 @@
         <v>92</v>
       </c>
       <c r="W1" t="s">
+        <v>153</v>
+      </c>
+      <c r="X1" t="s">
         <v>58</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>60</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>61</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>74</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>22</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1048,51 +1072,54 @@
       <c r="V2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X2">
         <v>0.01</v>
       </c>
-      <c r="X2" t="str">
-        <f t="shared" ref="X2:X20" si="0">"""&amp;"&amp;RIGHT(M2,LEN(M2)-1)&amp;";"""</f>
+      <c r="Y2" t="str">
+        <f t="shared" ref="Y2:Y21" si="0">"""&amp;"&amp;RIGHT(M2,LEN(M2)-1)&amp;";"""</f>
         <v>"&amp;pi;"</v>
       </c>
-      <c r="Y2" t="str">
+      <c r="Z2" t="str">
         <f>IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
-      <c r="Z2" t="str">
-        <f t="shared" ref="Z2:Z20" si="1">"manyParamSliderMaker(minVal ="&amp;S2&amp;", maxVal = "&amp;T2&amp;", startVals = "&amp;U2&amp;", stepVal = "&amp;W2&amp;", paramHTML = "&amp;X2&amp;", multi = "&amp;Y2&amp;", sigmaScale ="&amp;V2&amp;","</f>
+      <c r="AA2" t="str">
+        <f t="shared" ref="AA2:AA21" si="1">"manyParamSliderMaker(minVal ="&amp;S2&amp;", maxVal = "&amp;T2&amp;", startVals = "&amp;U2&amp;", stepVal = "&amp;X2&amp;", paramHTML = "&amp;Y2&amp;", multi = "&amp;Z2&amp;", sigmaScale ="&amp;V2&amp;","</f>
         <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AA2" t="str">
+      <c r="AB2" t="str">
         <f>$B2&amp;"ParamTransform"</f>
         <v>bernParamTransform</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AC2" t="str">
         <f>$B2&amp;"PDF"</f>
         <v>bernPDF</v>
       </c>
-      <c r="AC2" t="str">
+      <c r="AD2" t="str">
         <f>B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
-      <c r="AD2" t="str">
+      <c r="AE2" t="str">
         <f>B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
-      <c r="AE2" t="str">
+      <c r="AF2" t="str">
         <f>B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
-      <c r="AF2" t="str">
+      <c r="AG2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="AG2" t="str">
+      <c r="AH2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1160,53 +1187,56 @@
       <c r="V3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X3">
         <v>0.01</v>
       </c>
-      <c r="X3" t="str">
+      <c r="Y3" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y3" t="str">
+      <c r="Z3" t="str">
         <f>IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
-      <c r="Z3" t="str">
+      <c r="AA3" t="str">
         <f t="shared" si="1"/>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AA3" t="str">
-        <f t="shared" ref="AA3:AA20" si="2">$B3&amp;"ParamTransform"</f>
+      <c r="AB3" t="str">
+        <f t="shared" ref="AB3:AB21" si="2">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
-      <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB20" si="3">$B3&amp;"PDF"</f>
+      <c r="AC3" t="str">
+        <f t="shared" ref="AC3:AC21" si="3">$B3&amp;"PDF"</f>
         <v>bernLogitPDF</v>
       </c>
-      <c r="AC3" t="str">
+      <c r="AD3" t="str">
         <f>B3&amp;"PlotDistr"</f>
         <v>bernLogitPlotDistr</v>
       </c>
-      <c r="AD3" t="str">
+      <c r="AE3" t="str">
         <f>B3&amp;"Draws"</f>
         <v>bernLogitDraws</v>
       </c>
-      <c r="AE3" t="str">
+      <c r="AF3" t="str">
         <f>B3&amp;"Latex"</f>
         <v>bernLogitLatex</v>
       </c>
-      <c r="AF3" t="str">
-        <f t="shared" ref="AF3:AF20" si="4">$B3&amp;"ChartDomain"</f>
+      <c r="AG3" t="str">
+        <f t="shared" ref="AG3:AG21" si="4">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
-      <c r="AG3" t="str">
-        <f t="shared" ref="AG3:AG20" si="5">$B3&amp;"LikelihoodFun"</f>
+      <c r="AH3" t="str">
+        <f t="shared" ref="AH3:AH21" si="5">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A20" si="6">A3+1</f>
+        <f t="shared" ref="A4:A21" si="6">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1272,51 +1302,54 @@
       <c r="V4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X4">
         <v>0.01</v>
       </c>
-      <c r="X4" t="str">
+      <c r="Y4" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y4" t="str">
+      <c r="Z4" t="str">
         <f>IF(F4=1,"""none""",IF(E4=F4,"""betas""","""fullNorm"""))</f>
         <v>"betas"</v>
       </c>
-      <c r="Z4" t="str">
+      <c r="AA4" t="str">
         <f t="shared" si="1"/>
         <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AA4" t="str">
+      <c r="AB4" t="str">
         <f t="shared" si="2"/>
         <v>bernLogitXParamTransform</v>
       </c>
-      <c r="AB4" t="str">
+      <c r="AC4" t="str">
         <f t="shared" si="3"/>
         <v>bernLogitXPDF</v>
       </c>
-      <c r="AC4" t="str">
+      <c r="AD4" t="str">
         <f>B4&amp;"PlotDistr"</f>
         <v>bernLogitXPlotDistr</v>
       </c>
-      <c r="AD4" t="str">
+      <c r="AE4" t="str">
         <f>B4&amp;"Draws"</f>
         <v>bernLogitXDraws</v>
       </c>
-      <c r="AE4" t="str">
+      <c r="AF4" t="str">
         <f>B4&amp;"Latex"</f>
         <v>bernLogitXLatex</v>
       </c>
-      <c r="AF4" t="str">
+      <c r="AG4" t="str">
         <f t="shared" si="4"/>
         <v>bernLogitXChartDomain</v>
       </c>
-      <c r="AG4" t="str">
+      <c r="AH4" t="str">
         <f t="shared" si="5"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -1384,51 +1417,54 @@
       <c r="V5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X5">
         <v>0.01</v>
       </c>
-      <c r="X5" t="str">
-        <f t="shared" ref="X5" si="7">"""&amp;"&amp;RIGHT(M5,LEN(M5)-1)&amp;";"""</f>
+      <c r="Y5" t="str">
+        <f t="shared" ref="Y5" si="7">"""&amp;"&amp;RIGHT(M5,LEN(M5)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y5" t="str">
+      <c r="Z5" t="str">
         <f>IF(F5=1,"""none""",IF(E5=F5,"""betas""","""fullNorm"""))</f>
         <v>"betas"</v>
       </c>
-      <c r="Z5" t="str">
-        <f t="shared" ref="Z5" si="8">"manyParamSliderMaker(minVal ="&amp;S5&amp;", maxVal = "&amp;T5&amp;", startVals = "&amp;U5&amp;", stepVal = "&amp;W5&amp;", paramHTML = "&amp;X5&amp;", multi = "&amp;Y5&amp;", sigmaScale ="&amp;V5&amp;","</f>
+      <c r="AA5" t="str">
+        <f t="shared" ref="AA5" si="8">"manyParamSliderMaker(minVal ="&amp;S5&amp;", maxVal = "&amp;T5&amp;", startVals = "&amp;U5&amp;", stepVal = "&amp;X5&amp;", paramHTML = "&amp;Y5&amp;", multi = "&amp;Z5&amp;", sigmaScale ="&amp;V5&amp;","</f>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AA5" t="str">
+      <c r="AB5" t="str">
         <f t="shared" si="2"/>
         <v>bernProbitXParamTransform</v>
       </c>
-      <c r="AB5" t="str">
+      <c r="AC5" t="str">
         <f t="shared" si="3"/>
         <v>bernProbitXPDF</v>
       </c>
-      <c r="AC5" t="str">
+      <c r="AD5" t="str">
         <f>B5&amp;"PlotDistr"</f>
         <v>bernProbitXPlotDistr</v>
       </c>
-      <c r="AD5" t="str">
+      <c r="AE5" t="str">
         <f>B5&amp;"Draws"</f>
         <v>bernProbitXDraws</v>
       </c>
-      <c r="AE5" t="str">
+      <c r="AF5" t="str">
         <f>B5&amp;"Latex"</f>
         <v>bernProbitXLatex</v>
       </c>
-      <c r="AF5" t="str">
+      <c r="AG5" t="str">
         <f t="shared" si="4"/>
         <v>bernProbitXChartDomain</v>
       </c>
-      <c r="AG5" t="str">
+      <c r="AH5" t="str">
         <f t="shared" si="5"/>
         <v>bernProbitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -1440,7 +1476,7 @@
         <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
@@ -1496,84 +1532,87 @@
       <c r="V6" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="X6">
         <v>0.01</v>
       </c>
-      <c r="X6" t="str">
-        <f t="shared" ref="X6" si="9">"""&amp;"&amp;RIGHT(M6,LEN(M6)-1)&amp;";"""</f>
+      <c r="Y6" t="str">
+        <f t="shared" ref="Y6" si="9">"""&amp;"&amp;RIGHT(M6,LEN(M6)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y6" t="str">
+      <c r="Z6" t="str">
         <f>IF(F6=1,"""none""",IF(E6=F6,"""betas""","""fullNorm"""))</f>
         <v>"fullNorm"</v>
       </c>
-      <c r="Z6" t="str">
-        <f t="shared" ref="Z6" si="10">"manyParamSliderMaker(minVal ="&amp;S6&amp;", maxVal = "&amp;T6&amp;", startVals = "&amp;U6&amp;", stepVal = "&amp;W6&amp;", paramHTML = "&amp;X6&amp;", multi = "&amp;Y6&amp;", sigmaScale ="&amp;V6&amp;","</f>
+      <c r="AA6" t="str">
+        <f t="shared" ref="AA6" si="10">"manyParamSliderMaker(minVal ="&amp;S6&amp;", maxVal = "&amp;T6&amp;", startVals = "&amp;U6&amp;", stepVal = "&amp;X6&amp;", paramHTML = "&amp;Y6&amp;", multi = "&amp;Z6&amp;", sigmaScale ="&amp;V6&amp;","</f>
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
       </c>
-      <c r="AA6" t="str">
+      <c r="AB6" t="str">
         <f t="shared" si="2"/>
         <v>orderedProbitXParamTransform</v>
       </c>
-      <c r="AB6" t="str">
+      <c r="AC6" t="str">
         <f t="shared" si="3"/>
         <v>orderedProbitXPDF</v>
       </c>
-      <c r="AC6" t="str">
-        <f t="shared" ref="AC6" si="11">B6&amp;"PlotDistr"</f>
+      <c r="AD6" t="str">
+        <f t="shared" ref="AD6" si="11">B6&amp;"PlotDistr"</f>
         <v>orderedProbitXPlotDistr</v>
       </c>
-      <c r="AD6" t="str">
-        <f t="shared" ref="AD6" si="12">B6&amp;"Draws"</f>
+      <c r="AE6" t="str">
+        <f t="shared" ref="AE6" si="12">B6&amp;"Draws"</f>
         <v>orderedProbitXDraws</v>
       </c>
-      <c r="AE6" t="str">
-        <f t="shared" ref="AE6" si="13">B6&amp;"Latex"</f>
+      <c r="AF6" t="str">
+        <f t="shared" ref="AF6" si="13">B6&amp;"Latex"</f>
         <v>orderedProbitXLatex</v>
       </c>
-      <c r="AF6" t="str">
+      <c r="AG6" t="str">
         <f t="shared" si="4"/>
         <v>orderedProbitXChartDomain</v>
       </c>
-      <c r="AG6" t="str">
+      <c r="AH6" t="str">
         <f t="shared" si="5"/>
         <v>orderedProbitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>146</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>28</v>
@@ -1582,104 +1621,107 @@
         <v>37</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="S7" s="1">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="T7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="W7">
+        <v>137</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="X7">
         <v>0.01</v>
       </c>
-      <c r="X7" t="str">
-        <f t="shared" si="0"/>
+      <c r="Y7" t="str">
+        <f t="shared" ref="Y7" si="14">"""&amp;"&amp;RIGHT(M7,LEN(M7)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y7" t="str">
+      <c r="Z7" t="str">
         <f>IF(F7=1,"""none""",IF(E7=F7,"""betas""","""fullNorm"""))</f>
-        <v>"none"</v>
-      </c>
-      <c r="Z7" t="str">
-        <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+        <v>"fullNorm"</v>
       </c>
       <c r="AA7" t="str">
+        <f t="shared" ref="AA7" si="15">"manyParamSliderMaker(minVal ="&amp;S7&amp;", maxVal = "&amp;T7&amp;", startVals = "&amp;U7&amp;", stepVal = "&amp;X7&amp;", paramHTML = "&amp;Y7&amp;", multi = "&amp;Z7&amp;", sigmaScale ="&amp;V7&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+      </c>
+      <c r="AB7" t="str">
         <f t="shared" si="2"/>
-        <v>styNormParamTransform</v>
-      </c>
-      <c r="AB7" t="str">
+        <v>orderedLogitXParamTransform</v>
+      </c>
+      <c r="AC7" t="str">
         <f t="shared" si="3"/>
-        <v>styNormPDF</v>
-      </c>
-      <c r="AC7" t="str">
-        <f>B7&amp;"PlotDistr"</f>
-        <v>styNormPlotDistr</v>
+        <v>orderedLogitXPDF</v>
       </c>
       <c r="AD7" t="str">
-        <f>B7&amp;"Draws"</f>
-        <v>styNormDraws</v>
+        <f t="shared" ref="AD7" si="16">B7&amp;"PlotDistr"</f>
+        <v>orderedLogitXPlotDistr</v>
       </c>
       <c r="AE7" t="str">
-        <f>B7&amp;"Latex"</f>
-        <v>styNormLatex</v>
+        <f t="shared" ref="AE7" si="17">B7&amp;"Draws"</f>
+        <v>orderedLogitXDraws</v>
       </c>
       <c r="AF7" t="str">
+        <f t="shared" ref="AF7" si="18">B7&amp;"Latex"</f>
+        <v>orderedLogitXLatex</v>
+      </c>
+      <c r="AG7" t="str">
         <f t="shared" si="4"/>
-        <v>styNormChartDomain</v>
-      </c>
-      <c r="AG7" t="str">
+        <v>orderedLogitXChartDomain</v>
+      </c>
+      <c r="AH7" t="str">
         <f t="shared" si="5"/>
-        <v>styNormLikelihoodFun</v>
+        <v>orderedLogitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>146</v>
@@ -1697,7 +1739,7 @@
         <v>40</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>84</v>
@@ -1709,89 +1751,92 @@
         <v>133</v>
       </c>
       <c r="S8" s="1">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="T8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X8">
         <v>0.01</v>
       </c>
-      <c r="X8" t="str">
+      <c r="Y8" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y8" t="str">
+      <c r="Z8" t="str">
         <f>IF(F8=1,"""none""",IF(E8=F8,"""betas""","""fullNorm"""))</f>
-        <v>"betas"</v>
-      </c>
-      <c r="Z8" t="str">
+        <v>"none"</v>
+      </c>
+      <c r="AA8" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AA8" t="str">
+        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB8" t="str">
         <f t="shared" si="2"/>
-        <v>styNormXParamTransform</v>
-      </c>
-      <c r="AB8" t="str">
+        <v>styNormParamTransform</v>
+      </c>
+      <c r="AC8" t="str">
         <f t="shared" si="3"/>
-        <v>styNormXPDF</v>
-      </c>
-      <c r="AC8" t="str">
+        <v>styNormPDF</v>
+      </c>
+      <c r="AD8" t="str">
         <f>B8&amp;"PlotDistr"</f>
-        <v>styNormXPlotDistr</v>
-      </c>
-      <c r="AD8" t="str">
+        <v>styNormPlotDistr</v>
+      </c>
+      <c r="AE8" t="str">
         <f>B8&amp;"Draws"</f>
-        <v>styNormXDraws</v>
-      </c>
-      <c r="AE8" t="str">
+        <v>styNormDraws</v>
+      </c>
+      <c r="AF8" t="str">
         <f>B8&amp;"Latex"</f>
-        <v>styNormXLatex</v>
-      </c>
-      <c r="AF8" t="str">
+        <v>styNormLatex</v>
+      </c>
+      <c r="AG8" t="str">
         <f t="shared" si="4"/>
-        <v>styNormXChartDomain</v>
-      </c>
-      <c r="AG8" t="str">
+        <v>styNormChartDomain</v>
+      </c>
+      <c r="AH8" t="str">
         <f t="shared" si="5"/>
-        <v>styNormXLikelihoodFun</v>
+        <v>styNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>146</v>
@@ -1800,7 +1845,7 @@
         <v>52</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>37</v>
@@ -1815,10 +1860,10 @@
         <v>84</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="S9" s="1">
         <v>-3</v>
@@ -1827,92 +1872,95 @@
         <v>3</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="W9">
+        <v>70</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X9">
         <v>0.01</v>
       </c>
-      <c r="X9" t="str">
+      <c r="Y9" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y9" t="str">
+      <c r="Z9" t="str">
         <f>IF(F9=1,"""none""",IF(E9=F9,"""betas""","""fullNorm"""))</f>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="Z9" t="str">
+        <v>"betas"</v>
+      </c>
+      <c r="AA9" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
-      </c>
-      <c r="AA9" t="str">
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AB9" t="str">
         <f t="shared" si="2"/>
-        <v>fullNormXParamTransform</v>
-      </c>
-      <c r="AB9" t="str">
+        <v>styNormXParamTransform</v>
+      </c>
+      <c r="AC9" t="str">
         <f t="shared" si="3"/>
-        <v>fullNormXPDF</v>
-      </c>
-      <c r="AC9" t="str">
+        <v>styNormXPDF</v>
+      </c>
+      <c r="AD9" t="str">
         <f>B9&amp;"PlotDistr"</f>
-        <v>fullNormXPlotDistr</v>
-      </c>
-      <c r="AD9" t="str">
+        <v>styNormXPlotDistr</v>
+      </c>
+      <c r="AE9" t="str">
         <f>B9&amp;"Draws"</f>
-        <v>fullNormXDraws</v>
-      </c>
-      <c r="AE9" t="str">
+        <v>styNormXDraws</v>
+      </c>
+      <c r="AF9" t="str">
         <f>B9&amp;"Latex"</f>
-        <v>fullNormXLatex</v>
-      </c>
-      <c r="AF9" t="str">
+        <v>styNormXLatex</v>
+      </c>
+      <c r="AG9" t="str">
         <f t="shared" si="4"/>
-        <v>fullNormXChartDomain</v>
-      </c>
-      <c r="AG9" t="str">
+        <v>styNormXChartDomain</v>
+      </c>
+      <c r="AH9" t="str">
         <f t="shared" si="5"/>
-        <v>fullNormXLikelihoodFun</v>
+        <v>styNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>146</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>37</v>
@@ -1921,101 +1969,104 @@
         <v>40</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="S10" s="1">
-        <v>-0.5</v>
+        <v>-3</v>
       </c>
       <c r="T10" s="1">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="W10">
+        <v>137</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X10">
         <v>0.01</v>
       </c>
-      <c r="X10" t="str">
+      <c r="Y10" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y10" t="str">
+      <c r="Z10" t="str">
         <f>IF(F10=1,"""none""",IF(E10=F10,"""betas""","""fullNorm"""))</f>
-        <v>"none"</v>
-      </c>
-      <c r="Z10" t="str">
+        <v>"fullNorm"</v>
+      </c>
+      <c r="AA10" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AA10" t="str">
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+      </c>
+      <c r="AB10" t="str">
         <f t="shared" si="2"/>
-        <v>logNormParamTransform</v>
-      </c>
-      <c r="AB10" t="str">
+        <v>fullNormXParamTransform</v>
+      </c>
+      <c r="AC10" t="str">
         <f t="shared" si="3"/>
-        <v>logNormPDF</v>
-      </c>
-      <c r="AC10" t="str">
+        <v>fullNormXPDF</v>
+      </c>
+      <c r="AD10" t="str">
         <f>B10&amp;"PlotDistr"</f>
-        <v>logNormPlotDistr</v>
-      </c>
-      <c r="AD10" t="str">
+        <v>fullNormXPlotDistr</v>
+      </c>
+      <c r="AE10" t="str">
         <f>B10&amp;"Draws"</f>
-        <v>logNormDraws</v>
-      </c>
-      <c r="AE10" t="str">
+        <v>fullNormXDraws</v>
+      </c>
+      <c r="AF10" t="str">
         <f>B10&amp;"Latex"</f>
-        <v>logNormLatex</v>
-      </c>
-      <c r="AF10" t="str">
+        <v>fullNormXLatex</v>
+      </c>
+      <c r="AG10" t="str">
         <f t="shared" si="4"/>
-        <v>logNormChartDomain</v>
-      </c>
-      <c r="AG10" t="str">
+        <v>fullNormXChartDomain</v>
+      </c>
+      <c r="AH10" t="str">
         <f t="shared" si="5"/>
-        <v>logNormLikelihoodFun</v>
+        <v>fullNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>110</v>
       </c>
       <c r="E11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>146</v>
@@ -2033,13 +2084,13 @@
         <v>40</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>76</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>93</v>
@@ -2051,177 +2102,183 @@
         <v>0.5</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X11">
         <v>0.01</v>
       </c>
-      <c r="X11" t="str">
+      <c r="Y11" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y11" t="str">
+      <c r="Z11" t="str">
         <f>IF(F11=1,"""none""",IF(E11=F11,"""betas""","""fullNorm"""))</f>
-        <v>"betas"</v>
-      </c>
-      <c r="Z11" t="str">
+        <v>"none"</v>
+      </c>
+      <c r="AA11" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AA11" t="str">
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB11" t="str">
         <f t="shared" si="2"/>
-        <v>logNormXParamTransform</v>
-      </c>
-      <c r="AB11" t="str">
+        <v>logNormParamTransform</v>
+      </c>
+      <c r="AC11" t="str">
         <f t="shared" si="3"/>
-        <v>logNormXPDF</v>
-      </c>
-      <c r="AC11" t="str">
+        <v>logNormPDF</v>
+      </c>
+      <c r="AD11" t="str">
         <f>B11&amp;"PlotDistr"</f>
-        <v>logNormXPlotDistr</v>
-      </c>
-      <c r="AD11" t="str">
+        <v>logNormPlotDistr</v>
+      </c>
+      <c r="AE11" t="str">
         <f>B11&amp;"Draws"</f>
-        <v>logNormXDraws</v>
-      </c>
-      <c r="AE11" t="str">
+        <v>logNormDraws</v>
+      </c>
+      <c r="AF11" t="str">
         <f>B11&amp;"Latex"</f>
-        <v>logNormXLatex</v>
-      </c>
-      <c r="AF11" t="str">
+        <v>logNormLatex</v>
+      </c>
+      <c r="AG11" t="str">
         <f t="shared" si="4"/>
-        <v>logNormXChartDomain</v>
-      </c>
-      <c r="AG11" t="str">
+        <v>logNormChartDomain</v>
+      </c>
+      <c r="AH11" t="str">
         <f t="shared" si="5"/>
-        <v>logNormXLikelihoodFun</v>
+        <v>logNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>146</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="S12" s="1">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="T12" s="1">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X12">
         <v>0.01</v>
       </c>
-      <c r="X12" t="str">
+      <c r="Y12" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;lambda;"</v>
-      </c>
-      <c r="Y12" t="str">
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z12" t="str">
         <f>IF(F12=1,"""none""",IF(E12=F12,"""betas""","""fullNorm"""))</f>
-        <v>"none"</v>
-      </c>
-      <c r="Z12" t="str">
+        <v>"betas"</v>
+      </c>
+      <c r="AA12" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AA12" t="str">
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AB12" t="str">
         <f t="shared" si="2"/>
-        <v>poisParamTransform</v>
-      </c>
-      <c r="AB12" t="str">
+        <v>logNormXParamTransform</v>
+      </c>
+      <c r="AC12" t="str">
         <f t="shared" si="3"/>
-        <v>poisPDF</v>
-      </c>
-      <c r="AC12" t="str">
+        <v>logNormXPDF</v>
+      </c>
+      <c r="AD12" t="str">
         <f>B12&amp;"PlotDistr"</f>
-        <v>poisPlotDistr</v>
-      </c>
-      <c r="AD12" t="str">
+        <v>logNormXPlotDistr</v>
+      </c>
+      <c r="AE12" t="str">
         <f>B12&amp;"Draws"</f>
-        <v>poisDraws</v>
-      </c>
-      <c r="AE12" t="str">
+        <v>logNormXDraws</v>
+      </c>
+      <c r="AF12" t="str">
         <f>B12&amp;"Latex"</f>
-        <v>poisLatex</v>
-      </c>
-      <c r="AF12" t="str">
+        <v>logNormXLatex</v>
+      </c>
+      <c r="AG12" t="str">
         <f t="shared" si="4"/>
-        <v>poisChartDomain</v>
-      </c>
-      <c r="AG12" t="str">
+        <v>logNormXChartDomain</v>
+      </c>
+      <c r="AH12" t="str">
         <f t="shared" si="5"/>
-        <v>poisLikelihoodFun</v>
+        <v>logNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
@@ -2236,7 +2293,7 @@
         <v>23</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>89</v>
@@ -2248,110 +2305,113 @@
         <v>53</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>38</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>77</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>78</v>
       </c>
       <c r="S13" s="1">
-        <v>-0.25</v>
+        <v>1</v>
       </c>
       <c r="T13" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="V13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X13">
         <v>0.01</v>
       </c>
-      <c r="X13" t="str">
+      <c r="Y13" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Y13" t="str">
+        <v>"&amp;lambda;"</v>
+      </c>
+      <c r="Z13" t="str">
         <f>IF(F13=1,"""none""",IF(E13=F13,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
-      <c r="Z13" t="str">
+      <c r="AA13" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AA13" t="str">
+        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB13" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpParamTransform</v>
-      </c>
-      <c r="AB13" t="str">
+        <v>poisParamTransform</v>
+      </c>
+      <c r="AC13" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpPDF</v>
-      </c>
-      <c r="AC13" t="str">
+        <v>poisPDF</v>
+      </c>
+      <c r="AD13" t="str">
         <f>B13&amp;"PlotDistr"</f>
-        <v>poisExpPlotDistr</v>
-      </c>
-      <c r="AD13" t="str">
+        <v>poisPlotDistr</v>
+      </c>
+      <c r="AE13" t="str">
         <f>B13&amp;"Draws"</f>
-        <v>poisExpDraws</v>
-      </c>
-      <c r="AE13" t="str">
+        <v>poisDraws</v>
+      </c>
+      <c r="AF13" t="str">
         <f>B13&amp;"Latex"</f>
-        <v>poisExpLatex</v>
-      </c>
-      <c r="AF13" t="str">
+        <v>poisLatex</v>
+      </c>
+      <c r="AG13" t="str">
         <f t="shared" si="4"/>
-        <v>poisExpChartDomain</v>
-      </c>
-      <c r="AG13" t="str">
+        <v>poisChartDomain</v>
+      </c>
+      <c r="AH13" t="str">
         <f t="shared" si="5"/>
-        <v>poisExpLikelihoodFun</v>
+        <v>poisLikelihoodFun</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>146</v>
@@ -2372,7 +2432,7 @@
         <v>45</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>72</v>
@@ -2387,92 +2447,95 @@
         <v>3</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="V14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X14">
         <v>0.01</v>
       </c>
-      <c r="X14" t="str">
+      <c r="Y14" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y14" t="str">
+      <c r="Z14" t="str">
         <f>IF(F14=1,"""none""",IF(E14=F14,"""betas""","""fullNorm"""))</f>
-        <v>"betas"</v>
-      </c>
-      <c r="Z14" t="str">
+        <v>"none"</v>
+      </c>
+      <c r="AA14" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AA14" t="str">
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB14" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpXParamTransform</v>
-      </c>
-      <c r="AB14" t="str">
+        <v>poisExpParamTransform</v>
+      </c>
+      <c r="AC14" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpXPDF</v>
-      </c>
-      <c r="AC14" t="str">
+        <v>poisExpPDF</v>
+      </c>
+      <c r="AD14" t="str">
         <f>B14&amp;"PlotDistr"</f>
-        <v>poisExpXPlotDistr</v>
-      </c>
-      <c r="AD14" t="str">
+        <v>poisExpPlotDistr</v>
+      </c>
+      <c r="AE14" t="str">
         <f>B14&amp;"Draws"</f>
-        <v>poisExpXDraws</v>
-      </c>
-      <c r="AE14" t="str">
+        <v>poisExpDraws</v>
+      </c>
+      <c r="AF14" t="str">
         <f>B14&amp;"Latex"</f>
-        <v>poisExpXLatex</v>
-      </c>
-      <c r="AF14" t="str">
+        <v>poisExpLatex</v>
+      </c>
+      <c r="AG14" t="str">
         <f t="shared" si="4"/>
-        <v>poisExpXChartDomain</v>
-      </c>
-      <c r="AG14" t="str">
+        <v>poisExpChartDomain</v>
+      </c>
+      <c r="AH14" t="str">
         <f t="shared" si="5"/>
-        <v>poisExpXLikelihoodFun</v>
+        <v>poisExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" s="1">
         <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>146</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>37</v>
@@ -2484,7 +2547,7 @@
         <v>45</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>72</v>
@@ -2496,98 +2559,101 @@
         <v>-0.25</v>
       </c>
       <c r="T15" s="1">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W15">
+        <v>70</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X15">
         <v>0.01</v>
       </c>
-      <c r="X15" t="str">
+      <c r="Y15" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y15" t="str">
+      <c r="Z15" t="str">
         <f>IF(F15=1,"""none""",IF(E15=F15,"""betas""","""fullNorm"""))</f>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="Z15" t="str">
+        <v>"betas"</v>
+      </c>
+      <c r="AA15" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 1.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1,2),</v>
-      </c>
-      <c r="AA15" t="str">
-        <f>$B15&amp;"ParamTransform"</f>
-        <v>negBinomXParamTransform</v>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="AB15" t="str">
-        <f>$B15&amp;"PDF"</f>
-        <v>negBinomXPDF</v>
+        <f t="shared" si="2"/>
+        <v>poisExpXParamTransform</v>
       </c>
       <c r="AC15" t="str">
+        <f t="shared" si="3"/>
+        <v>poisExpXPDF</v>
+      </c>
+      <c r="AD15" t="str">
         <f>B15&amp;"PlotDistr"</f>
-        <v>negBinomXPlotDistr</v>
-      </c>
-      <c r="AD15" t="str">
+        <v>poisExpXPlotDistr</v>
+      </c>
+      <c r="AE15" t="str">
         <f>B15&amp;"Draws"</f>
-        <v>negBinomXDraws</v>
-      </c>
-      <c r="AE15" t="str">
+        <v>poisExpXDraws</v>
+      </c>
+      <c r="AF15" t="str">
         <f>B15&amp;"Latex"</f>
-        <v>negBinomXLatex</v>
-      </c>
-      <c r="AF15" t="str">
-        <f>$B15&amp;"ChartDomain"</f>
-        <v>negBinomXChartDomain</v>
+        <v>poisExpXLatex</v>
       </c>
       <c r="AG15" t="str">
-        <f>$B15&amp;"LikelihoodFun"</f>
-        <v>negBinomXLikelihoodFun</v>
+        <f t="shared" si="4"/>
+        <v>poisExpXChartDomain</v>
+      </c>
+      <c r="AH15" t="str">
+        <f t="shared" si="5"/>
+        <v>poisExpXLikelihoodFun</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>146</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>38</v>
@@ -2596,80 +2662,83 @@
         <v>45</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>78</v>
       </c>
       <c r="S16" s="1">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="T16" s="1">
         <v>1.5</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="W16">
+        <v>96</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X16">
         <v>0.01</v>
       </c>
-      <c r="X16" t="str">
+      <c r="Y16" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;lambda;"</v>
-      </c>
-      <c r="Y16" t="str">
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z16" t="str">
         <f>IF(F16=1,"""none""",IF(E16=F16,"""betas""","""fullNorm"""))</f>
-        <v>"none"</v>
-      </c>
-      <c r="Z16" t="str">
+        <v>"fullNorm"</v>
+      </c>
+      <c r="AA16" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AA16" t="str">
-        <f t="shared" si="2"/>
-        <v>expParamTransform</v>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 1.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1,2),</v>
       </c>
       <c r="AB16" t="str">
-        <f t="shared" si="3"/>
-        <v>expPDF</v>
+        <f>$B16&amp;"ParamTransform"</f>
+        <v>negBinomXParamTransform</v>
       </c>
       <c r="AC16" t="str">
+        <f>$B16&amp;"PDF"</f>
+        <v>negBinomXPDF</v>
+      </c>
+      <c r="AD16" t="str">
         <f>B16&amp;"PlotDistr"</f>
-        <v>expPlotDistr</v>
-      </c>
-      <c r="AD16" t="str">
+        <v>negBinomXPlotDistr</v>
+      </c>
+      <c r="AE16" t="str">
         <f>B16&amp;"Draws"</f>
-        <v>expDraws</v>
-      </c>
-      <c r="AE16" t="str">
+        <v>negBinomXDraws</v>
+      </c>
+      <c r="AF16" t="str">
         <f>B16&amp;"Latex"</f>
-        <v>expLatex</v>
-      </c>
-      <c r="AF16" t="str">
-        <f t="shared" si="4"/>
-        <v>expChartDomain</v>
+        <v>negBinomXLatex</v>
       </c>
       <c r="AG16" t="str">
-        <f t="shared" si="5"/>
-        <v>expLikelihoodFun</v>
+        <f>$B16&amp;"ChartDomain"</f>
+        <v>negBinomXChartDomain</v>
+      </c>
+      <c r="AH16" t="str">
+        <f>$B16&amp;"LikelihoodFun"</f>
+        <v>negBinomXLikelihoodFun</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -2684,7 +2753,7 @@
         <v>24</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>89</v>
@@ -2696,10 +2765,10 @@
         <v>48</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>38</v>
@@ -2717,10 +2786,10 @@
         <v>78</v>
       </c>
       <c r="S17" s="1">
-        <v>-2</v>
+        <v>0.25</v>
       </c>
       <c r="T17" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>64</v>
@@ -2728,78 +2797,81 @@
       <c r="V17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X17">
         <v>0.01</v>
       </c>
-      <c r="X17" t="str">
+      <c r="Y17" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Y17" t="str">
+        <v>"&amp;lambda;"</v>
+      </c>
+      <c r="Z17" t="str">
         <f>IF(F17=1,"""none""",IF(E17=F17,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
-      <c r="Z17" t="str">
+      <c r="AA17" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AA17" t="str">
+        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB17" t="str">
         <f t="shared" si="2"/>
-        <v>expExpParamTransform</v>
-      </c>
-      <c r="AB17" t="str">
+        <v>expParamTransform</v>
+      </c>
+      <c r="AC17" t="str">
         <f t="shared" si="3"/>
-        <v>expExpPDF</v>
-      </c>
-      <c r="AC17" t="str">
+        <v>expPDF</v>
+      </c>
+      <c r="AD17" t="str">
         <f>B17&amp;"PlotDistr"</f>
-        <v>expExpPlotDistr</v>
-      </c>
-      <c r="AD17" t="str">
+        <v>expPlotDistr</v>
+      </c>
+      <c r="AE17" t="str">
         <f>B17&amp;"Draws"</f>
-        <v>expExpDraws</v>
-      </c>
-      <c r="AE17" t="str">
+        <v>expDraws</v>
+      </c>
+      <c r="AF17" t="str">
         <f>B17&amp;"Latex"</f>
-        <v>expExpLatex</v>
-      </c>
-      <c r="AF17" t="str">
+        <v>expLatex</v>
+      </c>
+      <c r="AG17" t="str">
         <f t="shared" si="4"/>
-        <v>expExpChartDomain</v>
-      </c>
-      <c r="AG17" t="str">
+        <v>expChartDomain</v>
+      </c>
+      <c r="AH17" t="str">
         <f t="shared" si="5"/>
-        <v>expExpLikelihoodFun</v>
+        <v>expLikelihoodFun</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>146</v>
@@ -2829,74 +2901,77 @@
         <v>78</v>
       </c>
       <c r="S18" s="1">
-        <v>-0.5</v>
+        <v>-2</v>
       </c>
       <c r="T18" s="1">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="V18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W18">
+      <c r="W18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X18">
         <v>0.01</v>
       </c>
-      <c r="X18" t="str">
+      <c r="Y18" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y18" t="str">
+      <c r="Z18" t="str">
         <f>IF(F18=1,"""none""",IF(E18=F18,"""betas""","""fullNorm"""))</f>
-        <v>"betas"</v>
-      </c>
-      <c r="Z18" t="str">
+        <v>"none"</v>
+      </c>
+      <c r="AA18" t="str">
         <f t="shared" si="1"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AA18" t="str">
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB18" t="str">
         <f t="shared" si="2"/>
-        <v>expExpXParamTransform</v>
-      </c>
-      <c r="AB18" t="str">
+        <v>expExpParamTransform</v>
+      </c>
+      <c r="AC18" t="str">
         <f t="shared" si="3"/>
-        <v>expExpXPDF</v>
-      </c>
-      <c r="AC18" t="str">
+        <v>expExpPDF</v>
+      </c>
+      <c r="AD18" t="str">
         <f>B18&amp;"PlotDistr"</f>
-        <v>expExpXPlotDistr</v>
-      </c>
-      <c r="AD18" t="str">
+        <v>expExpPlotDistr</v>
+      </c>
+      <c r="AE18" t="str">
         <f>B18&amp;"Draws"</f>
-        <v>expExpXDraws</v>
-      </c>
-      <c r="AE18" t="str">
+        <v>expExpDraws</v>
+      </c>
+      <c r="AF18" t="str">
         <f>B18&amp;"Latex"</f>
-        <v>expExpXLatex</v>
-      </c>
-      <c r="AF18" t="str">
+        <v>expExpLatex</v>
+      </c>
+      <c r="AG18" t="str">
         <f t="shared" si="4"/>
-        <v>expExpXChartDomain</v>
-      </c>
-      <c r="AG18" t="str">
+        <v>expExpChartDomain</v>
+      </c>
+      <c r="AH18" t="str">
         <f t="shared" si="5"/>
-        <v>expExpXLikelihoodFun</v>
+        <v>expExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>124</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>87</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -2908,7 +2983,7 @@
         <v>24</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>90</v>
@@ -2938,7 +3013,7 @@
         <v>80</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="S19" s="1">
         <v>-0.5</v>
@@ -2952,60 +3027,63 @@
       <c r="V19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W19">
+      <c r="W19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X19">
         <v>0.01</v>
       </c>
-      <c r="X19" t="str">
+      <c r="Y19" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y19" t="str">
+      <c r="Z19" t="str">
         <f>IF(F19=1,"""none""",IF(E19=F19,"""betas""","""fullNorm"""))</f>
         <v>"betas"</v>
       </c>
-      <c r="Z19" t="str">
+      <c r="AA19" t="str">
         <f t="shared" si="1"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AA19" t="str">
+      <c r="AB19" t="str">
         <f t="shared" si="2"/>
-        <v>neumayerParamTransform</v>
-      </c>
-      <c r="AB19" t="str">
+        <v>expExpXParamTransform</v>
+      </c>
+      <c r="AC19" t="str">
         <f t="shared" si="3"/>
-        <v>neumayerPDF</v>
-      </c>
-      <c r="AC19" t="str">
-        <f t="shared" ref="AC19" si="14">B19&amp;"PlotDistr"</f>
-        <v>neumayerPlotDistr</v>
+        <v>expExpXPDF</v>
       </c>
       <c r="AD19" t="str">
-        <f t="shared" ref="AD19" si="15">B19&amp;"Draws"</f>
-        <v>neumayerDraws</v>
+        <f>B19&amp;"PlotDistr"</f>
+        <v>expExpXPlotDistr</v>
       </c>
       <c r="AE19" t="str">
-        <f t="shared" ref="AE19" si="16">B19&amp;"Latex"</f>
-        <v>neumayerLatex</v>
+        <f>B19&amp;"Draws"</f>
+        <v>expExpXDraws</v>
       </c>
       <c r="AF19" t="str">
+        <f>B19&amp;"Latex"</f>
+        <v>expExpXLatex</v>
+      </c>
+      <c r="AG19" t="str">
         <f t="shared" si="4"/>
-        <v>neumayerChartDomain</v>
-      </c>
-      <c r="AG19" t="str">
+        <v>expExpXChartDomain</v>
+      </c>
+      <c r="AH19" t="str">
         <f t="shared" si="5"/>
-        <v>neumayerLikelihoodFun</v>
+        <v>expExpXLikelihoodFun</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>87</v>
@@ -3020,7 +3098,7 @@
         <v>24</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>90</v>
@@ -3064,46 +3142,164 @@
       <c r="V20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W20">
+      <c r="W20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X20">
         <v>0.01</v>
       </c>
-      <c r="X20" t="str">
+      <c r="Y20" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Y20" t="str">
+      <c r="Z20" t="str">
         <f>IF(F20=1,"""none""",IF(E20=F20,"""betas""","""fullNorm"""))</f>
         <v>"betas"</v>
       </c>
-      <c r="Z20" t="str">
+      <c r="AA20" t="str">
         <f t="shared" si="1"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AA20" t="str">
+      <c r="AB20" t="str">
+        <f t="shared" si="2"/>
+        <v>neumayerParamTransform</v>
+      </c>
+      <c r="AC20" t="str">
+        <f t="shared" si="3"/>
+        <v>neumayerPDF</v>
+      </c>
+      <c r="AD20" t="str">
+        <f t="shared" ref="AD20" si="19">B20&amp;"PlotDistr"</f>
+        <v>neumayerPlotDistr</v>
+      </c>
+      <c r="AE20" t="str">
+        <f t="shared" ref="AE20" si="20">B20&amp;"Draws"</f>
+        <v>neumayerDraws</v>
+      </c>
+      <c r="AF20" t="str">
+        <f t="shared" ref="AF20" si="21">B20&amp;"Latex"</f>
+        <v>neumayerLatex</v>
+      </c>
+      <c r="AG20" t="str">
+        <f t="shared" si="4"/>
+        <v>neumayerChartDomain</v>
+      </c>
+      <c r="AH20" t="str">
+        <f t="shared" si="5"/>
+        <v>neumayerLikelihoodFun</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S21" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X21">
+        <v>0.01</v>
+      </c>
+      <c r="Y21" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z21" t="str">
+        <f>IF(F21=1,"""none""",IF(E21=F21,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
+      </c>
+      <c r="AA21" t="str">
+        <f t="shared" si="1"/>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AB21" t="str">
         <f t="shared" si="2"/>
         <v>drehJenParamTransform</v>
       </c>
-      <c r="AB20" t="str">
+      <c r="AC21" t="str">
         <f t="shared" si="3"/>
         <v>drehJenPDF</v>
       </c>
-      <c r="AC20" t="str">
-        <f>B20&amp;"PlotDistr"</f>
+      <c r="AD21" t="str">
+        <f>B21&amp;"PlotDistr"</f>
         <v>drehJenPlotDistr</v>
       </c>
-      <c r="AD20" t="str">
-        <f>B20&amp;"Draws"</f>
+      <c r="AE21" t="str">
+        <f>B21&amp;"Draws"</f>
         <v>drehJenDraws</v>
       </c>
-      <c r="AE20" t="str">
-        <f>B20&amp;"Latex"</f>
+      <c r="AF21" t="str">
+        <f>B21&amp;"Latex"</f>
         <v>drehJenLatex</v>
       </c>
-      <c r="AF20" t="str">
+      <c r="AG21" t="str">
         <f t="shared" si="4"/>
         <v>drehJenChartDomain</v>
       </c>
-      <c r="AG20" t="str">
+      <c r="AH21" t="str">
         <f t="shared" si="5"/>
         <v>drehJenLikelihoodFun</v>
       </c>

</xml_diff>

<commit_message>
refactor of prob page
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A49DDF-365E-495D-9B07-8F9BB5623EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD14187-7043-4E93-84D3-CDF28ECA2E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>expExp</t>
   </si>
   <si>
-    <t>distrGroups</t>
-  </si>
-  <si>
     <t>distrList</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>dataprintList</t>
   </si>
   <si>
-    <t>randomDrawList</t>
-  </si>
-  <si>
     <t>latexList</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>styNormX</t>
   </si>
   <si>
-    <t>transformFunList</t>
-  </si>
-  <si>
     <t>paramTex</t>
   </si>
   <si>
@@ -153,9 +144,6 @@
     <t>\lambda</t>
   </si>
   <si>
-    <t>metaParamTex</t>
-  </si>
-  <si>
     <t>\mu</t>
   </si>
   <si>
@@ -502,6 +490,18 @@
   </si>
   <si>
     <t>styLogPDF</t>
+  </si>
+  <si>
+    <t>distrGroup</t>
+  </si>
+  <si>
+    <t>transformFun</t>
+  </si>
+  <si>
+    <t>intrParamTex</t>
+  </si>
+  <si>
+    <t>drawFun</t>
   </si>
 </sst>
 </file>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,100 +909,100 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>154</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" t="s">
+        <v>149</v>
+      </c>
+      <c r="X1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>71</v>
-      </c>
-      <c r="R1" t="s">
-        <v>131</v>
-      </c>
-      <c r="S1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" t="s">
-        <v>56</v>
-      </c>
-      <c r="U1" t="s">
-        <v>57</v>
-      </c>
-      <c r="V1" t="s">
-        <v>92</v>
-      </c>
-      <c r="W1" t="s">
-        <v>153</v>
-      </c>
-      <c r="X1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>22</v>
-      </c>
       <c r="AG1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AH1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -1025,40 +1025,40 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="S2" s="1">
         <v>0</v>
@@ -1067,13 +1067,13 @@
         <v>1</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X2">
         <v>0.01</v>
@@ -1083,11 +1083,11 @@
         <v>"&amp;pi;"</v>
       </c>
       <c r="Z2" t="str">
-        <f>IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
+        <f t="shared" ref="Z2:Z21" si="1">IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
       <c r="AA2" t="str">
-        <f t="shared" ref="AA2:AA21" si="1">"manyParamSliderMaker(minVal ="&amp;S2&amp;", maxVal = "&amp;T2&amp;", startVals = "&amp;U2&amp;", stepVal = "&amp;X2&amp;", paramHTML = "&amp;Y2&amp;", multi = "&amp;Z2&amp;", sigmaScale ="&amp;V2&amp;","</f>
+        <f t="shared" ref="AA2:AA21" si="2">"manyParamSliderMaker(minVal ="&amp;S2&amp;", maxVal = "&amp;T2&amp;", startVals = "&amp;U2&amp;", stepVal = "&amp;X2&amp;", paramHTML = "&amp;Y2&amp;", multi = "&amp;Z2&amp;", sigmaScale ="&amp;V2&amp;","</f>
         <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB2" t="str">
@@ -1128,7 +1128,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -1140,40 +1140,40 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="S3" s="1">
         <v>-2</v>
@@ -1182,13 +1182,13 @@
         <v>2</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X3">
         <v>0.01</v>
@@ -1198,19 +1198,19 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z3" t="str">
-        <f>IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
       <c r="AA3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB21" si="2">$B3&amp;"ParamTransform"</f>
+        <f t="shared" ref="AB3:AB21" si="3">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
       <c r="AC3" t="str">
-        <f t="shared" ref="AC3:AC21" si="3">$B3&amp;"PDF"</f>
+        <f t="shared" ref="AC3:AC21" si="4">$B3&amp;"PDF"</f>
         <v>bernLogitPDF</v>
       </c>
       <c r="AD3" t="str">
@@ -1226,24 +1226,24 @@
         <v>bernLogitLatex</v>
       </c>
       <c r="AG3" t="str">
-        <f t="shared" ref="AG3:AG21" si="4">$B3&amp;"ChartDomain"</f>
+        <f t="shared" ref="AG3:AG21" si="5">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
       <c r="AH3" t="str">
-        <f t="shared" ref="AH3:AH21" si="5">$B3&amp;"LikelihoodFun"</f>
+        <f t="shared" ref="AH3:AH21" si="6">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A21" si="6">A3+1</f>
+        <f t="shared" ref="A4:A21" si="7">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -1255,40 +1255,40 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="S4" s="1">
         <v>-4</v>
@@ -1297,13 +1297,13 @@
         <v>4</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X4">
         <v>0.01</v>
@@ -1313,19 +1313,19 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z4" t="str">
-        <f>IF(F4=1,"""none""",IF(E4=F4,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
       <c r="AA4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="AB4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>bernLogitXParamTransform</v>
       </c>
       <c r="AC4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>bernLogitXPDF</v>
       </c>
       <c r="AD4" t="str">
@@ -1341,24 +1341,24 @@
         <v>bernLogitXLatex</v>
       </c>
       <c r="AG4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>bernLogitXChartDomain</v>
       </c>
       <c r="AH4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -1370,40 +1370,40 @@
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="S5" s="1">
         <v>-2</v>
@@ -1412,35 +1412,35 @@
         <v>2</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X5">
         <v>0.01</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" ref="Y5" si="7">"""&amp;"&amp;RIGHT(M5,LEN(M5)-1)&amp;";"""</f>
+        <f t="shared" ref="Y5" si="8">"""&amp;"&amp;RIGHT(M5,LEN(M5)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z5" t="str">
-        <f>IF(F5=1,"""none""",IF(E5=F5,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
       <c r="AA5" t="str">
-        <f t="shared" ref="AA5" si="8">"manyParamSliderMaker(minVal ="&amp;S5&amp;", maxVal = "&amp;T5&amp;", startVals = "&amp;U5&amp;", stepVal = "&amp;X5&amp;", paramHTML = "&amp;Y5&amp;", multi = "&amp;Z5&amp;", sigmaScale ="&amp;V5&amp;","</f>
+        <f t="shared" ref="AA5" si="9">"manyParamSliderMaker(minVal ="&amp;S5&amp;", maxVal = "&amp;T5&amp;", startVals = "&amp;U5&amp;", stepVal = "&amp;X5&amp;", paramHTML = "&amp;Y5&amp;", multi = "&amp;Z5&amp;", sigmaScale ="&amp;V5&amp;","</f>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="AB5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>bernProbitXParamTransform</v>
       </c>
       <c r="AC5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>bernProbitXPDF</v>
       </c>
       <c r="AD5" t="str">
@@ -1456,27 +1456,27 @@
         <v>bernProbitXLatex</v>
       </c>
       <c r="AG5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>bernProbitXChartDomain</v>
       </c>
       <c r="AH5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>bernProbitXLikelihoodFun</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
@@ -1485,40 +1485,40 @@
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="S6" s="1">
         <v>-3</v>
@@ -1527,71 +1527,71 @@
         <v>3</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="X6">
         <v>0.01</v>
       </c>
       <c r="Y6" t="str">
-        <f t="shared" ref="Y6" si="9">"""&amp;"&amp;RIGHT(M6,LEN(M6)-1)&amp;";"""</f>
+        <f t="shared" ref="Y6" si="10">"""&amp;"&amp;RIGHT(M6,LEN(M6)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z6" t="str">
-        <f>IF(F6=1,"""none""",IF(E6=F6,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
       <c r="AA6" t="str">
-        <f t="shared" ref="AA6" si="10">"manyParamSliderMaker(minVal ="&amp;S6&amp;", maxVal = "&amp;T6&amp;", startVals = "&amp;U6&amp;", stepVal = "&amp;X6&amp;", paramHTML = "&amp;Y6&amp;", multi = "&amp;Z6&amp;", sigmaScale ="&amp;V6&amp;","</f>
+        <f t="shared" ref="AA6" si="11">"manyParamSliderMaker(minVal ="&amp;S6&amp;", maxVal = "&amp;T6&amp;", startVals = "&amp;U6&amp;", stepVal = "&amp;X6&amp;", paramHTML = "&amp;Y6&amp;", multi = "&amp;Z6&amp;", sigmaScale ="&amp;V6&amp;","</f>
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
       </c>
       <c r="AB6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>orderedProbitXParamTransform</v>
       </c>
       <c r="AC6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>orderedProbitXPDF</v>
       </c>
       <c r="AD6" t="str">
-        <f t="shared" ref="AD6" si="11">B6&amp;"PlotDistr"</f>
+        <f t="shared" ref="AD6" si="12">B6&amp;"PlotDistr"</f>
         <v>orderedProbitXPlotDistr</v>
       </c>
       <c r="AE6" t="str">
-        <f t="shared" ref="AE6" si="12">B6&amp;"Draws"</f>
+        <f t="shared" ref="AE6" si="13">B6&amp;"Draws"</f>
         <v>orderedProbitXDraws</v>
       </c>
       <c r="AF6" t="str">
-        <f t="shared" ref="AF6" si="13">B6&amp;"Latex"</f>
+        <f t="shared" ref="AF6" si="14">B6&amp;"Latex"</f>
         <v>orderedProbitXLatex</v>
       </c>
       <c r="AG6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>orderedProbitXChartDomain</v>
       </c>
       <c r="AH6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>orderedProbitXLikelihoodFun</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E7" s="1">
         <v>3</v>
@@ -1600,40 +1600,40 @@
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="S7" s="1">
         <v>-3</v>
@@ -1642,68 +1642,68 @@
         <v>3</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="X7">
         <v>0.01</v>
       </c>
       <c r="Y7" t="str">
-        <f t="shared" ref="Y7" si="14">"""&amp;"&amp;RIGHT(M7,LEN(M7)-1)&amp;";"""</f>
+        <f t="shared" ref="Y7" si="15">"""&amp;"&amp;RIGHT(M7,LEN(M7)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z7" t="str">
-        <f>IF(F7=1,"""none""",IF(E7=F7,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
       <c r="AA7" t="str">
-        <f t="shared" ref="AA7" si="15">"manyParamSliderMaker(minVal ="&amp;S7&amp;", maxVal = "&amp;T7&amp;", startVals = "&amp;U7&amp;", stepVal = "&amp;X7&amp;", paramHTML = "&amp;Y7&amp;", multi = "&amp;Z7&amp;", sigmaScale ="&amp;V7&amp;","</f>
+        <f t="shared" ref="AA7" si="16">"manyParamSliderMaker(minVal ="&amp;S7&amp;", maxVal = "&amp;T7&amp;", startVals = "&amp;U7&amp;", stepVal = "&amp;X7&amp;", paramHTML = "&amp;Y7&amp;", multi = "&amp;Z7&amp;", sigmaScale ="&amp;V7&amp;","</f>
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
       </c>
       <c r="AB7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>orderedLogitXParamTransform</v>
       </c>
       <c r="AC7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>orderedLogitXPDF</v>
       </c>
       <c r="AD7" t="str">
-        <f t="shared" ref="AD7" si="16">B7&amp;"PlotDistr"</f>
+        <f t="shared" ref="AD7" si="17">B7&amp;"PlotDistr"</f>
         <v>orderedLogitXPlotDistr</v>
       </c>
       <c r="AE7" t="str">
-        <f t="shared" ref="AE7" si="17">B7&amp;"Draws"</f>
+        <f t="shared" ref="AE7" si="18">B7&amp;"Draws"</f>
         <v>orderedLogitXDraws</v>
       </c>
       <c r="AF7" t="str">
-        <f t="shared" ref="AF7" si="18">B7&amp;"Latex"</f>
+        <f t="shared" ref="AF7" si="19">B7&amp;"Latex"</f>
         <v>orderedLogitXLatex</v>
       </c>
       <c r="AG7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>orderedLogitXChartDomain</v>
       </c>
       <c r="AH7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>orderedLogitXLikelihoodFun</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
@@ -1715,40 +1715,40 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="S8" s="1">
         <v>-4</v>
@@ -1757,13 +1757,13 @@
         <v>4</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X8">
         <v>0.01</v>
@@ -1773,52 +1773,52 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z8" t="str">
-        <f>IF(F8=1,"""none""",IF(E8=F8,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
       <c r="AA8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>styNormParamTransform</v>
       </c>
       <c r="AC8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>styNormPDF</v>
       </c>
       <c r="AD8" t="str">
-        <f>B8&amp;"PlotDistr"</f>
+        <f t="shared" ref="AD8:AD19" si="20">B8&amp;"PlotDistr"</f>
         <v>styNormPlotDistr</v>
       </c>
       <c r="AE8" t="str">
-        <f>B8&amp;"Draws"</f>
+        <f t="shared" ref="AE8:AE19" si="21">B8&amp;"Draws"</f>
         <v>styNormDraws</v>
       </c>
       <c r="AF8" t="str">
-        <f>B8&amp;"Latex"</f>
+        <f t="shared" ref="AF8:AF19" si="22">B8&amp;"Latex"</f>
         <v>styNormLatex</v>
       </c>
       <c r="AG8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>styNormChartDomain</v>
       </c>
       <c r="AH8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>styNormLikelihoodFun</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
@@ -1830,40 +1830,40 @@
         <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="S9" s="1">
         <v>-3</v>
@@ -1872,13 +1872,13 @@
         <v>3</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X9">
         <v>0.01</v>
@@ -1888,52 +1888,52 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z9" t="str">
-        <f>IF(F9=1,"""none""",IF(E9=F9,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
       <c r="AA9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="AB9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>styNormXParamTransform</v>
       </c>
       <c r="AC9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>styNormXPDF</v>
       </c>
       <c r="AD9" t="str">
-        <f>B9&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>styNormXPlotDistr</v>
       </c>
       <c r="AE9" t="str">
-        <f>B9&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>styNormXDraws</v>
       </c>
       <c r="AF9" t="str">
-        <f>B9&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>styNormXLatex</v>
       </c>
       <c r="AG9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>styNormXChartDomain</v>
       </c>
       <c r="AH9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>styNormXLikelihoodFun</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
@@ -1945,40 +1945,40 @@
         <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S10" s="1">
         <v>-3</v>
@@ -1987,13 +1987,13 @@
         <v>3</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X10">
         <v>0.01</v>
@@ -2003,55 +2003,55 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z10" t="str">
-        <f>IF(F10=1,"""none""",IF(E10=F10,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
       <c r="AA10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>fullNormXParamTransform</v>
       </c>
       <c r="AC10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>fullNormXPDF</v>
       </c>
       <c r="AD10" t="str">
-        <f>B10&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>fullNormXPlotDistr</v>
       </c>
       <c r="AE10" t="str">
-        <f>B10&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>fullNormXDraws</v>
       </c>
       <c r="AF10" t="str">
-        <f>B10&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>fullNormXLatex</v>
       </c>
       <c r="AG10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>fullNormXChartDomain</v>
       </c>
       <c r="AH10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>fullNormXLikelihoodFun</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -2060,40 +2060,40 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="S11" s="1">
         <v>-0.5</v>
@@ -2102,13 +2102,13 @@
         <v>0.5</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X11">
         <v>0.01</v>
@@ -2118,55 +2118,55 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z11" t="str">
-        <f>IF(F11=1,"""none""",IF(E11=F11,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
       <c r="AA11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>logNormParamTransform</v>
       </c>
       <c r="AC11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>logNormPDF</v>
       </c>
       <c r="AD11" t="str">
-        <f>B11&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>logNormPlotDistr</v>
       </c>
       <c r="AE11" t="str">
-        <f>B11&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>logNormDraws</v>
       </c>
       <c r="AF11" t="str">
-        <f>B11&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>logNormLatex</v>
       </c>
       <c r="AG11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>logNormChartDomain</v>
       </c>
       <c r="AH11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>logNormLikelihoodFun</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -2175,40 +2175,40 @@
         <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="S12" s="1">
         <v>-0.5</v>
@@ -2217,13 +2217,13 @@
         <v>0.5</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X12">
         <v>0.01</v>
@@ -2233,45 +2233,45 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z12" t="str">
-        <f>IF(F12=1,"""none""",IF(E12=F12,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
       <c r="AA12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="AB12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>logNormXParamTransform</v>
       </c>
       <c r="AC12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>logNormXPDF</v>
       </c>
       <c r="AD12" t="str">
-        <f>B12&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>logNormXPlotDistr</v>
       </c>
       <c r="AE12" t="str">
-        <f>B12&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>logNormXDraws</v>
       </c>
       <c r="AF12" t="str">
-        <f>B12&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>logNormXLatex</v>
       </c>
       <c r="AG12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>logNormXChartDomain</v>
       </c>
       <c r="AH12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>logNormXLikelihoodFun</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2290,40 +2290,40 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S13" s="1">
         <v>1</v>
@@ -2332,13 +2332,13 @@
         <v>10</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X13">
         <v>0.01</v>
@@ -2348,52 +2348,52 @@
         <v>"&amp;lambda;"</v>
       </c>
       <c r="Z13" t="str">
-        <f>IF(F13=1,"""none""",IF(E13=F13,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
       <c r="AA13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>poisParamTransform</v>
       </c>
       <c r="AC13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>poisPDF</v>
       </c>
       <c r="AD13" t="str">
-        <f>B13&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>poisPlotDistr</v>
       </c>
       <c r="AE13" t="str">
-        <f>B13&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>poisDraws</v>
       </c>
       <c r="AF13" t="str">
-        <f>B13&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>poisLatex</v>
       </c>
       <c r="AG13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>poisChartDomain</v>
       </c>
       <c r="AH13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>poisLikelihoodFun</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>0</v>
@@ -2405,40 +2405,40 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S14" s="1">
         <v>-0.25</v>
@@ -2447,13 +2447,13 @@
         <v>3</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X14">
         <v>0.01</v>
@@ -2463,52 +2463,52 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z14" t="str">
-        <f>IF(F14=1,"""none""",IF(E14=F14,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
       <c r="AA14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>poisExpParamTransform</v>
       </c>
       <c r="AC14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>poisExpPDF</v>
       </c>
       <c r="AD14" t="str">
-        <f>B14&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>poisExpPlotDistr</v>
       </c>
       <c r="AE14" t="str">
-        <f>B14&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>poisExpDraws</v>
       </c>
       <c r="AF14" t="str">
-        <f>B14&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>poisExpLatex</v>
       </c>
       <c r="AG14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>poisExpChartDomain</v>
       </c>
       <c r="AH14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>poisExpLikelihoodFun</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>0</v>
@@ -2520,40 +2520,40 @@
         <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S15" s="1">
         <v>-0.25</v>
@@ -2562,13 +2562,13 @@
         <v>3</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X15">
         <v>0.01</v>
@@ -2578,52 +2578,52 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z15" t="str">
-        <f>IF(F15=1,"""none""",IF(E15=F15,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
       <c r="AA15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="AB15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>poisExpXParamTransform</v>
       </c>
       <c r="AC15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>poisExpXPDF</v>
       </c>
       <c r="AD15" t="str">
-        <f>B15&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>poisExpXPlotDistr</v>
       </c>
       <c r="AE15" t="str">
-        <f>B15&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>poisExpXDraws</v>
       </c>
       <c r="AF15" t="str">
-        <f>B15&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>poisExpXLatex</v>
       </c>
       <c r="AG15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>poisExpXChartDomain</v>
       </c>
       <c r="AH15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>0</v>
@@ -2635,40 +2635,40 @@
         <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S16" s="1">
         <v>-0.25</v>
@@ -2677,13 +2677,13 @@
         <v>1.5</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X16">
         <v>0.01</v>
@@ -2693,11 +2693,11 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z16" t="str">
-        <f>IF(F16=1,"""none""",IF(E16=F16,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
       <c r="AA16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 1.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1,2),</v>
       </c>
       <c r="AB16" t="str">
@@ -2709,15 +2709,15 @@
         <v>negBinomXPDF</v>
       </c>
       <c r="AD16" t="str">
-        <f>B16&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>negBinomXPlotDistr</v>
       </c>
       <c r="AE16" t="str">
-        <f>B16&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>negBinomXDraws</v>
       </c>
       <c r="AF16" t="str">
-        <f>B16&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>negBinomXLatex</v>
       </c>
       <c r="AG16" t="str">
@@ -2731,7 +2731,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2750,40 +2750,40 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S17" s="1">
         <v>0.25</v>
@@ -2792,13 +2792,13 @@
         <v>1.5</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X17">
         <v>0.01</v>
@@ -2808,52 +2808,52 @@
         <v>"&amp;lambda;"</v>
       </c>
       <c r="Z17" t="str">
-        <f>IF(F17=1,"""none""",IF(E17=F17,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
       <c r="AA17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>expParamTransform</v>
       </c>
       <c r="AC17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>expPDF</v>
       </c>
       <c r="AD17" t="str">
-        <f>B17&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>expPlotDistr</v>
       </c>
       <c r="AE17" t="str">
-        <f>B17&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>expDraws</v>
       </c>
       <c r="AF17" t="str">
-        <f>B17&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>expLatex</v>
       </c>
       <c r="AG17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>expChartDomain</v>
       </c>
       <c r="AH17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>expLikelihoodFun</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -2865,40 +2865,40 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S18" s="1">
         <v>-2</v>
@@ -2907,13 +2907,13 @@
         <v>2</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X18">
         <v>0.01</v>
@@ -2923,52 +2923,52 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z18" t="str">
-        <f>IF(F18=1,"""none""",IF(E18=F18,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
       <c r="AA18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>expExpParamTransform</v>
       </c>
       <c r="AC18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>expExpPDF</v>
       </c>
       <c r="AD18" t="str">
-        <f>B18&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>expExpPlotDistr</v>
       </c>
       <c r="AE18" t="str">
-        <f>B18&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>expExpDraws</v>
       </c>
       <c r="AF18" t="str">
-        <f>B18&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>expExpLatex</v>
       </c>
       <c r="AG18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>expExpChartDomain</v>
       </c>
       <c r="AH18" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>expExpLikelihoodFun</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -2980,40 +2980,40 @@
         <v>3</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S19" s="1">
         <v>-0.5</v>
@@ -3022,13 +3022,13 @@
         <v>0.5</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X19">
         <v>0.01</v>
@@ -3038,55 +3038,55 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z19" t="str">
-        <f>IF(F19=1,"""none""",IF(E19=F19,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
       <c r="AA19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="AB19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>expExpXParamTransform</v>
       </c>
       <c r="AC19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>expExpXPDF</v>
       </c>
       <c r="AD19" t="str">
-        <f>B19&amp;"PlotDistr"</f>
+        <f t="shared" si="20"/>
         <v>expExpXPlotDistr</v>
       </c>
       <c r="AE19" t="str">
-        <f>B19&amp;"Draws"</f>
+        <f t="shared" si="21"/>
         <v>expExpXDraws</v>
       </c>
       <c r="AF19" t="str">
-        <f>B19&amp;"Latex"</f>
+        <f t="shared" si="22"/>
         <v>expExpXLatex</v>
       </c>
       <c r="AG19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>expExpXChartDomain</v>
       </c>
       <c r="AH19" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>expExpXLikelihoodFun</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E20" s="1">
         <v>3</v>
@@ -3095,40 +3095,40 @@
         <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="S20" s="1">
         <v>-0.5</v>
@@ -3137,13 +3137,13 @@
         <v>0.5</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X20">
         <v>0.01</v>
@@ -3153,55 +3153,55 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z20" t="str">
-        <f>IF(F20=1,"""none""",IF(E20=F20,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
       <c r="AA20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="AB20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>neumayerParamTransform</v>
       </c>
       <c r="AC20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>neumayerPDF</v>
       </c>
       <c r="AD20" t="str">
-        <f t="shared" ref="AD20" si="19">B20&amp;"PlotDistr"</f>
+        <f t="shared" ref="AD20" si="23">B20&amp;"PlotDistr"</f>
         <v>neumayerPlotDistr</v>
       </c>
       <c r="AE20" t="str">
-        <f t="shared" ref="AE20" si="20">B20&amp;"Draws"</f>
+        <f t="shared" ref="AE20" si="24">B20&amp;"Draws"</f>
         <v>neumayerDraws</v>
       </c>
       <c r="AF20" t="str">
-        <f t="shared" ref="AF20" si="21">B20&amp;"Latex"</f>
+        <f t="shared" ref="AF20" si="25">B20&amp;"Latex"</f>
         <v>neumayerLatex</v>
       </c>
       <c r="AG20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>neumayerChartDomain</v>
       </c>
       <c r="AH20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>neumayerLikelihoodFun</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -3210,40 +3210,40 @@
         <v>3</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="S21" s="1">
         <v>-0.5</v>
@@ -3252,13 +3252,13 @@
         <v>0.5</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X21">
         <v>0.01</v>
@@ -3268,19 +3268,19 @@
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z21" t="str">
-        <f>IF(F21=1,"""none""",IF(E21=F21,"""betas""","""fullNorm"""))</f>
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
       <c r="AA21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
       <c r="AB21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>drehJenParamTransform</v>
       </c>
       <c r="AC21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>drehJenPDF</v>
       </c>
       <c r="AD21" t="str">
@@ -3296,11 +3296,11 @@
         <v>drehJenLatex</v>
       </c>
       <c r="AG21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>drehJenChartDomain</v>
       </c>
       <c r="AH21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>drehJenLikelihoodFun</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MLE page of overhaul
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD14187-7043-4E93-84D3-CDF28ECA2E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71DC4F1-1751-40DE-B14D-E8026A9C61FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="152">
   <si>
     <t>Poisson</t>
   </si>
@@ -90,9 +90,6 @@
     <t>marginalsChoicesList</t>
   </si>
   <si>
-    <t>distrPlotList</t>
-  </si>
-  <si>
     <t>dataprintList</t>
   </si>
   <si>
@@ -111,18 +108,6 @@
     <t>likelihoodFun</t>
   </si>
   <si>
-    <t>paramName</t>
-  </si>
-  <si>
-    <t>Beta</t>
-  </si>
-  <si>
-    <t>Pi</t>
-  </si>
-  <si>
-    <t>Lambda</t>
-  </si>
-  <si>
     <t>poisExpX</t>
   </si>
   <si>
@@ -279,15 +264,6 @@
     <t>c(-8,8)</t>
   </si>
   <si>
-    <t>drehJen</t>
-  </si>
-  <si>
-    <t>Dreher &amp; Jensen</t>
-  </si>
-  <si>
-    <t>Real</t>
-  </si>
-  <si>
     <t>negBinomX</t>
   </si>
   <si>
@@ -306,9 +282,6 @@
     <t>c(-2,2)</t>
   </si>
   <si>
-    <t>Beta/Gamma</t>
-  </si>
-  <si>
     <t>c("Beta0", "Beta1", "Beta2","Gamma")</t>
   </si>
   <si>
@@ -396,18 +369,9 @@
     <t>list("Exponential (Exp, X)","Exponential (Exp)", "Exponential")</t>
   </si>
   <si>
-    <t>neumayer</t>
-  </si>
-  <si>
-    <t>Neumayer (2003)</t>
-  </si>
-  <si>
     <t>c(.25,.2,.25,0)</t>
   </si>
   <si>
-    <t>list("Stylized Normal","Log Normal","Stylized Normal (X)")</t>
-  </si>
-  <si>
     <t>c("Beta0", "Beta1", "Beta2", "Beta3","Gamma")</t>
   </si>
   <si>
@@ -420,9 +384,6 @@
     <t>funcFormRange</t>
   </si>
   <si>
-    <t>c(-10,10)</t>
-  </si>
-  <si>
     <t>c(-6,6)</t>
   </si>
   <si>
@@ -502,6 +463,33 @@
   </si>
   <si>
     <t>drawFun</t>
+  </si>
+  <si>
+    <t>distrPlot</t>
+  </si>
+  <si>
+    <t>paramList</t>
+  </si>
+  <si>
+    <t>c("\\pi")</t>
+  </si>
+  <si>
+    <t>c("\\lambda")</t>
+  </si>
+  <si>
+    <t>c("\\beta")</t>
+  </si>
+  <si>
+    <t>c("\\beta_0", "\\beta_1", "\\gamma")</t>
+  </si>
+  <si>
+    <t>c("\\beta_0", "\\beta_1", "\\beta_2")</t>
+  </si>
+  <si>
+    <t>c("\\beta_0", "\\beta_1", "\\beta_2", "\\gamma")</t>
+  </si>
+  <si>
+    <t>c("\\beta_0", "\\beta_1", "\\beta_2", "\\beta_3", "\\gamma")</t>
   </si>
 </sst>
 </file>
@@ -868,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,97 +900,97 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
         <v>17</v>
       </c>
       <c r="J1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
         <v>141</v>
       </c>
-      <c r="K1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
-        <v>154</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
       <c r="P1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" t="s">
+        <v>115</v>
+      </c>
+      <c r="S1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" t="s">
+        <v>80</v>
+      </c>
+      <c r="W1" t="s">
+        <v>136</v>
+      </c>
+      <c r="X1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC1" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R1" t="s">
-        <v>127</v>
-      </c>
-      <c r="S1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V1" t="s">
-        <v>88</v>
-      </c>
-      <c r="W1" t="s">
-        <v>149</v>
-      </c>
-      <c r="X1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>153</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>70</v>
-      </c>
       <c r="AD1" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="AE1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="AF1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AG1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH1" t="s">
         <v>23</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -1025,40 +1013,40 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="S2" s="1">
         <v>0</v>
@@ -1067,27 +1055,27 @@
         <v>1</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X2">
         <v>0.01</v>
       </c>
       <c r="Y2" t="str">
-        <f t="shared" ref="Y2:Y21" si="0">"""&amp;"&amp;RIGHT(M2,LEN(M2)-1)&amp;";"""</f>
+        <f>"""&amp;"&amp;RIGHT(M2,LEN(M2)-1)&amp;";"""</f>
         <v>"&amp;pi;"</v>
       </c>
       <c r="Z2" t="str">
-        <f t="shared" ref="Z2:Z21" si="1">IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
+        <f>IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
       <c r="AA2" t="str">
-        <f t="shared" ref="AA2:AA21" si="2">"manyParamSliderMaker(minVal ="&amp;S2&amp;", maxVal = "&amp;T2&amp;", startVals = "&amp;U2&amp;", stepVal = "&amp;X2&amp;", paramHTML = "&amp;Y2&amp;", multi = "&amp;Z2&amp;", sigmaScale ="&amp;V2&amp;","</f>
+        <f t="shared" ref="AA2:AA19" si="0">"manyParamSliderMaker(minVal ="&amp;S2&amp;", maxVal = "&amp;T2&amp;", startVals = "&amp;U2&amp;", stepVal = "&amp;X2&amp;", paramHTML = "&amp;Y2&amp;", multi = "&amp;Z2&amp;", sigmaScale ="&amp;V2&amp;","</f>
         <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB2" t="str">
@@ -1128,7 +1116,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -1140,40 +1128,40 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="S3" s="1">
         <v>-2</v>
@@ -1182,35 +1170,35 @@
         <v>2</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X3">
         <v>0.01</v>
       </c>
       <c r="Y3" t="str">
+        <f>"""&amp;"&amp;RIGHT(M3,LEN(M3)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z3" t="str">
+        <f>IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
+      <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z3" t="str">
-        <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="AA3" t="str">
-        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
       <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB21" si="3">$B3&amp;"ParamTransform"</f>
+        <f t="shared" ref="AB3:AB19" si="1">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
       <c r="AC3" t="str">
-        <f t="shared" ref="AC3:AC21" si="4">$B3&amp;"PDF"</f>
+        <f t="shared" ref="AC3:AC19" si="2">$B3&amp;"PDF"</f>
         <v>bernLogitPDF</v>
       </c>
       <c r="AD3" t="str">
@@ -1226,24 +1214,24 @@
         <v>bernLogitLatex</v>
       </c>
       <c r="AG3" t="str">
-        <f t="shared" ref="AG3:AG21" si="5">$B3&amp;"ChartDomain"</f>
+        <f t="shared" ref="AG3:AG19" si="3">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
       <c r="AH3" t="str">
-        <f t="shared" ref="AH3:AH21" si="6">$B3&amp;"LikelihoodFun"</f>
+        <f t="shared" ref="AH3:AH19" si="4">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A21" si="7">A3+1</f>
+        <f t="shared" ref="A4:A19" si="5">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -1255,40 +1243,40 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="S4" s="1">
         <v>-4</v>
@@ -1297,35 +1285,35 @@
         <v>4</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X4">
         <v>0.01</v>
       </c>
       <c r="Y4" t="str">
+        <f>"""&amp;"&amp;RIGHT(M4,LEN(M4)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z4" t="str">
+        <f>IF(F4=1,"""none""",IF(E4=F4,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
+      </c>
+      <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z4" t="str">
+        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="AA4" t="str">
+        <v>bernLogitXParamTransform</v>
+      </c>
+      <c r="AC4" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AB4" t="str">
-        <f t="shared" si="3"/>
-        <v>bernLogitXParamTransform</v>
-      </c>
-      <c r="AC4" t="str">
-        <f t="shared" si="4"/>
         <v>bernLogitXPDF</v>
       </c>
       <c r="AD4" t="str">
@@ -1341,24 +1329,24 @@
         <v>bernLogitXLatex</v>
       </c>
       <c r="AG4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>bernLogitXChartDomain</v>
       </c>
       <c r="AH4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -1370,40 +1358,40 @@
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="S5" s="1">
         <v>-2</v>
@@ -1412,35 +1400,35 @@
         <v>2</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X5">
         <v>0.01</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" ref="Y5" si="8">"""&amp;"&amp;RIGHT(M5,LEN(M5)-1)&amp;";"""</f>
+        <f>"""&amp;"&amp;RIGHT(M5,LEN(M5)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z5" t="str">
+        <f>IF(F5=1,"""none""",IF(E5=F5,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
+      </c>
+      <c r="AA5" t="str">
+        <f t="shared" ref="AA5" si="6">"manyParamSliderMaker(minVal ="&amp;S5&amp;", maxVal = "&amp;T5&amp;", startVals = "&amp;U5&amp;", stepVal = "&amp;X5&amp;", paramHTML = "&amp;Y5&amp;", multi = "&amp;Z5&amp;", sigmaScale ="&amp;V5&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="AA5" t="str">
-        <f t="shared" ref="AA5" si="9">"manyParamSliderMaker(minVal ="&amp;S5&amp;", maxVal = "&amp;T5&amp;", startVals = "&amp;U5&amp;", stepVal = "&amp;X5&amp;", paramHTML = "&amp;Y5&amp;", multi = "&amp;Z5&amp;", sigmaScale ="&amp;V5&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AB5" t="str">
-        <f t="shared" si="3"/>
         <v>bernProbitXParamTransform</v>
       </c>
       <c r="AC5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>bernProbitXPDF</v>
       </c>
       <c r="AD5" t="str">
@@ -1456,27 +1444,27 @@
         <v>bernProbitXLatex</v>
       </c>
       <c r="AG5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>bernProbitXChartDomain</v>
       </c>
       <c r="AH5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>bernProbitXLikelihoodFun</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
@@ -1485,40 +1473,40 @@
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="S6" s="1">
         <v>-3</v>
@@ -1527,71 +1515,71 @@
         <v>3</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="X6">
         <v>0.01</v>
       </c>
       <c r="Y6" t="str">
-        <f t="shared" ref="Y6" si="10">"""&amp;"&amp;RIGHT(M6,LEN(M6)-1)&amp;";"""</f>
+        <f>"""&amp;"&amp;RIGHT(M6,LEN(M6)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z6" t="str">
+        <f>IF(F6=1,"""none""",IF(E6=F6,"""betas""","""fullNorm"""))</f>
+        <v>"fullNorm"</v>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" ref="AA6" si="7">"manyParamSliderMaker(minVal ="&amp;S6&amp;", maxVal = "&amp;T6&amp;", startVals = "&amp;U6&amp;", stepVal = "&amp;X6&amp;", paramHTML = "&amp;Y6&amp;", multi = "&amp;Z6&amp;", sigmaScale ="&amp;V6&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+      </c>
+      <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="AA6" t="str">
-        <f t="shared" ref="AA6" si="11">"manyParamSliderMaker(minVal ="&amp;S6&amp;", maxVal = "&amp;T6&amp;", startVals = "&amp;U6&amp;", stepVal = "&amp;X6&amp;", paramHTML = "&amp;Y6&amp;", multi = "&amp;Z6&amp;", sigmaScale ="&amp;V6&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
-      </c>
-      <c r="AB6" t="str">
+        <v>orderedProbitXParamTransform</v>
+      </c>
+      <c r="AC6" t="str">
+        <f t="shared" si="2"/>
+        <v>orderedProbitXPDF</v>
+      </c>
+      <c r="AD6" t="str">
+        <f>B6&amp;"PlotDistr"</f>
+        <v>orderedProbitXPlotDistr</v>
+      </c>
+      <c r="AE6" t="str">
+        <f>B6&amp;"Draws"</f>
+        <v>orderedProbitXDraws</v>
+      </c>
+      <c r="AF6" t="str">
+        <f>B6&amp;"Latex"</f>
+        <v>orderedProbitXLatex</v>
+      </c>
+      <c r="AG6" t="str">
         <f t="shared" si="3"/>
-        <v>orderedProbitXParamTransform</v>
-      </c>
-      <c r="AC6" t="str">
+        <v>orderedProbitXChartDomain</v>
+      </c>
+      <c r="AH6" t="str">
         <f t="shared" si="4"/>
-        <v>orderedProbitXPDF</v>
-      </c>
-      <c r="AD6" t="str">
-        <f t="shared" ref="AD6" si="12">B6&amp;"PlotDistr"</f>
-        <v>orderedProbitXPlotDistr</v>
-      </c>
-      <c r="AE6" t="str">
-        <f t="shared" ref="AE6" si="13">B6&amp;"Draws"</f>
-        <v>orderedProbitXDraws</v>
-      </c>
-      <c r="AF6" t="str">
-        <f t="shared" ref="AF6" si="14">B6&amp;"Latex"</f>
-        <v>orderedProbitXLatex</v>
-      </c>
-      <c r="AG6" t="str">
-        <f t="shared" si="5"/>
-        <v>orderedProbitXChartDomain</v>
-      </c>
-      <c r="AH6" t="str">
-        <f t="shared" si="6"/>
         <v>orderedProbitXLikelihoodFun</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="E7" s="1">
         <v>3</v>
@@ -1600,40 +1588,40 @@
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="M7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="S7" s="1">
         <v>-3</v>
@@ -1642,68 +1630,68 @@
         <v>3</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="X7">
         <v>0.01</v>
       </c>
       <c r="Y7" t="str">
-        <f t="shared" ref="Y7" si="15">"""&amp;"&amp;RIGHT(M7,LEN(M7)-1)&amp;";"""</f>
+        <f>"""&amp;"&amp;RIGHT(M7,LEN(M7)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="Z7" t="str">
+        <f>IF(F7=1,"""none""",IF(E7=F7,"""betas""","""fullNorm"""))</f>
+        <v>"fullNorm"</v>
+      </c>
+      <c r="AA7" t="str">
+        <f t="shared" ref="AA7" si="8">"manyParamSliderMaker(minVal ="&amp;S7&amp;", maxVal = "&amp;T7&amp;", startVals = "&amp;U7&amp;", stepVal = "&amp;X7&amp;", paramHTML = "&amp;Y7&amp;", multi = "&amp;Z7&amp;", sigmaScale ="&amp;V7&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+      </c>
+      <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="AA7" t="str">
-        <f t="shared" ref="AA7" si="16">"manyParamSliderMaker(minVal ="&amp;S7&amp;", maxVal = "&amp;T7&amp;", startVals = "&amp;U7&amp;", stepVal = "&amp;X7&amp;", paramHTML = "&amp;Y7&amp;", multi = "&amp;Z7&amp;", sigmaScale ="&amp;V7&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
-      </c>
-      <c r="AB7" t="str">
+        <v>orderedLogitXParamTransform</v>
+      </c>
+      <c r="AC7" t="str">
+        <f t="shared" si="2"/>
+        <v>orderedLogitXPDF</v>
+      </c>
+      <c r="AD7" t="str">
+        <f t="shared" ref="AD7" si="9">B7&amp;"PlotDistr"</f>
+        <v>orderedLogitXPlotDistr</v>
+      </c>
+      <c r="AE7" t="str">
+        <f t="shared" ref="AE7" si="10">B7&amp;"Draws"</f>
+        <v>orderedLogitXDraws</v>
+      </c>
+      <c r="AF7" t="str">
+        <f t="shared" ref="AF7" si="11">B7&amp;"Latex"</f>
+        <v>orderedLogitXLatex</v>
+      </c>
+      <c r="AG7" t="str">
         <f t="shared" si="3"/>
-        <v>orderedLogitXParamTransform</v>
-      </c>
-      <c r="AC7" t="str">
+        <v>orderedLogitXChartDomain</v>
+      </c>
+      <c r="AH7" t="str">
         <f t="shared" si="4"/>
-        <v>orderedLogitXPDF</v>
-      </c>
-      <c r="AD7" t="str">
-        <f t="shared" ref="AD7" si="17">B7&amp;"PlotDistr"</f>
-        <v>orderedLogitXPlotDistr</v>
-      </c>
-      <c r="AE7" t="str">
-        <f t="shared" ref="AE7" si="18">B7&amp;"Draws"</f>
-        <v>orderedLogitXDraws</v>
-      </c>
-      <c r="AF7" t="str">
-        <f t="shared" ref="AF7" si="19">B7&amp;"Latex"</f>
-        <v>orderedLogitXLatex</v>
-      </c>
-      <c r="AG7" t="str">
-        <f t="shared" si="5"/>
-        <v>orderedLogitXChartDomain</v>
-      </c>
-      <c r="AH7" t="str">
-        <f t="shared" si="6"/>
         <v>orderedLogitXLikelihoodFun</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
@@ -1715,40 +1703,40 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="S8" s="1">
         <v>-4</v>
@@ -1757,68 +1745,68 @@
         <v>4</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X8">
         <v>0.01</v>
       </c>
       <c r="Y8" t="str">
+        <f>"""&amp;"&amp;RIGHT(M8,LEN(M8)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z8" t="str">
+        <f>IF(F8=1,"""none""",IF(E8=F8,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
+      <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z8" t="str">
+        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="AA8" t="str">
+        <v>styNormParamTransform</v>
+      </c>
+      <c r="AC8" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AB8" t="str">
+        <v>styNormPDF</v>
+      </c>
+      <c r="AD8" t="str">
+        <f t="shared" ref="AD8:AD19" si="12">B8&amp;"PlotDistr"</f>
+        <v>styNormPlotDistr</v>
+      </c>
+      <c r="AE8" t="str">
+        <f t="shared" ref="AE8:AE19" si="13">B8&amp;"Draws"</f>
+        <v>styNormDraws</v>
+      </c>
+      <c r="AF8" t="str">
+        <f t="shared" ref="AF8:AF19" si="14">B8&amp;"Latex"</f>
+        <v>styNormLatex</v>
+      </c>
+      <c r="AG8" t="str">
         <f t="shared" si="3"/>
-        <v>styNormParamTransform</v>
-      </c>
-      <c r="AC8" t="str">
+        <v>styNormChartDomain</v>
+      </c>
+      <c r="AH8" t="str">
         <f t="shared" si="4"/>
-        <v>styNormPDF</v>
-      </c>
-      <c r="AD8" t="str">
-        <f t="shared" ref="AD8:AD19" si="20">B8&amp;"PlotDistr"</f>
-        <v>styNormPlotDistr</v>
-      </c>
-      <c r="AE8" t="str">
-        <f t="shared" ref="AE8:AE19" si="21">B8&amp;"Draws"</f>
-        <v>styNormDraws</v>
-      </c>
-      <c r="AF8" t="str">
-        <f t="shared" ref="AF8:AF19" si="22">B8&amp;"Latex"</f>
-        <v>styNormLatex</v>
-      </c>
-      <c r="AG8" t="str">
-        <f t="shared" si="5"/>
-        <v>styNormChartDomain</v>
-      </c>
-      <c r="AH8" t="str">
-        <f t="shared" si="6"/>
         <v>styNormLikelihoodFun</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
@@ -1830,40 +1818,40 @@
         <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="P9" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="S9" s="1">
         <v>-3</v>
@@ -1872,68 +1860,68 @@
         <v>3</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X9">
         <v>0.01</v>
       </c>
       <c r="Y9" t="str">
+        <f>"""&amp;"&amp;RIGHT(M9,LEN(M9)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z9" t="str">
+        <f>IF(F9=1,"""none""",IF(E9=F9,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
+      </c>
+      <c r="AA9" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z9" t="str">
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AB9" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="AA9" t="str">
+        <v>styNormXParamTransform</v>
+      </c>
+      <c r="AC9" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AB9" t="str">
+        <v>styNormXPDF</v>
+      </c>
+      <c r="AD9" t="str">
+        <f t="shared" si="12"/>
+        <v>styNormXPlotDistr</v>
+      </c>
+      <c r="AE9" t="str">
+        <f t="shared" si="13"/>
+        <v>styNormXDraws</v>
+      </c>
+      <c r="AF9" t="str">
+        <f t="shared" si="14"/>
+        <v>styNormXLatex</v>
+      </c>
+      <c r="AG9" t="str">
         <f t="shared" si="3"/>
-        <v>styNormXParamTransform</v>
-      </c>
-      <c r="AC9" t="str">
+        <v>styNormXChartDomain</v>
+      </c>
+      <c r="AH9" t="str">
         <f t="shared" si="4"/>
-        <v>styNormXPDF</v>
-      </c>
-      <c r="AD9" t="str">
-        <f t="shared" si="20"/>
-        <v>styNormXPlotDistr</v>
-      </c>
-      <c r="AE9" t="str">
-        <f t="shared" si="21"/>
-        <v>styNormXDraws</v>
-      </c>
-      <c r="AF9" t="str">
-        <f t="shared" si="22"/>
-        <v>styNormXLatex</v>
-      </c>
-      <c r="AG9" t="str">
-        <f t="shared" si="5"/>
-        <v>styNormXChartDomain</v>
-      </c>
-      <c r="AH9" t="str">
-        <f t="shared" si="6"/>
         <v>styNormXLikelihoodFun</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
@@ -1945,40 +1933,40 @@
         <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="S10" s="1">
         <v>-3</v>
@@ -1987,71 +1975,71 @@
         <v>3</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X10">
         <v>0.01</v>
       </c>
       <c r="Y10" t="str">
+        <f>"""&amp;"&amp;RIGHT(M10,LEN(M10)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z10" t="str">
+        <f>IF(F10=1,"""none""",IF(E10=F10,"""betas""","""fullNorm"""))</f>
+        <v>"fullNorm"</v>
+      </c>
+      <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z10" t="str">
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+      </c>
+      <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="AA10" t="str">
+        <v>fullNormXParamTransform</v>
+      </c>
+      <c r="AC10" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
-      </c>
-      <c r="AB10" t="str">
+        <v>fullNormXPDF</v>
+      </c>
+      <c r="AD10" t="str">
+        <f t="shared" si="12"/>
+        <v>fullNormXPlotDistr</v>
+      </c>
+      <c r="AE10" t="str">
+        <f t="shared" si="13"/>
+        <v>fullNormXDraws</v>
+      </c>
+      <c r="AF10" t="str">
+        <f t="shared" si="14"/>
+        <v>fullNormXLatex</v>
+      </c>
+      <c r="AG10" t="str">
         <f t="shared" si="3"/>
-        <v>fullNormXParamTransform</v>
-      </c>
-      <c r="AC10" t="str">
+        <v>fullNormXChartDomain</v>
+      </c>
+      <c r="AH10" t="str">
         <f t="shared" si="4"/>
-        <v>fullNormXPDF</v>
-      </c>
-      <c r="AD10" t="str">
-        <f t="shared" si="20"/>
-        <v>fullNormXPlotDistr</v>
-      </c>
-      <c r="AE10" t="str">
-        <f t="shared" si="21"/>
-        <v>fullNormXDraws</v>
-      </c>
-      <c r="AF10" t="str">
-        <f t="shared" si="22"/>
-        <v>fullNormXLatex</v>
-      </c>
-      <c r="AG10" t="str">
-        <f t="shared" si="5"/>
-        <v>fullNormXChartDomain</v>
-      </c>
-      <c r="AH10" t="str">
-        <f t="shared" si="6"/>
         <v>fullNormXLikelihoodFun</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -2060,40 +2048,40 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="S11" s="1">
         <v>-0.5</v>
@@ -2102,71 +2090,71 @@
         <v>0.5</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X11">
         <v>0.01</v>
       </c>
       <c r="Y11" t="str">
+        <f>"""&amp;"&amp;RIGHT(M11,LEN(M11)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z11" t="str">
+        <f>IF(F11=1,"""none""",IF(E11=F11,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
+      <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z11" t="str">
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="AA11" t="str">
+        <v>logNormParamTransform</v>
+      </c>
+      <c r="AC11" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AB11" t="str">
+        <v>logNormPDF</v>
+      </c>
+      <c r="AD11" t="str">
+        <f t="shared" si="12"/>
+        <v>logNormPlotDistr</v>
+      </c>
+      <c r="AE11" t="str">
+        <f t="shared" si="13"/>
+        <v>logNormDraws</v>
+      </c>
+      <c r="AF11" t="str">
+        <f t="shared" si="14"/>
+        <v>logNormLatex</v>
+      </c>
+      <c r="AG11" t="str">
         <f t="shared" si="3"/>
-        <v>logNormParamTransform</v>
-      </c>
-      <c r="AC11" t="str">
+        <v>logNormChartDomain</v>
+      </c>
+      <c r="AH11" t="str">
         <f t="shared" si="4"/>
-        <v>logNormPDF</v>
-      </c>
-      <c r="AD11" t="str">
-        <f t="shared" si="20"/>
-        <v>logNormPlotDistr</v>
-      </c>
-      <c r="AE11" t="str">
-        <f t="shared" si="21"/>
-        <v>logNormDraws</v>
-      </c>
-      <c r="AF11" t="str">
-        <f t="shared" si="22"/>
-        <v>logNormLatex</v>
-      </c>
-      <c r="AG11" t="str">
-        <f t="shared" si="5"/>
-        <v>logNormChartDomain</v>
-      </c>
-      <c r="AH11" t="str">
-        <f t="shared" si="6"/>
         <v>logNormLikelihoodFun</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -2175,40 +2163,40 @@
         <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="S12" s="1">
         <v>-0.5</v>
@@ -2217,61 +2205,61 @@
         <v>0.5</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X12">
         <v>0.01</v>
       </c>
       <c r="Y12" t="str">
+        <f>"""&amp;"&amp;RIGHT(M12,LEN(M12)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z12" t="str">
+        <f>IF(F12=1,"""none""",IF(E12=F12,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
+      </c>
+      <c r="AA12" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z12" t="str">
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AB12" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="AA12" t="str">
+        <v>logNormXParamTransform</v>
+      </c>
+      <c r="AC12" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AB12" t="str">
+        <v>logNormXPDF</v>
+      </c>
+      <c r="AD12" t="str">
+        <f t="shared" si="12"/>
+        <v>logNormXPlotDistr</v>
+      </c>
+      <c r="AE12" t="str">
+        <f t="shared" si="13"/>
+        <v>logNormXDraws</v>
+      </c>
+      <c r="AF12" t="str">
+        <f t="shared" si="14"/>
+        <v>logNormXLatex</v>
+      </c>
+      <c r="AG12" t="str">
         <f t="shared" si="3"/>
-        <v>logNormXParamTransform</v>
-      </c>
-      <c r="AC12" t="str">
+        <v>logNormXChartDomain</v>
+      </c>
+      <c r="AH12" t="str">
         <f t="shared" si="4"/>
-        <v>logNormXPDF</v>
-      </c>
-      <c r="AD12" t="str">
-        <f t="shared" si="20"/>
-        <v>logNormXPlotDistr</v>
-      </c>
-      <c r="AE12" t="str">
-        <f t="shared" si="21"/>
-        <v>logNormXDraws</v>
-      </c>
-      <c r="AF12" t="str">
-        <f t="shared" si="22"/>
-        <v>logNormXLatex</v>
-      </c>
-      <c r="AG12" t="str">
-        <f t="shared" si="5"/>
-        <v>logNormXChartDomain</v>
-      </c>
-      <c r="AH12" t="str">
-        <f t="shared" si="6"/>
         <v>logNormXLikelihoodFun</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2290,40 +2278,40 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>28</v>
+        <v>146</v>
       </c>
       <c r="M13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="P13" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S13" s="1">
         <v>1</v>
@@ -2332,68 +2320,68 @@
         <v>10</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X13">
         <v>0.01</v>
       </c>
       <c r="Y13" t="str">
+        <f>"""&amp;"&amp;RIGHT(M13,LEN(M13)-1)&amp;";"""</f>
+        <v>"&amp;lambda;"</v>
+      </c>
+      <c r="Z13" t="str">
+        <f>IF(F13=1,"""none""",IF(E13=F13,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
+      <c r="AA13" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;lambda;"</v>
-      </c>
-      <c r="Z13" t="str">
+        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB13" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="AA13" t="str">
+        <v>poisParamTransform</v>
+      </c>
+      <c r="AC13" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AB13" t="str">
+        <v>poisPDF</v>
+      </c>
+      <c r="AD13" t="str">
+        <f t="shared" si="12"/>
+        <v>poisPlotDistr</v>
+      </c>
+      <c r="AE13" t="str">
+        <f t="shared" si="13"/>
+        <v>poisDraws</v>
+      </c>
+      <c r="AF13" t="str">
+        <f t="shared" si="14"/>
+        <v>poisLatex</v>
+      </c>
+      <c r="AG13" t="str">
         <f t="shared" si="3"/>
-        <v>poisParamTransform</v>
-      </c>
-      <c r="AC13" t="str">
+        <v>poisChartDomain</v>
+      </c>
+      <c r="AH13" t="str">
         <f t="shared" si="4"/>
-        <v>poisPDF</v>
-      </c>
-      <c r="AD13" t="str">
-        <f t="shared" si="20"/>
-        <v>poisPlotDistr</v>
-      </c>
-      <c r="AE13" t="str">
-        <f t="shared" si="21"/>
-        <v>poisDraws</v>
-      </c>
-      <c r="AF13" t="str">
-        <f t="shared" si="22"/>
-        <v>poisLatex</v>
-      </c>
-      <c r="AG13" t="str">
-        <f t="shared" si="5"/>
-        <v>poisChartDomain</v>
-      </c>
-      <c r="AH13" t="str">
-        <f t="shared" si="6"/>
         <v>poisLikelihoodFun</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>0</v>
@@ -2405,40 +2393,40 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S14" s="1">
         <v>-0.25</v>
@@ -2447,68 +2435,68 @@
         <v>3</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X14">
         <v>0.01</v>
       </c>
       <c r="Y14" t="str">
+        <f>"""&amp;"&amp;RIGHT(M14,LEN(M14)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z14" t="str">
+        <f>IF(F14=1,"""none""",IF(E14=F14,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
+      <c r="AA14" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z14" t="str">
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB14" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="AA14" t="str">
+        <v>poisExpParamTransform</v>
+      </c>
+      <c r="AC14" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AB14" t="str">
+        <v>poisExpPDF</v>
+      </c>
+      <c r="AD14" t="str">
+        <f t="shared" si="12"/>
+        <v>poisExpPlotDistr</v>
+      </c>
+      <c r="AE14" t="str">
+        <f t="shared" si="13"/>
+        <v>poisExpDraws</v>
+      </c>
+      <c r="AF14" t="str">
+        <f t="shared" si="14"/>
+        <v>poisExpLatex</v>
+      </c>
+      <c r="AG14" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpParamTransform</v>
-      </c>
-      <c r="AC14" t="str">
+        <v>poisExpChartDomain</v>
+      </c>
+      <c r="AH14" t="str">
         <f t="shared" si="4"/>
-        <v>poisExpPDF</v>
-      </c>
-      <c r="AD14" t="str">
-        <f t="shared" si="20"/>
-        <v>poisExpPlotDistr</v>
-      </c>
-      <c r="AE14" t="str">
-        <f t="shared" si="21"/>
-        <v>poisExpDraws</v>
-      </c>
-      <c r="AF14" t="str">
-        <f t="shared" si="22"/>
-        <v>poisExpLatex</v>
-      </c>
-      <c r="AG14" t="str">
-        <f t="shared" si="5"/>
-        <v>poisExpChartDomain</v>
-      </c>
-      <c r="AH14" t="str">
-        <f t="shared" si="6"/>
         <v>poisExpLikelihoodFun</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>0</v>
@@ -2520,40 +2508,40 @@
         <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S15" s="1">
         <v>-0.25</v>
@@ -2562,68 +2550,68 @@
         <v>3</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X15">
         <v>0.01</v>
       </c>
       <c r="Y15" t="str">
+        <f>"""&amp;"&amp;RIGHT(M15,LEN(M15)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z15" t="str">
+        <f>IF(F15=1,"""none""",IF(E15=F15,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
+      </c>
+      <c r="AA15" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z15" t="str">
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AB15" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="AA15" t="str">
+        <v>poisExpXParamTransform</v>
+      </c>
+      <c r="AC15" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AB15" t="str">
+        <v>poisExpXPDF</v>
+      </c>
+      <c r="AD15" t="str">
+        <f t="shared" si="12"/>
+        <v>poisExpXPlotDistr</v>
+      </c>
+      <c r="AE15" t="str">
+        <f t="shared" si="13"/>
+        <v>poisExpXDraws</v>
+      </c>
+      <c r="AF15" t="str">
+        <f t="shared" si="14"/>
+        <v>poisExpXLatex</v>
+      </c>
+      <c r="AG15" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpXParamTransform</v>
-      </c>
-      <c r="AC15" t="str">
+        <v>poisExpXChartDomain</v>
+      </c>
+      <c r="AH15" t="str">
         <f t="shared" si="4"/>
-        <v>poisExpXPDF</v>
-      </c>
-      <c r="AD15" t="str">
-        <f t="shared" si="20"/>
-        <v>poisExpXPlotDistr</v>
-      </c>
-      <c r="AE15" t="str">
-        <f t="shared" si="21"/>
-        <v>poisExpXDraws</v>
-      </c>
-      <c r="AF15" t="str">
-        <f t="shared" si="22"/>
-        <v>poisExpXLatex</v>
-      </c>
-      <c r="AG15" t="str">
-        <f t="shared" si="5"/>
-        <v>poisExpXChartDomain</v>
-      </c>
-      <c r="AH15" t="str">
-        <f t="shared" si="6"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>0</v>
@@ -2635,40 +2623,40 @@
         <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S16" s="1">
         <v>-0.25</v>
@@ -2677,27 +2665,27 @@
         <v>1.5</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X16">
         <v>0.01</v>
       </c>
       <c r="Y16" t="str">
+        <f>"""&amp;"&amp;RIGHT(M16,LEN(M16)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z16" t="str">
+        <f>IF(F16=1,"""none""",IF(E16=F16,"""betas""","""fullNorm"""))</f>
+        <v>"fullNorm"</v>
+      </c>
+      <c r="AA16" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z16" t="str">
-        <f t="shared" si="1"/>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="AA16" t="str">
-        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 1.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1,2),</v>
       </c>
       <c r="AB16" t="str">
@@ -2709,15 +2697,15 @@
         <v>negBinomXPDF</v>
       </c>
       <c r="AD16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="12"/>
         <v>negBinomXPlotDistr</v>
       </c>
       <c r="AE16" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="13"/>
         <v>negBinomXDraws</v>
       </c>
       <c r="AF16" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="14"/>
         <v>negBinomXLatex</v>
       </c>
       <c r="AG16" t="str">
@@ -2731,7 +2719,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2750,40 +2738,40 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>28</v>
+        <v>146</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S17" s="1">
         <v>0.25</v>
@@ -2792,68 +2780,68 @@
         <v>1.5</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X17">
         <v>0.01</v>
       </c>
       <c r="Y17" t="str">
+        <f>"""&amp;"&amp;RIGHT(M17,LEN(M17)-1)&amp;";"""</f>
+        <v>"&amp;lambda;"</v>
+      </c>
+      <c r="Z17" t="str">
+        <f>IF(F17=1,"""none""",IF(E17=F17,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
+      <c r="AA17" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;lambda;"</v>
-      </c>
-      <c r="Z17" t="str">
+        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB17" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="AA17" t="str">
+        <v>expParamTransform</v>
+      </c>
+      <c r="AC17" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AB17" t="str">
+        <v>expPDF</v>
+      </c>
+      <c r="AD17" t="str">
+        <f t="shared" si="12"/>
+        <v>expPlotDistr</v>
+      </c>
+      <c r="AE17" t="str">
+        <f t="shared" si="13"/>
+        <v>expDraws</v>
+      </c>
+      <c r="AF17" t="str">
+        <f t="shared" si="14"/>
+        <v>expLatex</v>
+      </c>
+      <c r="AG17" t="str">
         <f t="shared" si="3"/>
-        <v>expParamTransform</v>
-      </c>
-      <c r="AC17" t="str">
+        <v>expChartDomain</v>
+      </c>
+      <c r="AH17" t="str">
         <f t="shared" si="4"/>
-        <v>expPDF</v>
-      </c>
-      <c r="AD17" t="str">
-        <f t="shared" si="20"/>
-        <v>expPlotDistr</v>
-      </c>
-      <c r="AE17" t="str">
-        <f t="shared" si="21"/>
-        <v>expDraws</v>
-      </c>
-      <c r="AF17" t="str">
-        <f t="shared" si="22"/>
-        <v>expLatex</v>
-      </c>
-      <c r="AG17" t="str">
-        <f t="shared" si="5"/>
-        <v>expChartDomain</v>
-      </c>
-      <c r="AH17" t="str">
-        <f t="shared" si="6"/>
         <v>expLikelihoodFun</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -2865,40 +2853,40 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S18" s="1">
         <v>-2</v>
@@ -2907,68 +2895,68 @@
         <v>2</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X18">
         <v>0.01</v>
       </c>
       <c r="Y18" t="str">
+        <f>"""&amp;"&amp;RIGHT(M18,LEN(M18)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z18" t="str">
+        <f>IF(F18=1,"""none""",IF(E18=F18,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
+      <c r="AA18" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z18" t="str">
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
+      </c>
+      <c r="AB18" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="AA18" t="str">
+        <v>expExpParamTransform</v>
+      </c>
+      <c r="AC18" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
-      </c>
-      <c r="AB18" t="str">
+        <v>expExpPDF</v>
+      </c>
+      <c r="AD18" t="str">
+        <f t="shared" si="12"/>
+        <v>expExpPlotDistr</v>
+      </c>
+      <c r="AE18" t="str">
+        <f t="shared" si="13"/>
+        <v>expExpDraws</v>
+      </c>
+      <c r="AF18" t="str">
+        <f t="shared" si="14"/>
+        <v>expExpLatex</v>
+      </c>
+      <c r="AG18" t="str">
         <f t="shared" si="3"/>
-        <v>expExpParamTransform</v>
-      </c>
-      <c r="AC18" t="str">
+        <v>expExpChartDomain</v>
+      </c>
+      <c r="AH18" t="str">
         <f t="shared" si="4"/>
-        <v>expExpPDF</v>
-      </c>
-      <c r="AD18" t="str">
-        <f t="shared" si="20"/>
-        <v>expExpPlotDistr</v>
-      </c>
-      <c r="AE18" t="str">
-        <f t="shared" si="21"/>
-        <v>expExpDraws</v>
-      </c>
-      <c r="AF18" t="str">
-        <f t="shared" si="22"/>
-        <v>expExpLatex</v>
-      </c>
-      <c r="AG18" t="str">
-        <f t="shared" si="5"/>
-        <v>expExpChartDomain</v>
-      </c>
-      <c r="AH18" t="str">
-        <f t="shared" si="6"/>
         <v>expExpLikelihoodFun</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -2980,40 +2968,40 @@
         <v>3</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S19" s="1">
         <v>-0.5</v>
@@ -3022,286 +3010,56 @@
         <v>0.5</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="X19">
         <v>0.01</v>
       </c>
       <c r="Y19" t="str">
+        <f>"""&amp;"&amp;RIGHT(M19,LEN(M19)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="Z19" t="str">
+        <f>IF(F19=1,"""none""",IF(E19=F19,"""betas""","""fullNorm"""))</f>
+        <v>"betas"</v>
+      </c>
+      <c r="AA19" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z19" t="str">
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AB19" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="AA19" t="str">
+        <v>expExpXParamTransform</v>
+      </c>
+      <c r="AC19" t="str">
         <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AB19" t="str">
+        <v>expExpXPDF</v>
+      </c>
+      <c r="AD19" t="str">
+        <f t="shared" si="12"/>
+        <v>expExpXPlotDistr</v>
+      </c>
+      <c r="AE19" t="str">
+        <f t="shared" si="13"/>
+        <v>expExpXDraws</v>
+      </c>
+      <c r="AF19" t="str">
+        <f t="shared" si="14"/>
+        <v>expExpXLatex</v>
+      </c>
+      <c r="AG19" t="str">
         <f t="shared" si="3"/>
-        <v>expExpXParamTransform</v>
-      </c>
-      <c r="AC19" t="str">
+        <v>expExpXChartDomain</v>
+      </c>
+      <c r="AH19" t="str">
         <f t="shared" si="4"/>
-        <v>expExpXPDF</v>
-      </c>
-      <c r="AD19" t="str">
-        <f t="shared" si="20"/>
-        <v>expExpXPlotDistr</v>
-      </c>
-      <c r="AE19" t="str">
-        <f t="shared" si="21"/>
-        <v>expExpXDraws</v>
-      </c>
-      <c r="AF19" t="str">
-        <f t="shared" si="22"/>
-        <v>expExpXLatex</v>
-      </c>
-      <c r="AG19" t="str">
-        <f t="shared" si="5"/>
-        <v>expExpXChartDomain</v>
-      </c>
-      <c r="AH19" t="str">
-        <f t="shared" si="6"/>
         <v>expExpXLikelihoodFun</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="7"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="1">
-        <v>3</v>
-      </c>
-      <c r="F20" s="1">
-        <v>3</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="S20" s="1">
-        <v>-0.5</v>
-      </c>
-      <c r="T20" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="X20">
-        <v>0.01</v>
-      </c>
-      <c r="Y20" t="str">
-        <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z20" t="str">
-        <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="AA20" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AB20" t="str">
-        <f t="shared" si="3"/>
-        <v>neumayerParamTransform</v>
-      </c>
-      <c r="AC20" t="str">
-        <f t="shared" si="4"/>
-        <v>neumayerPDF</v>
-      </c>
-      <c r="AD20" t="str">
-        <f t="shared" ref="AD20" si="23">B20&amp;"PlotDistr"</f>
-        <v>neumayerPlotDistr</v>
-      </c>
-      <c r="AE20" t="str">
-        <f t="shared" ref="AE20" si="24">B20&amp;"Draws"</f>
-        <v>neumayerDraws</v>
-      </c>
-      <c r="AF20" t="str">
-        <f t="shared" ref="AF20" si="25">B20&amp;"Latex"</f>
-        <v>neumayerLatex</v>
-      </c>
-      <c r="AG20" t="str">
-        <f t="shared" si="5"/>
-        <v>neumayerChartDomain</v>
-      </c>
-      <c r="AH20" t="str">
-        <f t="shared" si="6"/>
-        <v>neumayerLikelihoodFun</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="7"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="1">
-        <v>3</v>
-      </c>
-      <c r="F21" s="1">
-        <v>3</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="S21" s="1">
-        <v>-0.5</v>
-      </c>
-      <c r="T21" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="X21">
-        <v>0.01</v>
-      </c>
-      <c r="Y21" t="str">
-        <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z21" t="str">
-        <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="AA21" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
-      <c r="AB21" t="str">
-        <f t="shared" si="3"/>
-        <v>drehJenParamTransform</v>
-      </c>
-      <c r="AC21" t="str">
-        <f t="shared" si="4"/>
-        <v>drehJenPDF</v>
-      </c>
-      <c r="AD21" t="str">
-        <f>B21&amp;"PlotDistr"</f>
-        <v>drehJenPlotDistr</v>
-      </c>
-      <c r="AE21" t="str">
-        <f>B21&amp;"Draws"</f>
-        <v>drehJenDraws</v>
-      </c>
-      <c r="AF21" t="str">
-        <f>B21&amp;"Latex"</f>
-        <v>drehJenLatex</v>
-      </c>
-      <c r="AG21" t="str">
-        <f t="shared" si="5"/>
-        <v>drehJenChartDomain</v>
-      </c>
-      <c r="AH21" t="str">
-        <f t="shared" si="6"/>
-        <v>drehJenLikelihoodFun</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first draft of plus x
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80FB7FC-F75A-437D-A680-90A27B4F2C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A6C076-EF5D-4788-AAD2-32CA0B05F2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="155">
   <si>
     <t>Poisson</t>
   </si>
@@ -393,9 +393,6 @@
     <t>c("Beta0", "Beta1")</t>
   </si>
   <si>
-    <t>c(-1,.6,3, 1,-1)</t>
-  </si>
-  <si>
     <t>c(-1.5,1.5)</t>
   </si>
   <si>
@@ -429,9 +426,6 @@
     <t>Nelder-Mead</t>
   </si>
   <si>
-    <t>c(1,-1,1.25)</t>
-  </si>
-  <si>
     <t>orderedLogitX</t>
   </si>
   <si>
@@ -492,7 +486,19 @@
     <t>c("\\beta_0", "\\beta_1", "\\beta_2", "\\beta_3", "\\gamma")</t>
   </si>
   <si>
-    <t>c(1,-2,1.25)</t>
+    <t>nNonXParams</t>
+  </si>
+  <si>
+    <t>c(1,-1,.25, .5)</t>
+  </si>
+  <si>
+    <t>c(1,-2,1.25, .5, .5)</t>
+  </si>
+  <si>
+    <t>c(1,-1,1.25, -.5,.5)</t>
+  </si>
+  <si>
+    <t>c(-1,.6,3, 1,-1,-.6)</t>
   </si>
 </sst>
 </file>
@@ -859,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:AH19"/>
+  <dimension ref="A1:AI19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,27 +878,27 @@
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="10" width="31.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="18" width="9.42578125" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" customWidth="1"/>
-    <col min="20" max="20" width="4.28515625" customWidth="1"/>
-    <col min="21" max="23" width="7.140625" customWidth="1"/>
-    <col min="24" max="24" width="6" customWidth="1"/>
-    <col min="25" max="26" width="4.28515625" customWidth="1"/>
-    <col min="27" max="27" width="16" customWidth="1"/>
-    <col min="28" max="29" width="26" customWidth="1"/>
-    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="15.5703125" customWidth="1"/>
+    <col min="6" max="7" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="11" width="31.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="18" max="19" width="9.42578125" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" customWidth="1"/>
+    <col min="21" max="21" width="4.28515625" customWidth="1"/>
+    <col min="22" max="24" width="7.140625" customWidth="1"/>
+    <col min="25" max="25" width="6" customWidth="1"/>
+    <col min="26" max="27" width="4.28515625" customWidth="1"/>
+    <col min="28" max="28" width="16" customWidth="1"/>
+    <col min="29" max="30" width="26" customWidth="1"/>
+    <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -903,7 +909,7 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
         <v>113</v>
@@ -912,91 +918,94 @@
         <v>114</v>
       </c>
       <c r="G1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
-        <v>128</v>
-      </c>
       <c r="K1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
-        <v>144</v>
-      </c>
       <c r="M1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>139</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" t="s">
+        <v>115</v>
+      </c>
+      <c r="T1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE1" t="s">
         <v>141</v>
       </c>
-      <c r="O1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
-      </c>
-      <c r="R1" t="s">
-        <v>115</v>
-      </c>
-      <c r="S1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" t="s">
-        <v>47</v>
-      </c>
-      <c r="U1" t="s">
-        <v>48</v>
-      </c>
-      <c r="V1" t="s">
-        <v>80</v>
-      </c>
-      <c r="W1" t="s">
-        <v>136</v>
-      </c>
-      <c r="X1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>140</v>
       </c>
-      <c r="AC1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>22</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1015,102 +1024,105 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="K2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>28</v>
+        <v>143</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="R2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>0</v>
       </c>
-      <c r="T2" s="1">
+      <c r="U2" s="1">
         <v>1</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y2">
         <v>0.01</v>
       </c>
-      <c r="Y2" t="str">
-        <f>"""&amp;"&amp;RIGHT(M2,LEN(M2)-1)&amp;";"""</f>
+      <c r="Z2" t="str">
+        <f t="shared" ref="Z2:Z19" si="0">"""&amp;"&amp;RIGHT(N2,LEN(N2)-1)&amp;";"""</f>
         <v>"&amp;pi;"</v>
       </c>
-      <c r="Z2" t="str">
-        <f>IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
+      <c r="AA2" t="str">
+        <f t="shared" ref="AA2:AA19" si="1">IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
-      <c r="AA2" t="str">
-        <f t="shared" ref="AA2:AA19" si="0">"manyParamSliderMaker(minVal ="&amp;S2&amp;", maxVal = "&amp;T2&amp;", startVals = "&amp;U2&amp;", stepVal = "&amp;X2&amp;", paramHTML = "&amp;Y2&amp;", multi = "&amp;Z2&amp;", sigmaScale ="&amp;V2&amp;","</f>
+      <c r="AB2" t="str">
+        <f t="shared" ref="AB2:AB19" si="2">"manyParamSliderMaker(minVal ="&amp;T2&amp;", maxVal = "&amp;U2&amp;", startVals = "&amp;V2&amp;", stepVal = "&amp;Y2&amp;", paramHTML = "&amp;Z2&amp;", multi = "&amp;AA2&amp;", sigmaScale ="&amp;W2&amp;","</f>
         <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AC2" t="str">
         <f>$B2&amp;"ParamTransform"</f>
         <v>bernParamTransform</v>
       </c>
-      <c r="AC2" t="str">
+      <c r="AD2" t="str">
         <f>$B2&amp;"PDF"</f>
         <v>bernPDF</v>
       </c>
-      <c r="AD2" t="str">
+      <c r="AE2" t="str">
         <f>B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
-      <c r="AE2" t="str">
+      <c r="AF2" t="str">
         <f>B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
-      <c r="AF2" t="str">
+      <c r="AG2" t="str">
         <f>B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
-      <c r="AG2" t="str">
+      <c r="AH2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="AH2" t="str">
+      <c r="AI2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1130,104 +1142,107 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="M3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="R3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>-2</v>
       </c>
-      <c r="T3" s="1">
+      <c r="U3" s="1">
         <v>2</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y3">
         <v>0.01</v>
       </c>
-      <c r="Y3" t="str">
-        <f>"""&amp;"&amp;RIGHT(M3,LEN(M3)-1)&amp;";"""</f>
+      <c r="Z3" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z3" t="str">
-        <f>IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
+      <c r="AA3" t="str">
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AA3" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB3" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB19" si="1">$B3&amp;"ParamTransform"</f>
+      <c r="AC3" t="str">
+        <f t="shared" ref="AC3:AC19" si="3">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
-      <c r="AC3" t="str">
-        <f t="shared" ref="AC3:AC19" si="2">$B3&amp;"PDF"</f>
+      <c r="AD3" t="str">
+        <f t="shared" ref="AD3:AD19" si="4">$B3&amp;"PDF"</f>
         <v>bernLogitPDF</v>
       </c>
-      <c r="AD3" t="str">
+      <c r="AE3" t="str">
         <f>B3&amp;"PlotDistr"</f>
         <v>bernLogitPlotDistr</v>
       </c>
-      <c r="AE3" t="str">
+      <c r="AF3" t="str">
         <f>B3&amp;"Draws"</f>
         <v>bernLogitDraws</v>
       </c>
-      <c r="AF3" t="str">
+      <c r="AG3" t="str">
         <f>B3&amp;"Latex"</f>
         <v>bernLogitLatex</v>
       </c>
-      <c r="AG3" t="str">
-        <f t="shared" ref="AG3:AG19" si="3">$B3&amp;"ChartDomain"</f>
+      <c r="AH3" t="str">
+        <f t="shared" ref="AH3:AH19" si="5">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
-      <c r="AH3" t="str">
-        <f t="shared" ref="AH3:AH19" si="4">$B3&amp;"LikelihoodFun"</f>
+      <c r="AI3" t="str">
+        <f t="shared" ref="AI3:AI19" si="6">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A19" si="5">A3+1</f>
+        <f t="shared" ref="A4:A19" si="7">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1240,454 +1255,466 @@
         <v>2</v>
       </c>
       <c r="E4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="M4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="R4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>-4</v>
       </c>
-      <c r="T4" s="1">
+      <c r="U4" s="1">
         <v>4</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="V4" s="1" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y4">
         <v>0.01</v>
       </c>
-      <c r="Y4" t="str">
-        <f>"""&amp;"&amp;RIGHT(M4,LEN(M4)-1)&amp;";"""</f>
+      <c r="Z4" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z4" t="str">
-        <f>IF(F4=1,"""none""",IF(E4=F4,"""betas""","""fullNorm"""))</f>
+      <c r="AA4" t="str">
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AA4" t="str">
-        <f t="shared" si="0"/>
-        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
-      </c>
       <c r="AB4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1,-1,.25, .5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
+      </c>
+      <c r="AC4" t="str">
+        <f t="shared" si="3"/>
         <v>bernLogitXParamTransform</v>
       </c>
-      <c r="AC4" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD4" t="str">
+        <f t="shared" si="4"/>
         <v>bernLogitXPDF</v>
       </c>
-      <c r="AD4" t="str">
+      <c r="AE4" t="str">
         <f>B4&amp;"PlotDistr"</f>
         <v>bernLogitXPlotDistr</v>
       </c>
-      <c r="AE4" t="str">
+      <c r="AF4" t="str">
         <f>B4&amp;"Draws"</f>
         <v>bernLogitXDraws</v>
       </c>
-      <c r="AF4" t="str">
+      <c r="AG4" t="str">
         <f>B4&amp;"Latex"</f>
         <v>bernLogitXLatex</v>
       </c>
-      <c r="AG4" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH4" t="str">
+        <f t="shared" si="5"/>
         <v>bernLogitXChartDomain</v>
       </c>
-      <c r="AH4" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI4" t="str">
+        <f t="shared" si="6"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="I5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="M5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="R5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <v>-2</v>
       </c>
-      <c r="T5" s="1">
+      <c r="U5" s="1">
         <v>2</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y5">
         <v>0.01</v>
       </c>
-      <c r="Y5" t="str">
-        <f>"""&amp;"&amp;RIGHT(M5,LEN(M5)-1)&amp;";"""</f>
+      <c r="Z5" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z5" t="str">
-        <f>IF(F5=1,"""none""",IF(E5=F5,"""betas""","""fullNorm"""))</f>
+      <c r="AA5" t="str">
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AA5" t="str">
-        <f t="shared" ref="AA5" si="6">"manyParamSliderMaker(minVal ="&amp;S5&amp;", maxVal = "&amp;T5&amp;", startVals = "&amp;U5&amp;", stepVal = "&amp;X5&amp;", paramHTML = "&amp;Y5&amp;", multi = "&amp;Z5&amp;", sigmaScale ="&amp;V5&amp;","</f>
+      <c r="AB5" t="str">
+        <f t="shared" ref="AB5" si="8">"manyParamSliderMaker(minVal ="&amp;T5&amp;", maxVal = "&amp;U5&amp;", startVals = "&amp;V5&amp;", stepVal = "&amp;Y5&amp;", paramHTML = "&amp;Z5&amp;", multi = "&amp;AA5&amp;", sigmaScale ="&amp;W5&amp;","</f>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AB5" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC5" t="str">
+        <f t="shared" si="3"/>
         <v>bernProbitXParamTransform</v>
       </c>
-      <c r="AC5" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD5" t="str">
+        <f t="shared" si="4"/>
         <v>bernProbitXPDF</v>
       </c>
-      <c r="AD5" t="str">
+      <c r="AE5" t="str">
         <f>B5&amp;"PlotDistr"</f>
         <v>bernProbitXPlotDistr</v>
       </c>
-      <c r="AE5" t="str">
+      <c r="AF5" t="str">
         <f>B5&amp;"Draws"</f>
         <v>bernProbitXDraws</v>
       </c>
-      <c r="AF5" t="str">
+      <c r="AG5" t="str">
         <f>B5&amp;"Latex"</f>
         <v>bernProbitXLatex</v>
       </c>
-      <c r="AG5" t="str">
+      <c r="AH5" t="str">
+        <f t="shared" si="5"/>
+        <v>bernProbitXChartDomain</v>
+      </c>
+      <c r="AI5" t="str">
+        <f t="shared" si="6"/>
+        <v>bernProbitXLikelihoodFun</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T6" s="1">
+        <v>-3</v>
+      </c>
+      <c r="U6" s="1">
+        <v>3</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y6">
+        <v>0.01</v>
+      </c>
+      <c r="Z6" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" si="1"/>
+        <v>"fullNorm"</v>
+      </c>
+      <c r="AB6" t="str">
+        <f t="shared" ref="AB6" si="9">"manyParamSliderMaker(minVal ="&amp;T6&amp;", maxVal = "&amp;U6&amp;", startVals = "&amp;V6&amp;", stepVal = "&amp;Y6&amp;", paramHTML = "&amp;Z6&amp;", multi = "&amp;AA6&amp;", sigmaScale ="&amp;W6&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-2,1.25, .5, .5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+      </c>
+      <c r="AC6" t="str">
         <f t="shared" si="3"/>
-        <v>bernProbitXChartDomain</v>
-      </c>
-      <c r="AH5" t="str">
+        <v>orderedProbitXParamTransform</v>
+      </c>
+      <c r="AD6" t="str">
         <f t="shared" si="4"/>
-        <v>bernProbitXLikelihoodFun</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S6" s="1">
-        <v>-3</v>
-      </c>
-      <c r="T6" s="1">
-        <v>3</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="X6">
-        <v>0.01</v>
-      </c>
-      <c r="Y6" t="str">
-        <f>"""&amp;"&amp;RIGHT(M6,LEN(M6)-1)&amp;";"""</f>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z6" t="str">
-        <f>IF(F6=1,"""none""",IF(E6=F6,"""betas""","""fullNorm"""))</f>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="AA6" t="str">
-        <f t="shared" ref="AA6" si="7">"manyParamSliderMaker(minVal ="&amp;S6&amp;", maxVal = "&amp;T6&amp;", startVals = "&amp;U6&amp;", stepVal = "&amp;X6&amp;", paramHTML = "&amp;Y6&amp;", multi = "&amp;Z6&amp;", sigmaScale ="&amp;V6&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-2,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
-      </c>
-      <c r="AB6" t="str">
-        <f t="shared" si="1"/>
-        <v>orderedProbitXParamTransform</v>
-      </c>
-      <c r="AC6" t="str">
-        <f t="shared" si="2"/>
         <v>orderedProbitXPDF</v>
       </c>
-      <c r="AD6" t="str">
+      <c r="AE6" t="str">
         <f>B6&amp;"PlotDistr"</f>
         <v>orderedProbitXPlotDistr</v>
       </c>
-      <c r="AE6" t="str">
+      <c r="AF6" t="str">
         <f>B6&amp;"Draws"</f>
         <v>orderedProbitXDraws</v>
       </c>
-      <c r="AF6" t="str">
+      <c r="AG6" t="str">
         <f>B6&amp;"Latex"</f>
         <v>orderedProbitXLatex</v>
       </c>
-      <c r="AG6" t="str">
+      <c r="AH6" t="str">
+        <f t="shared" si="5"/>
+        <v>orderedProbitXChartDomain</v>
+      </c>
+      <c r="AI6" t="str">
+        <f t="shared" si="6"/>
+        <v>orderedProbitXLikelihoodFun</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T7" s="1">
+        <v>-3</v>
+      </c>
+      <c r="U7" s="1">
+        <v>3</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y7">
+        <v>0.01</v>
+      </c>
+      <c r="Z7" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="AA7" t="str">
+        <f t="shared" si="1"/>
+        <v>"fullNorm"</v>
+      </c>
+      <c r="AB7" t="str">
+        <f t="shared" ref="AB7" si="10">"manyParamSliderMaker(minVal ="&amp;T7&amp;", maxVal = "&amp;U7&amp;", startVals = "&amp;V7&amp;", stepVal = "&amp;Y7&amp;", paramHTML = "&amp;Z7&amp;", multi = "&amp;AA7&amp;", sigmaScale ="&amp;W7&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25, -.5,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+      </c>
+      <c r="AC7" t="str">
         <f t="shared" si="3"/>
-        <v>orderedProbitXChartDomain</v>
-      </c>
-      <c r="AH6" t="str">
+        <v>orderedLogitXParamTransform</v>
+      </c>
+      <c r="AD7" t="str">
         <f t="shared" si="4"/>
-        <v>orderedProbitXLikelihoodFun</v>
+        <v>orderedLogitXPDF</v>
+      </c>
+      <c r="AE7" t="str">
+        <f t="shared" ref="AE7" si="11">B7&amp;"PlotDistr"</f>
+        <v>orderedLogitXPlotDistr</v>
+      </c>
+      <c r="AF7" t="str">
+        <f t="shared" ref="AF7" si="12">B7&amp;"Draws"</f>
+        <v>orderedLogitXDraws</v>
+      </c>
+      <c r="AG7" t="str">
+        <f t="shared" ref="AG7" si="13">B7&amp;"Latex"</f>
+        <v>orderedLogitXLatex</v>
+      </c>
+      <c r="AH7" t="str">
+        <f t="shared" si="5"/>
+        <v>orderedLogitXChartDomain</v>
+      </c>
+      <c r="AI7" t="str">
+        <f t="shared" si="6"/>
+        <v>orderedLogitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S7" s="1">
-        <v>-3</v>
-      </c>
-      <c r="T7" s="1">
-        <v>3</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="X7">
-        <v>0.01</v>
-      </c>
-      <c r="Y7" t="str">
-        <f>"""&amp;"&amp;RIGHT(M7,LEN(M7)-1)&amp;";"""</f>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="Z7" t="str">
-        <f>IF(F7=1,"""none""",IF(E7=F7,"""betas""","""fullNorm"""))</f>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="AA7" t="str">
-        <f t="shared" ref="AA7" si="8">"manyParamSliderMaker(minVal ="&amp;S7&amp;", maxVal = "&amp;T7&amp;", startVals = "&amp;U7&amp;", stepVal = "&amp;X7&amp;", paramHTML = "&amp;Y7&amp;", multi = "&amp;Z7&amp;", sigmaScale ="&amp;V7&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
-      </c>
-      <c r="AB7" t="str">
-        <f t="shared" si="1"/>
-        <v>orderedLogitXParamTransform</v>
-      </c>
-      <c r="AC7" t="str">
-        <f t="shared" si="2"/>
-        <v>orderedLogitXPDF</v>
-      </c>
-      <c r="AD7" t="str">
-        <f t="shared" ref="AD7" si="9">B7&amp;"PlotDistr"</f>
-        <v>orderedLogitXPlotDistr</v>
-      </c>
-      <c r="AE7" t="str">
-        <f t="shared" ref="AE7" si="10">B7&amp;"Draws"</f>
-        <v>orderedLogitXDraws</v>
-      </c>
-      <c r="AF7" t="str">
-        <f t="shared" ref="AF7" si="11">B7&amp;"Latex"</f>
-        <v>orderedLogitXLatex</v>
-      </c>
-      <c r="AG7" t="str">
-        <f t="shared" si="3"/>
-        <v>orderedLogitXChartDomain</v>
-      </c>
-      <c r="AH7" t="str">
-        <f t="shared" si="4"/>
-        <v>orderedLogitXLikelihoodFun</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1705,104 +1732,107 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="M8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>-4</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U8" s="1">
         <v>4</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X8">
+      <c r="X8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y8">
         <v>0.01</v>
       </c>
-      <c r="Y8" t="str">
-        <f>"""&amp;"&amp;RIGHT(M8,LEN(M8)-1)&amp;";"""</f>
+      <c r="Z8" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z8" t="str">
-        <f>IF(F8=1,"""none""",IF(E8=F8,"""betas""","""fullNorm"""))</f>
+      <c r="AA8" t="str">
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AA8" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB8" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AB8" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC8" t="str">
+        <f t="shared" si="3"/>
         <v>styNormParamTransform</v>
       </c>
-      <c r="AC8" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD8" t="str">
+        <f t="shared" si="4"/>
         <v>styNormPDF</v>
       </c>
-      <c r="AD8" t="str">
-        <f t="shared" ref="AD8:AD19" si="12">B8&amp;"PlotDistr"</f>
+      <c r="AE8" t="str">
+        <f t="shared" ref="AE8:AE19" si="14">B8&amp;"PlotDistr"</f>
         <v>styNormPlotDistr</v>
       </c>
-      <c r="AE8" t="str">
-        <f t="shared" ref="AE8:AE19" si="13">B8&amp;"Draws"</f>
+      <c r="AF8" t="str">
+        <f t="shared" ref="AF8:AF19" si="15">B8&amp;"Draws"</f>
         <v>styNormDraws</v>
       </c>
-      <c r="AF8" t="str">
-        <f t="shared" ref="AF8:AF19" si="14">B8&amp;"Latex"</f>
+      <c r="AG8" t="str">
+        <f t="shared" ref="AG8:AG19" si="16">B8&amp;"Latex"</f>
         <v>styNormLatex</v>
       </c>
-      <c r="AG8" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH8" t="str">
+        <f t="shared" si="5"/>
         <v>styNormChartDomain</v>
       </c>
-      <c r="AH8" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI8" t="str">
+        <f t="shared" si="6"/>
         <v>styNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1815,109 +1845,112 @@
         <v>3</v>
       </c>
       <c r="E9" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="M9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T9" s="1">
         <v>-3</v>
       </c>
-      <c r="T9" s="1">
+      <c r="U9" s="1">
         <v>3</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="V9" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y9">
         <v>0.01</v>
       </c>
-      <c r="Y9" t="str">
-        <f>"""&amp;"&amp;RIGHT(M9,LEN(M9)-1)&amp;";"""</f>
+      <c r="Z9" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z9" t="str">
-        <f>IF(F9=1,"""none""",IF(E9=F9,"""betas""","""fullNorm"""))</f>
+      <c r="AA9" t="str">
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AA9" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB9" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AB9" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC9" t="str">
+        <f t="shared" si="3"/>
         <v>styNormXParamTransform</v>
       </c>
-      <c r="AC9" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD9" t="str">
+        <f t="shared" si="4"/>
         <v>styNormXPDF</v>
       </c>
-      <c r="AD9" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE9" t="str">
+        <f t="shared" si="14"/>
         <v>styNormXPlotDistr</v>
       </c>
-      <c r="AE9" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF9" t="str">
+        <f t="shared" si="15"/>
         <v>styNormXDraws</v>
       </c>
-      <c r="AF9" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG9" t="str">
+        <f t="shared" si="16"/>
         <v>styNormXLatex</v>
       </c>
-      <c r="AG9" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH9" t="str">
+        <f t="shared" si="5"/>
         <v>styNormXChartDomain</v>
       </c>
-      <c r="AH9" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI9" t="str">
+        <f t="shared" si="6"/>
         <v>styNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1930,109 +1963,112 @@
         <v>3</v>
       </c>
       <c r="E10" s="1">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1">
         <v>5</v>
       </c>
-      <c r="F10" s="1">
-        <v>4</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="M10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <v>-3</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U10" s="1">
         <v>3</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="V10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="W10" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="V10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="X10">
+      <c r="X10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y10">
         <v>0.01</v>
       </c>
-      <c r="Y10" t="str">
-        <f>"""&amp;"&amp;RIGHT(M10,LEN(M10)-1)&amp;";"""</f>
+      <c r="Z10" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z10" t="str">
-        <f>IF(F10=1,"""none""",IF(E10=F10,"""betas""","""fullNorm"""))</f>
+      <c r="AA10" t="str">
+        <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
-      <c r="AA10" t="str">
-        <f t="shared" si="0"/>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
-      </c>
       <c r="AB10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1,-.6), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1.5,1.5),</v>
+      </c>
+      <c r="AC10" t="str">
+        <f t="shared" si="3"/>
         <v>fullNormXParamTransform</v>
       </c>
-      <c r="AC10" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD10" t="str">
+        <f t="shared" si="4"/>
         <v>fullNormXPDF</v>
       </c>
-      <c r="AD10" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE10" t="str">
+        <f t="shared" si="14"/>
         <v>fullNormXPlotDistr</v>
       </c>
-      <c r="AE10" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF10" t="str">
+        <f t="shared" si="15"/>
         <v>fullNormXDraws</v>
       </c>
-      <c r="AF10" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG10" t="str">
+        <f t="shared" si="16"/>
         <v>fullNormXLatex</v>
       </c>
-      <c r="AG10" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH10" t="str">
+        <f t="shared" si="5"/>
         <v>fullNormXChartDomain</v>
       </c>
-      <c r="AH10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI10" t="str">
+        <f t="shared" si="6"/>
         <v>fullNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2050,104 +2086,107 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="M11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <v>-0.5</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U11" s="1">
         <v>0.5</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="V11" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y11">
         <v>0.01</v>
       </c>
-      <c r="Y11" t="str">
-        <f>"""&amp;"&amp;RIGHT(M11,LEN(M11)-1)&amp;";"""</f>
+      <c r="Z11" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z11" t="str">
-        <f>IF(F11=1,"""none""",IF(E11=F11,"""betas""","""fullNorm"""))</f>
+      <c r="AA11" t="str">
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AA11" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB11" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AB11" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC11" t="str">
+        <f t="shared" si="3"/>
         <v>logNormParamTransform</v>
       </c>
-      <c r="AC11" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD11" t="str">
+        <f t="shared" si="4"/>
         <v>logNormPDF</v>
       </c>
-      <c r="AD11" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE11" t="str">
+        <f t="shared" si="14"/>
         <v>logNormPlotDistr</v>
       </c>
-      <c r="AE11" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF11" t="str">
+        <f t="shared" si="15"/>
         <v>logNormDraws</v>
       </c>
-      <c r="AF11" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG11" t="str">
+        <f t="shared" si="16"/>
         <v>logNormLatex</v>
       </c>
-      <c r="AG11" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH11" t="str">
+        <f t="shared" si="5"/>
         <v>logNormChartDomain</v>
       </c>
-      <c r="AH11" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI11" t="str">
+        <f t="shared" si="6"/>
         <v>logNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2165,104 +2204,107 @@
       <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="M12" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T12" s="1">
         <v>-0.5</v>
       </c>
-      <c r="T12" s="1">
+      <c r="U12" s="1">
         <v>0.5</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="V12" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y12">
         <v>0.01</v>
       </c>
-      <c r="Y12" t="str">
-        <f>"""&amp;"&amp;RIGHT(M12,LEN(M12)-1)&amp;";"""</f>
+      <c r="Z12" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z12" t="str">
-        <f>IF(F12=1,"""none""",IF(E12=F12,"""betas""","""fullNorm"""))</f>
+      <c r="AA12" t="str">
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AA12" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB12" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AB12" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC12" t="str">
+        <f t="shared" si="3"/>
         <v>logNormXParamTransform</v>
       </c>
-      <c r="AC12" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD12" t="str">
+        <f t="shared" si="4"/>
         <v>logNormXPDF</v>
       </c>
-      <c r="AD12" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE12" t="str">
+        <f t="shared" si="14"/>
         <v>logNormXPlotDistr</v>
       </c>
-      <c r="AE12" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF12" t="str">
+        <f t="shared" si="15"/>
         <v>logNormXDraws</v>
       </c>
-      <c r="AF12" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG12" t="str">
+        <f t="shared" si="16"/>
         <v>logNormXLatex</v>
       </c>
-      <c r="AG12" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH12" t="str">
+        <f t="shared" si="5"/>
         <v>logNormXChartDomain</v>
       </c>
-      <c r="AH12" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI12" t="str">
+        <f t="shared" si="6"/>
         <v>logNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2280,104 +2322,107 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="M13" s="1" t="s">
-        <v>30</v>
+        <v>144</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S13" s="1">
+      <c r="T13" s="1">
         <v>1</v>
       </c>
-      <c r="T13" s="1">
+      <c r="U13" s="1">
         <v>10</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="V13" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y13">
         <v>0.01</v>
       </c>
-      <c r="Y13" t="str">
-        <f>"""&amp;"&amp;RIGHT(M13,LEN(M13)-1)&amp;";"""</f>
+      <c r="Z13" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;lambda;"</v>
       </c>
-      <c r="Z13" t="str">
-        <f>IF(F13=1,"""none""",IF(E13=F13,"""betas""","""fullNorm"""))</f>
+      <c r="AA13" t="str">
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AA13" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB13" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AB13" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC13" t="str">
+        <f t="shared" si="3"/>
         <v>poisParamTransform</v>
       </c>
-      <c r="AC13" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD13" t="str">
+        <f t="shared" si="4"/>
         <v>poisPDF</v>
       </c>
-      <c r="AD13" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE13" t="str">
+        <f t="shared" si="14"/>
         <v>poisPlotDistr</v>
       </c>
-      <c r="AE13" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF13" t="str">
+        <f t="shared" si="15"/>
         <v>poisDraws</v>
       </c>
-      <c r="AF13" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG13" t="str">
+        <f t="shared" si="16"/>
         <v>poisLatex</v>
       </c>
-      <c r="AG13" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH13" t="str">
+        <f t="shared" si="5"/>
         <v>poisChartDomain</v>
       </c>
-      <c r="AH13" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI13" t="str">
+        <f t="shared" si="6"/>
         <v>poisLikelihoodFun</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2395,104 +2440,107 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="M14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S14" s="1">
+      <c r="T14" s="1">
         <v>-0.25</v>
       </c>
-      <c r="T14" s="1">
+      <c r="U14" s="1">
         <v>3</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="V14" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y14">
         <v>0.01</v>
       </c>
-      <c r="Y14" t="str">
-        <f>"""&amp;"&amp;RIGHT(M14,LEN(M14)-1)&amp;";"""</f>
+      <c r="Z14" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z14" t="str">
-        <f>IF(F14=1,"""none""",IF(E14=F14,"""betas""","""fullNorm"""))</f>
+      <c r="AA14" t="str">
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AA14" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB14" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AB14" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC14" t="str">
+        <f t="shared" si="3"/>
         <v>poisExpParamTransform</v>
       </c>
-      <c r="AC14" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD14" t="str">
+        <f t="shared" si="4"/>
         <v>poisExpPDF</v>
       </c>
-      <c r="AD14" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE14" t="str">
+        <f t="shared" si="14"/>
         <v>poisExpPlotDistr</v>
       </c>
-      <c r="AE14" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF14" t="str">
+        <f t="shared" si="15"/>
         <v>poisExpDraws</v>
       </c>
-      <c r="AF14" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG14" t="str">
+        <f t="shared" si="16"/>
         <v>poisExpLatex</v>
       </c>
-      <c r="AG14" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH14" t="str">
+        <f t="shared" si="5"/>
         <v>poisExpChartDomain</v>
       </c>
-      <c r="AH14" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI14" t="str">
+        <f t="shared" si="6"/>
         <v>poisExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2510,104 +2558,107 @@
       <c r="F15" s="1">
         <v>3</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="M15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S15" s="1">
+      <c r="T15" s="1">
         <v>-0.25</v>
       </c>
-      <c r="T15" s="1">
+      <c r="U15" s="1">
         <v>3</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="V15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="V15" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X15">
+      <c r="X15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y15">
         <v>0.01</v>
       </c>
-      <c r="Y15" t="str">
-        <f>"""&amp;"&amp;RIGHT(M15,LEN(M15)-1)&amp;";"""</f>
+      <c r="Z15" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z15" t="str">
-        <f>IF(F15=1,"""none""",IF(E15=F15,"""betas""","""fullNorm"""))</f>
+      <c r="AA15" t="str">
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AA15" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB15" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AB15" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC15" t="str">
+        <f t="shared" si="3"/>
         <v>poisExpXParamTransform</v>
       </c>
-      <c r="AC15" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD15" t="str">
+        <f t="shared" si="4"/>
         <v>poisExpXPDF</v>
       </c>
-      <c r="AD15" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE15" t="str">
+        <f t="shared" si="14"/>
         <v>poisExpXPlotDistr</v>
       </c>
-      <c r="AE15" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF15" t="str">
+        <f t="shared" si="15"/>
         <v>poisExpXDraws</v>
       </c>
-      <c r="AF15" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG15" t="str">
+        <f t="shared" si="16"/>
         <v>poisExpXLatex</v>
       </c>
-      <c r="AG15" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH15" t="str">
+        <f t="shared" si="5"/>
         <v>poisExpXChartDomain</v>
       </c>
-      <c r="AH15" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI15" t="str">
+        <f t="shared" si="6"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2620,109 +2671,112 @@
         <v>0</v>
       </c>
       <c r="E16" s="1">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1">
         <v>4</v>
       </c>
-      <c r="F16" s="1">
-        <v>3</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="M16" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S16" s="1">
+      <c r="T16" s="1">
         <v>-0.25</v>
       </c>
-      <c r="T16" s="1">
+      <c r="U16" s="1">
         <v>1.5</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="V16" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="W16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="W16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="X16">
+      <c r="X16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y16">
         <v>0.01</v>
       </c>
-      <c r="Y16" t="str">
-        <f>"""&amp;"&amp;RIGHT(M16,LEN(M16)-1)&amp;";"""</f>
+      <c r="Z16" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z16" t="str">
-        <f>IF(F16=1,"""none""",IF(E16=F16,"""betas""","""fullNorm"""))</f>
+      <c r="AA16" t="str">
+        <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
-      <c r="AA16" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB16" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 1.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(-1,2),</v>
       </c>
-      <c r="AB16" t="str">
+      <c r="AC16" t="str">
         <f>$B16&amp;"ParamTransform"</f>
         <v>negBinomXParamTransform</v>
       </c>
-      <c r="AC16" t="str">
+      <c r="AD16" t="str">
         <f>$B16&amp;"PDF"</f>
         <v>negBinomXPDF</v>
       </c>
-      <c r="AD16" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE16" t="str">
+        <f t="shared" si="14"/>
         <v>negBinomXPlotDistr</v>
       </c>
-      <c r="AE16" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF16" t="str">
+        <f t="shared" si="15"/>
         <v>negBinomXDraws</v>
       </c>
-      <c r="AF16" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG16" t="str">
+        <f t="shared" si="16"/>
         <v>negBinomXLatex</v>
       </c>
-      <c r="AG16" t="str">
+      <c r="AH16" t="str">
         <f>$B16&amp;"ChartDomain"</f>
         <v>negBinomXChartDomain</v>
       </c>
-      <c r="AH16" t="str">
+      <c r="AI16" t="str">
         <f>$B16&amp;"LikelihoodFun"</f>
         <v>negBinomXLikelihoodFun</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2740,104 +2794,107 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="M17" s="1" t="s">
-        <v>30</v>
+        <v>144</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S17" s="1">
+      <c r="T17" s="1">
         <v>0.25</v>
       </c>
-      <c r="T17" s="1">
+      <c r="U17" s="1">
         <v>1.5</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="V17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="V17" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y17">
         <v>0.01</v>
       </c>
-      <c r="Y17" t="str">
-        <f>"""&amp;"&amp;RIGHT(M17,LEN(M17)-1)&amp;";"""</f>
+      <c r="Z17" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;lambda;"</v>
       </c>
-      <c r="Z17" t="str">
-        <f>IF(F17=1,"""none""",IF(E17=F17,"""betas""","""fullNorm"""))</f>
+      <c r="AA17" t="str">
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AA17" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB17" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AB17" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC17" t="str">
+        <f t="shared" si="3"/>
         <v>expParamTransform</v>
       </c>
-      <c r="AC17" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD17" t="str">
+        <f t="shared" si="4"/>
         <v>expPDF</v>
       </c>
-      <c r="AD17" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE17" t="str">
+        <f t="shared" si="14"/>
         <v>expPlotDistr</v>
       </c>
-      <c r="AE17" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF17" t="str">
+        <f t="shared" si="15"/>
         <v>expDraws</v>
       </c>
-      <c r="AF17" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG17" t="str">
+        <f t="shared" si="16"/>
         <v>expLatex</v>
       </c>
-      <c r="AG17" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH17" t="str">
+        <f t="shared" si="5"/>
         <v>expChartDomain</v>
       </c>
-      <c r="AH17" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI17" t="str">
+        <f t="shared" si="6"/>
         <v>expLikelihoodFun</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2855,104 +2912,107 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="M18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S18" s="1">
+      <c r="T18" s="1">
         <v>-2</v>
       </c>
-      <c r="T18" s="1">
+      <c r="U18" s="1">
         <v>2</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="V18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="V18" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X18">
+      <c r="X18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y18">
         <v>0.01</v>
       </c>
-      <c r="Y18" t="str">
-        <f>"""&amp;"&amp;RIGHT(M18,LEN(M18)-1)&amp;";"""</f>
+      <c r="Z18" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z18" t="str">
-        <f>IF(F18=1,"""none""",IF(E18=F18,"""betas""","""fullNorm"""))</f>
+      <c r="AA18" t="str">
+        <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AA18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB18" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AB18" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC18" t="str">
+        <f t="shared" si="3"/>
         <v>expExpParamTransform</v>
       </c>
-      <c r="AC18" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD18" t="str">
+        <f t="shared" si="4"/>
         <v>expExpPDF</v>
       </c>
-      <c r="AD18" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE18" t="str">
+        <f t="shared" si="14"/>
         <v>expExpPlotDistr</v>
       </c>
-      <c r="AE18" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF18" t="str">
+        <f t="shared" si="15"/>
         <v>expExpDraws</v>
       </c>
-      <c r="AF18" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG18" t="str">
+        <f t="shared" si="16"/>
         <v>expExpLatex</v>
       </c>
-      <c r="AG18" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH18" t="str">
+        <f t="shared" si="5"/>
         <v>expExpChartDomain</v>
       </c>
-      <c r="AH18" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI18" t="str">
+        <f t="shared" si="6"/>
         <v>expExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2970,98 +3030,101 @@
       <c r="F19" s="1">
         <v>3</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="K19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="M19" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S19" s="1">
+      <c r="T19" s="1">
         <v>-0.5</v>
       </c>
-      <c r="T19" s="1">
+      <c r="U19" s="1">
         <v>0.5</v>
       </c>
-      <c r="U19" s="1" t="s">
+      <c r="V19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="V19" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="W19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X19">
+      <c r="X19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y19">
         <v>0.01</v>
       </c>
-      <c r="Y19" t="str">
-        <f>"""&amp;"&amp;RIGHT(M19,LEN(M19)-1)&amp;";"""</f>
+      <c r="Z19" t="str">
+        <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="Z19" t="str">
-        <f>IF(F19=1,"""none""",IF(E19=F19,"""betas""","""fullNorm"""))</f>
+      <c r="AA19" t="str">
+        <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AA19" t="str">
-        <f t="shared" si="0"/>
+      <c r="AB19" t="str">
+        <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AB19" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC19" t="str">
+        <f t="shared" si="3"/>
         <v>expExpXParamTransform</v>
       </c>
-      <c r="AC19" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD19" t="str">
+        <f t="shared" si="4"/>
         <v>expExpXPDF</v>
       </c>
-      <c r="AD19" t="str">
-        <f t="shared" si="12"/>
+      <c r="AE19" t="str">
+        <f t="shared" si="14"/>
         <v>expExpXPlotDistr</v>
       </c>
-      <c r="AE19" t="str">
-        <f t="shared" si="13"/>
+      <c r="AF19" t="str">
+        <f t="shared" si="15"/>
         <v>expExpXDraws</v>
       </c>
-      <c r="AF19" t="str">
-        <f t="shared" si="14"/>
+      <c r="AG19" t="str">
+        <f t="shared" si="16"/>
         <v>expExpXLatex</v>
       </c>
-      <c r="AG19" t="str">
-        <f t="shared" si="3"/>
+      <c r="AH19" t="str">
+        <f t="shared" si="5"/>
         <v>expExpXChartDomain</v>
       </c>
-      <c r="AH19" t="str">
-        <f t="shared" si="4"/>
+      <c r="AI19" t="str">
+        <f t="shared" si="6"/>
         <v>expExpXLikelihoodFun</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes, white space removal
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECCD0EA-2640-47A9-9E07-38B6D6D32381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B950AA94-1788-479E-BF2E-336F77789C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="167">
   <si>
     <t>Poisson</t>
   </si>
@@ -294,30 +294,9 @@
     <t>Bernoulli (Logit, X)</t>
   </si>
   <si>
-    <t>list("Bernoulli","Bernoulli (Logit)", "Bernoulli (Logit, X)")</t>
-  </si>
-  <si>
-    <t>list("Bernoulli (Logit)","Bernoulli", "Bernoulli (Logit, X)")</t>
-  </si>
-  <si>
-    <t>list("Bernoulli (Logit, X)","Bernoulli","Bernoulli (Logit)")</t>
-  </si>
-  <si>
-    <t>list("Stylized Normal","Stylized Normal (X)")</t>
-  </si>
-  <si>
-    <t>list("Stylized Normal (X)","Stylized Normal")</t>
-  </si>
-  <si>
     <t>list("Normal (X)", "Stylized Normal (X)","Stylized Normal")</t>
   </si>
   <si>
-    <t>list("Log Normal","Stylized Normal","Stylized Normal (X)")</t>
-  </si>
-  <si>
-    <t>list("Log Normal (X)","Stylized Normal","Stylized Normal (X)")</t>
-  </si>
-  <si>
     <t>Stylized Normal</t>
   </si>
   <si>
@@ -408,9 +387,6 @@
     <t>Ordered Probit (X)</t>
   </si>
   <si>
-    <t>list("Ordered Probit (X)")</t>
-  </si>
-  <si>
     <t>c(1,3)</t>
   </si>
   <si>
@@ -432,9 +408,6 @@
     <t>Ordered</t>
   </si>
   <si>
-    <t>list("Ordered Logit (X)")</t>
-  </si>
-  <si>
     <t>yStarPDF</t>
   </si>
   <si>
@@ -513,9 +486,6 @@
     <t>c(1,2)</t>
   </si>
   <si>
-    <t>c(0,4)</t>
-  </si>
-  <si>
     <t>reparamTex</t>
   </si>
   <si>
@@ -529,6 +499,42 @@
   </si>
   <si>
     <t>c(-2.5,2.5)</t>
+  </si>
+  <si>
+    <t>sliderMinA</t>
+  </si>
+  <si>
+    <t>sliderMaxA</t>
+  </si>
+  <si>
+    <t>c(0.1,4)</t>
+  </si>
+  <si>
+    <t>list("Bernoulli","Bernoulli (Logit)", "Bernoulli (Logit, X)","Bernoulli (Probit, X)")</t>
+  </si>
+  <si>
+    <t>list("Bernoulli (Logit)","Bernoulli", "Bernoulli (Logit, X)","Bernoulli (Probit, X)")</t>
+  </si>
+  <si>
+    <t>list("Bernoulli (Logit, X)","Bernoulli","Bernoulli (Logit)","Bernoulli (Probit, X)")</t>
+  </si>
+  <si>
+    <t>list("Ordered Probit (X)","Ordered Logit (X)")</t>
+  </si>
+  <si>
+    <t>list("Ordered Logit (X)","Ordered Probit (X)")</t>
+  </si>
+  <si>
+    <t>list("Stylized Normal","Stylized Normal (X)","Normal (X)")</t>
+  </si>
+  <si>
+    <t>list("Stylized Normal (X)","Stylized Normal","Normal (X)")</t>
+  </si>
+  <si>
+    <t>list("Log Normal","Stylized Normal","Stylized Normal (X)","Normal (X)")</t>
+  </si>
+  <si>
+    <t>list("Log Normal (X)","Stylized Normal","Stylized Normal (X)","Normal (X)")</t>
   </si>
 </sst>
 </file>
@@ -895,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:AL19"/>
+  <dimension ref="A1:AN19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,19 +922,19 @@
     <col min="19" max="19" width="10" customWidth="1"/>
     <col min="20" max="21" width="9.42578125" customWidth="1"/>
     <col min="22" max="22" width="6.140625" customWidth="1"/>
-    <col min="23" max="23" width="4.28515625" customWidth="1"/>
-    <col min="24" max="27" width="7.140625" customWidth="1"/>
-    <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="30" width="4.28515625" customWidth="1"/>
-    <col min="31" max="31" width="16" customWidth="1"/>
-    <col min="32" max="33" width="26" customWidth="1"/>
-    <col min="34" max="34" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="15.5703125" customWidth="1"/>
+    <col min="23" max="25" width="4.28515625" customWidth="1"/>
+    <col min="26" max="29" width="7.140625" customWidth="1"/>
+    <col min="30" max="30" width="6" customWidth="1"/>
+    <col min="31" max="32" width="4.28515625" customWidth="1"/>
+    <col min="33" max="33" width="16" customWidth="1"/>
+    <col min="34" max="35" width="26" customWidth="1"/>
+    <col min="36" max="36" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -939,16 +945,16 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
@@ -960,25 +966,25 @@
         <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="L1" t="s">
         <v>34</v>
       </c>
       <c r="M1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="N1" t="s">
         <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="P1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="Q1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="R1" t="s">
         <v>32</v>
@@ -990,7 +996,7 @@
         <v>62</v>
       </c>
       <c r="U1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="V1" t="s">
         <v>46</v>
@@ -999,52 +1005,58 @@
         <v>47</v>
       </c>
       <c r="X1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z1" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>80</v>
       </c>
-      <c r="Z1" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>133</v>
-      </c>
       <c r="AB1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD1" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>52</v>
       </c>
-      <c r="AF1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AI1" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>139</v>
-      </c>
       <c r="AJ1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL1" t="s">
         <v>19</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>22</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1070,19 +1082,19 @@
         <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>86</v>
+        <v>158</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>28</v>
@@ -1114,63 +1126,69 @@
       <c r="W2" s="1">
         <v>1</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2">
         <v>0.01</v>
       </c>
-      <c r="AC2" t="str">
-        <f t="shared" ref="AC2:AC19" si="0">"""&amp;"&amp;RIGHT(N2,LEN(N2)-1)&amp;";"""</f>
+      <c r="AE2" t="str">
+        <f t="shared" ref="AE2:AE19" si="0">"""&amp;"&amp;RIGHT(N2,LEN(N2)-1)&amp;";"""</f>
         <v>"&amp;pi;"</v>
       </c>
-      <c r="AD2" t="str">
-        <f t="shared" ref="AD2:AD19" si="1">IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
+      <c r="AF2" t="str">
+        <f t="shared" ref="AF2:AF19" si="1">IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
-      <c r="AE2" t="str">
-        <f t="shared" ref="AE2:AE19" si="2">"manyParamSliderMaker(minVal ="&amp;V2&amp;", maxVal = "&amp;W2&amp;", startVals = "&amp;X2&amp;", stepVal = "&amp;AB2&amp;", paramHTML = "&amp;AC2&amp;", multi = "&amp;AD2&amp;", sigmaScale ="&amp;Y2&amp;","</f>
+      <c r="AG2" t="str">
+        <f t="shared" ref="AG2:AG19" si="2">"manyParamSliderMaker(minVal ="&amp;V2&amp;", maxVal = "&amp;W2&amp;", startVals = "&amp;Z2&amp;", stepVal = "&amp;AD2&amp;", paramHTML = "&amp;AE2&amp;", multi = "&amp;AF2&amp;", sigmaScale ="&amp;AA2&amp;","</f>
         <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AF2" t="str">
+      <c r="AH2" t="str">
         <f>$B2&amp;"ParamTransform"</f>
         <v>bernParamTransform</v>
       </c>
-      <c r="AG2" t="str">
+      <c r="AI2" t="str">
         <f>$B2&amp;"PDF"</f>
         <v>bernPDF</v>
       </c>
-      <c r="AH2" t="str">
+      <c r="AJ2" t="str">
         <f>B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
-      <c r="AI2" t="str">
+      <c r="AK2" t="str">
         <f>B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
-      <c r="AJ2" t="str">
+      <c r="AL2" t="str">
         <f>B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
-      <c r="AK2" t="str">
+      <c r="AM2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="AL2" t="str">
+      <c r="AN2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1197,19 +1215,19 @@
         <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>87</v>
+        <v>159</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>29</v>
@@ -1241,63 +1259,69 @@
       <c r="W3" s="1">
         <v>2</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="X3" s="1">
+        <v>-3</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD3">
         <v>0.01</v>
       </c>
-      <c r="AC3" t="str">
+      <c r="AE3" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD3" t="str">
+      <c r="AF3" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AE3" t="str">
+      <c r="AG3" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AF3" t="str">
-        <f t="shared" ref="AF3:AF19" si="3">$B3&amp;"ParamTransform"</f>
+      <c r="AH3" t="str">
+        <f t="shared" ref="AH3:AH19" si="3">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
-      <c r="AG3" t="str">
-        <f t="shared" ref="AG3:AG19" si="4">$B3&amp;"PDF"</f>
+      <c r="AI3" t="str">
+        <f t="shared" ref="AI3:AI19" si="4">$B3&amp;"PDF"</f>
         <v>bernLogitPDF</v>
       </c>
-      <c r="AH3" t="str">
+      <c r="AJ3" t="str">
         <f>B3&amp;"PlotDistr"</f>
         <v>bernLogitPlotDistr</v>
       </c>
-      <c r="AI3" t="str">
+      <c r="AK3" t="str">
         <f>B3&amp;"Draws"</f>
         <v>bernLogitDraws</v>
       </c>
-      <c r="AJ3" t="str">
+      <c r="AL3" t="str">
         <f>B3&amp;"Latex"</f>
         <v>bernLogitLatex</v>
       </c>
-      <c r="AK3" t="str">
-        <f t="shared" ref="AK3:AK19" si="5">$B3&amp;"ChartDomain"</f>
+      <c r="AM3" t="str">
+        <f t="shared" ref="AM3:AM19" si="5">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
-      <c r="AL3" t="str">
-        <f t="shared" ref="AL3:AL19" si="6">$B3&amp;"LikelihoodFun"</f>
+      <c r="AN3" t="str">
+        <f t="shared" ref="AN3:AN19" si="6">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A19" si="7">A3+1</f>
         <v>3</v>
@@ -1324,19 +1348,19 @@
         <v>20</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>88</v>
+        <v>160</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>29</v>
@@ -1368,72 +1392,78 @@
       <c r="W4" s="1">
         <v>4</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>61</v>
+      <c r="X4" s="1">
+        <v>-5</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>5</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD4">
         <v>0.01</v>
       </c>
-      <c r="AC4" t="str">
+      <c r="AE4" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD4" t="str">
+      <c r="AF4" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AE4" t="str">
+      <c r="AG4" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1,-1,.25, .5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AF4" t="str">
+      <c r="AH4" t="str">
         <f t="shared" si="3"/>
         <v>bernLogitXParamTransform</v>
       </c>
-      <c r="AG4" t="str">
+      <c r="AI4" t="str">
         <f t="shared" si="4"/>
         <v>bernLogitXPDF</v>
       </c>
-      <c r="AH4" t="str">
+      <c r="AJ4" t="str">
         <f>B4&amp;"PlotDistr"</f>
         <v>bernLogitXPlotDistr</v>
       </c>
-      <c r="AI4" t="str">
+      <c r="AK4" t="str">
         <f>B4&amp;"Draws"</f>
         <v>bernLogitXDraws</v>
       </c>
-      <c r="AJ4" t="str">
+      <c r="AL4" t="str">
         <f>B4&amp;"Latex"</f>
         <v>bernLogitXLatex</v>
       </c>
-      <c r="AK4" t="str">
+      <c r="AM4" t="str">
         <f t="shared" si="5"/>
         <v>bernLogitXChartDomain</v>
       </c>
-      <c r="AL4" t="str">
+      <c r="AN4" t="str">
         <f t="shared" si="6"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -1451,19 +1481,19 @@
         <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>29</v>
@@ -1495,75 +1525,81 @@
       <c r="W5" s="1">
         <v>2</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Y5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD5">
         <v>0.01</v>
       </c>
-      <c r="AC5" t="str">
+      <c r="AE5" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD5" t="str">
+      <c r="AF5" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AE5" t="str">
-        <f t="shared" ref="AE5" si="8">"manyParamSliderMaker(minVal ="&amp;V5&amp;", maxVal = "&amp;W5&amp;", startVals = "&amp;X5&amp;", stepVal = "&amp;AB5&amp;", paramHTML = "&amp;AC5&amp;", multi = "&amp;AD5&amp;", sigmaScale ="&amp;Y5&amp;","</f>
+      <c r="AG5" t="str">
+        <f t="shared" ref="AG5" si="8">"manyParamSliderMaker(minVal ="&amp;V5&amp;", maxVal = "&amp;W5&amp;", startVals = "&amp;Z5&amp;", stepVal = "&amp;AD5&amp;", paramHTML = "&amp;AE5&amp;", multi = "&amp;AF5&amp;", sigmaScale ="&amp;AA5&amp;","</f>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AF5" t="str">
+      <c r="AH5" t="str">
         <f t="shared" si="3"/>
         <v>bernProbitXParamTransform</v>
       </c>
-      <c r="AG5" t="str">
+      <c r="AI5" t="str">
         <f t="shared" si="4"/>
         <v>bernProbitXPDF</v>
       </c>
-      <c r="AH5" t="str">
+      <c r="AJ5" t="str">
         <f>B5&amp;"PlotDistr"</f>
         <v>bernProbitXPlotDistr</v>
       </c>
-      <c r="AI5" t="str">
+      <c r="AK5" t="str">
         <f>B5&amp;"Draws"</f>
         <v>bernProbitXDraws</v>
       </c>
-      <c r="AJ5" t="str">
+      <c r="AL5" t="str">
         <f>B5&amp;"Latex"</f>
         <v>bernProbitXLatex</v>
       </c>
-      <c r="AK5" t="str">
+      <c r="AM5" t="str">
         <f t="shared" si="5"/>
         <v>bernProbitXChartDomain</v>
       </c>
-      <c r="AL5" t="str">
+      <c r="AN5" t="str">
         <f t="shared" si="6"/>
         <v>bernProbitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -1578,19 +1614,19 @@
         <v>20</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>29</v>
@@ -1599,16 +1635,16 @@
         <v>31</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>61</v>
@@ -1622,75 +1658,81 @@
       <c r="W6" s="1">
         <v>3</v>
       </c>
-      <c r="X6" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>159</v>
+      <c r="X6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>4</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB6">
+        <v>157</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD6">
         <v>0.01</v>
       </c>
-      <c r="AC6" t="str">
+      <c r="AE6" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD6" t="str">
+      <c r="AF6" t="str">
         <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
-      <c r="AE6" t="str">
-        <f t="shared" ref="AE6" si="9">"manyParamSliderMaker(minVal ="&amp;V6&amp;", maxVal = "&amp;W6&amp;", startVals = "&amp;X6&amp;", stepVal = "&amp;AB6&amp;", paramHTML = "&amp;AC6&amp;", multi = "&amp;AD6&amp;", sigmaScale ="&amp;Y6&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-2,1.25, .5, .5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(0,4),</v>
-      </c>
-      <c r="AF6" t="str">
+      <c r="AG6" t="str">
+        <f t="shared" ref="AG6" si="9">"manyParamSliderMaker(minVal ="&amp;V6&amp;", maxVal = "&amp;W6&amp;", startVals = "&amp;Z6&amp;", stepVal = "&amp;AD6&amp;", paramHTML = "&amp;AE6&amp;", multi = "&amp;AF6&amp;", sigmaScale ="&amp;AA6&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-2,1.25, .5, .5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(0.1,4),</v>
+      </c>
+      <c r="AH6" t="str">
         <f t="shared" si="3"/>
         <v>orderedProbitXParamTransform</v>
       </c>
-      <c r="AG6" t="str">
+      <c r="AI6" t="str">
         <f t="shared" si="4"/>
         <v>orderedProbitXPDF</v>
       </c>
-      <c r="AH6" t="str">
+      <c r="AJ6" t="str">
         <f>B6&amp;"PlotDistr"</f>
         <v>orderedProbitXPlotDistr</v>
       </c>
-      <c r="AI6" t="str">
+      <c r="AK6" t="str">
         <f>B6&amp;"Draws"</f>
         <v>orderedProbitXDraws</v>
       </c>
-      <c r="AJ6" t="str">
+      <c r="AL6" t="str">
         <f>B6&amp;"Latex"</f>
         <v>orderedProbitXLatex</v>
       </c>
-      <c r="AK6" t="str">
+      <c r="AM6" t="str">
         <f t="shared" si="5"/>
         <v>orderedProbitXChartDomain</v>
       </c>
-      <c r="AL6" t="str">
+      <c r="AN6" t="str">
         <f t="shared" si="6"/>
         <v>orderedProbitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -1705,19 +1747,19 @@
         <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>132</v>
+        <v>162</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>29</v>
@@ -1726,16 +1768,16 @@
         <v>31</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>61</v>
@@ -1749,63 +1791,69 @@
       <c r="W7" s="1">
         <v>3</v>
       </c>
-      <c r="X7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>159</v>
+      <c r="X7" s="1">
+        <v>-4</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>4</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AB7">
+        <v>157</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD7">
         <v>0.01</v>
       </c>
-      <c r="AC7" t="str">
+      <c r="AE7" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD7" t="str">
+      <c r="AF7" t="str">
         <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
-      <c r="AE7" t="str">
-        <f t="shared" ref="AE7" si="10">"manyParamSliderMaker(minVal ="&amp;V7&amp;", maxVal = "&amp;W7&amp;", startVals = "&amp;X7&amp;", stepVal = "&amp;AB7&amp;", paramHTML = "&amp;AC7&amp;", multi = "&amp;AD7&amp;", sigmaScale ="&amp;Y7&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25, -.5,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(0,4),</v>
-      </c>
-      <c r="AF7" t="str">
+      <c r="AG7" t="str">
+        <f t="shared" ref="AG7" si="10">"manyParamSliderMaker(minVal ="&amp;V7&amp;", maxVal = "&amp;W7&amp;", startVals = "&amp;Z7&amp;", stepVal = "&amp;AD7&amp;", paramHTML = "&amp;AE7&amp;", multi = "&amp;AF7&amp;", sigmaScale ="&amp;AA7&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,1.25, -.5,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(0.1,4),</v>
+      </c>
+      <c r="AH7" t="str">
         <f t="shared" si="3"/>
         <v>orderedLogitXParamTransform</v>
       </c>
-      <c r="AG7" t="str">
+      <c r="AI7" t="str">
         <f t="shared" si="4"/>
         <v>orderedLogitXPDF</v>
       </c>
-      <c r="AH7" t="str">
-        <f t="shared" ref="AH7" si="11">B7&amp;"PlotDistr"</f>
+      <c r="AJ7" t="str">
+        <f t="shared" ref="AJ7" si="11">B7&amp;"PlotDistr"</f>
         <v>orderedLogitXPlotDistr</v>
       </c>
-      <c r="AI7" t="str">
-        <f t="shared" ref="AI7" si="12">B7&amp;"Draws"</f>
+      <c r="AK7" t="str">
+        <f t="shared" ref="AK7" si="12">B7&amp;"Draws"</f>
         <v>orderedLogitXDraws</v>
       </c>
-      <c r="AJ7" t="str">
-        <f t="shared" ref="AJ7" si="13">B7&amp;"Latex"</f>
+      <c r="AL7" t="str">
+        <f t="shared" ref="AL7" si="13">B7&amp;"Latex"</f>
         <v>orderedLogitXLatex</v>
       </c>
-      <c r="AK7" t="str">
+      <c r="AM7" t="str">
         <f t="shared" si="5"/>
         <v>orderedLogitXChartDomain</v>
       </c>
-      <c r="AL7" t="str">
+      <c r="AN7" t="str">
         <f t="shared" si="6"/>
         <v>orderedLogitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="7"/>
         <v>7</v>
@@ -1814,7 +1862,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
@@ -1832,19 +1880,19 @@
         <v>21</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>29</v>
@@ -1868,7 +1916,7 @@
         <v>63</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="V8" s="1">
         <v>-4</v>
@@ -1876,63 +1924,69 @@
       <c r="W8" s="1">
         <v>4</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="X8" s="1">
+        <v>-5</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Y8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB8">
+      <c r="AB8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD8">
         <v>0.01</v>
       </c>
-      <c r="AC8" t="str">
+      <c r="AE8" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD8" t="str">
+      <c r="AF8" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AE8" t="str">
+      <c r="AG8" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-4, maxVal = 4, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AF8" t="str">
+      <c r="AH8" t="str">
         <f t="shared" si="3"/>
         <v>styNormParamTransform</v>
       </c>
-      <c r="AG8" t="str">
+      <c r="AI8" t="str">
         <f t="shared" si="4"/>
         <v>styNormPDF</v>
       </c>
-      <c r="AH8" t="str">
-        <f t="shared" ref="AH8:AH19" si="14">B8&amp;"PlotDistr"</f>
+      <c r="AJ8" t="str">
+        <f t="shared" ref="AJ8:AJ19" si="14">B8&amp;"PlotDistr"</f>
         <v>styNormPlotDistr</v>
       </c>
-      <c r="AI8" t="str">
-        <f t="shared" ref="AI8:AI19" si="15">B8&amp;"Draws"</f>
+      <c r="AK8" t="str">
+        <f t="shared" ref="AK8:AK19" si="15">B8&amp;"Draws"</f>
         <v>styNormDraws</v>
       </c>
-      <c r="AJ8" t="str">
-        <f t="shared" ref="AJ8:AJ19" si="16">B8&amp;"Latex"</f>
+      <c r="AL8" t="str">
+        <f t="shared" ref="AL8:AL19" si="16">B8&amp;"Latex"</f>
         <v>styNormLatex</v>
       </c>
-      <c r="AK8" t="str">
+      <c r="AM8" t="str">
         <f t="shared" si="5"/>
         <v>styNormChartDomain</v>
       </c>
-      <c r="AL8" t="str">
+      <c r="AN8" t="str">
         <f t="shared" si="6"/>
         <v>styNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="7"/>
         <v>8</v>
@@ -1941,7 +1995,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
@@ -1959,19 +2013,19 @@
         <v>21</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>29</v>
@@ -1995,7 +2049,7 @@
         <v>63</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="V9" s="1">
         <v>-3</v>
@@ -2003,63 +2057,69 @@
       <c r="W9" s="1">
         <v>3</v>
       </c>
-      <c r="X9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>61</v>
+      <c r="X9" s="1">
+        <v>-4</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>4</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="AA9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB9">
+      <c r="AB9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD9">
         <v>0.01</v>
       </c>
-      <c r="AC9" t="str">
+      <c r="AE9" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD9" t="str">
+      <c r="AF9" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AE9" t="str">
+      <c r="AG9" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AF9" t="str">
+      <c r="AH9" t="str">
         <f t="shared" si="3"/>
         <v>styNormXParamTransform</v>
       </c>
-      <c r="AG9" t="str">
+      <c r="AI9" t="str">
         <f t="shared" si="4"/>
         <v>styNormXPDF</v>
       </c>
-      <c r="AH9" t="str">
+      <c r="AJ9" t="str">
         <f t="shared" si="14"/>
         <v>styNormXPlotDistr</v>
       </c>
-      <c r="AI9" t="str">
+      <c r="AK9" t="str">
         <f t="shared" si="15"/>
         <v>styNormXDraws</v>
       </c>
-      <c r="AJ9" t="str">
+      <c r="AL9" t="str">
         <f t="shared" si="16"/>
         <v>styNormXLatex</v>
       </c>
-      <c r="AK9" t="str">
+      <c r="AM9" t="str">
         <f t="shared" si="5"/>
         <v>styNormXChartDomain</v>
       </c>
-      <c r="AL9" t="str">
+      <c r="AN9" t="str">
         <f t="shared" si="6"/>
         <v>styNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="7"/>
         <v>9</v>
@@ -2068,7 +2128,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
@@ -2086,19 +2146,19 @@
         <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>29</v>
@@ -2107,10 +2167,10 @@
         <v>31</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>36</v>
@@ -2130,63 +2190,69 @@
       <c r="W10" s="1">
         <v>3</v>
       </c>
-      <c r="X10" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>156</v>
+      <c r="X10" s="1">
+        <v>-4</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>4</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB10">
+        <v>147</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD10">
         <v>0.01</v>
       </c>
-      <c r="AC10" t="str">
+      <c r="AE10" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD10" t="str">
+      <c r="AF10" t="str">
         <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
-      <c r="AE10" t="str">
+      <c r="AG10" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,.6,3, 1,-1,-.6), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(0,2),</v>
       </c>
-      <c r="AF10" t="str">
+      <c r="AH10" t="str">
         <f t="shared" si="3"/>
         <v>fullNormXParamTransform</v>
       </c>
-      <c r="AG10" t="str">
+      <c r="AI10" t="str">
         <f t="shared" si="4"/>
         <v>fullNormXPDF</v>
       </c>
-      <c r="AH10" t="str">
+      <c r="AJ10" t="str">
         <f t="shared" si="14"/>
         <v>fullNormXPlotDistr</v>
       </c>
-      <c r="AI10" t="str">
+      <c r="AK10" t="str">
         <f t="shared" si="15"/>
         <v>fullNormXDraws</v>
       </c>
-      <c r="AJ10" t="str">
+      <c r="AL10" t="str">
         <f t="shared" si="16"/>
         <v>fullNormXLatex</v>
       </c>
-      <c r="AK10" t="str">
+      <c r="AM10" t="str">
         <f t="shared" si="5"/>
         <v>fullNormXChartDomain</v>
       </c>
-      <c r="AL10" t="str">
+      <c r="AN10" t="str">
         <f t="shared" si="6"/>
         <v>fullNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="7"/>
         <v>10</v>
@@ -2195,10 +2261,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -2213,19 +2279,19 @@
         <v>21</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>92</v>
+        <v>165</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>29</v>
@@ -2257,63 +2323,69 @@
       <c r="W11" s="1">
         <v>0.5</v>
       </c>
-      <c r="X11" s="1" t="s">
+      <c r="X11" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Z11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Y11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z11" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD11">
         <v>0.01</v>
       </c>
-      <c r="AC11" t="str">
+      <c r="AE11" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD11" t="str">
+      <c r="AF11" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AE11" t="str">
+      <c r="AG11" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AF11" t="str">
+      <c r="AH11" t="str">
         <f t="shared" si="3"/>
         <v>logNormParamTransform</v>
       </c>
-      <c r="AG11" t="str">
+      <c r="AI11" t="str">
         <f t="shared" si="4"/>
         <v>logNormPDF</v>
       </c>
-      <c r="AH11" t="str">
+      <c r="AJ11" t="str">
         <f t="shared" si="14"/>
         <v>logNormPlotDistr</v>
       </c>
-      <c r="AI11" t="str">
+      <c r="AK11" t="str">
         <f t="shared" si="15"/>
         <v>logNormDraws</v>
       </c>
-      <c r="AJ11" t="str">
+      <c r="AL11" t="str">
         <f t="shared" si="16"/>
         <v>logNormLatex</v>
       </c>
-      <c r="AK11" t="str">
+      <c r="AM11" t="str">
         <f t="shared" si="5"/>
         <v>logNormChartDomain</v>
       </c>
-      <c r="AL11" t="str">
+      <c r="AN11" t="str">
         <f t="shared" si="6"/>
         <v>logNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="7"/>
         <v>11</v>
@@ -2322,10 +2394,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -2340,19 +2412,19 @@
         <v>21</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>93</v>
+        <v>166</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>29</v>
@@ -2384,63 +2456,69 @@
       <c r="W12" s="1">
         <v>0.5</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="X12" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Z12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Y12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD12">
         <v>0.01</v>
       </c>
-      <c r="AC12" t="str">
+      <c r="AE12" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD12" t="str">
+      <c r="AF12" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AE12" t="str">
+      <c r="AG12" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AF12" t="str">
+      <c r="AH12" t="str">
         <f t="shared" si="3"/>
         <v>logNormXParamTransform</v>
       </c>
-      <c r="AG12" t="str">
+      <c r="AI12" t="str">
         <f t="shared" si="4"/>
         <v>logNormXPDF</v>
       </c>
-      <c r="AH12" t="str">
+      <c r="AJ12" t="str">
         <f t="shared" si="14"/>
         <v>logNormXPlotDistr</v>
       </c>
-      <c r="AI12" t="str">
+      <c r="AK12" t="str">
         <f t="shared" si="15"/>
         <v>logNormXDraws</v>
       </c>
-      <c r="AJ12" t="str">
+      <c r="AL12" t="str">
         <f t="shared" si="16"/>
         <v>logNormXLatex</v>
       </c>
-      <c r="AK12" t="str">
+      <c r="AM12" t="str">
         <f t="shared" si="5"/>
         <v>logNormXChartDomain</v>
       </c>
-      <c r="AL12" t="str">
+      <c r="AN12" t="str">
         <f t="shared" si="6"/>
         <v>logNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="7"/>
         <v>12</v>
@@ -2467,19 +2545,19 @@
         <v>20</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>30</v>
@@ -2511,63 +2589,69 @@
       <c r="W13" s="1">
         <v>20</v>
       </c>
-      <c r="X13" s="1" t="s">
+      <c r="X13" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Y13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD13">
         <v>0.01</v>
       </c>
-      <c r="AC13" t="str">
+      <c r="AE13" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;lambda;"</v>
       </c>
-      <c r="AD13" t="str">
+      <c r="AF13" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AE13" t="str">
+      <c r="AG13" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =1, maxVal = 20, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AF13" t="str">
+      <c r="AH13" t="str">
         <f t="shared" si="3"/>
         <v>poisParamTransform</v>
       </c>
-      <c r="AG13" t="str">
+      <c r="AI13" t="str">
         <f t="shared" si="4"/>
         <v>poisPDF</v>
       </c>
-      <c r="AH13" t="str">
+      <c r="AJ13" t="str">
         <f t="shared" si="14"/>
         <v>poisPlotDistr</v>
       </c>
-      <c r="AI13" t="str">
+      <c r="AK13" t="str">
         <f t="shared" si="15"/>
         <v>poisDraws</v>
       </c>
-      <c r="AJ13" t="str">
+      <c r="AL13" t="str">
         <f t="shared" si="16"/>
         <v>poisLatex</v>
       </c>
-      <c r="AK13" t="str">
+      <c r="AM13" t="str">
         <f t="shared" si="5"/>
         <v>poisChartDomain</v>
       </c>
-      <c r="AL13" t="str">
+      <c r="AN13" t="str">
         <f t="shared" si="6"/>
         <v>poisLikelihoodFun</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="7"/>
         <v>13</v>
@@ -2576,7 +2660,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>0</v>
@@ -2594,19 +2678,19 @@
         <v>20</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>29</v>
@@ -2638,63 +2722,69 @@
       <c r="W14" s="1">
         <v>3</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="X14" s="1">
+        <v>-1.25</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Y14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB14">
+      <c r="AB14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD14">
         <v>0.01</v>
       </c>
-      <c r="AC14" t="str">
+      <c r="AE14" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD14" t="str">
+      <c r="AF14" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AE14" t="str">
+      <c r="AG14" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AF14" t="str">
+      <c r="AH14" t="str">
         <f t="shared" si="3"/>
         <v>poisExpParamTransform</v>
       </c>
-      <c r="AG14" t="str">
+      <c r="AI14" t="str">
         <f t="shared" si="4"/>
         <v>poisExpPDF</v>
       </c>
-      <c r="AH14" t="str">
+      <c r="AJ14" t="str">
         <f t="shared" si="14"/>
         <v>poisExpPlotDistr</v>
       </c>
-      <c r="AI14" t="str">
+      <c r="AK14" t="str">
         <f t="shared" si="15"/>
         <v>poisExpDraws</v>
       </c>
-      <c r="AJ14" t="str">
+      <c r="AL14" t="str">
         <f t="shared" si="16"/>
         <v>poisExpLatex</v>
       </c>
-      <c r="AK14" t="str">
+      <c r="AM14" t="str">
         <f t="shared" si="5"/>
         <v>poisExpChartDomain</v>
       </c>
-      <c r="AL14" t="str">
+      <c r="AN14" t="str">
         <f t="shared" si="6"/>
         <v>poisExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="7"/>
         <v>14</v>
@@ -2703,7 +2793,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>0</v>
@@ -2721,19 +2811,19 @@
         <v>20</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>29</v>
@@ -2765,63 +2855,69 @@
       <c r="W15" s="1">
         <v>3</v>
       </c>
-      <c r="X15" s="1" t="s">
+      <c r="X15" s="1">
+        <v>-1.25</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z15" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB15">
+      <c r="AB15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD15">
         <v>0.01</v>
       </c>
-      <c r="AC15" t="str">
+      <c r="AE15" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD15" t="str">
+      <c r="AF15" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AE15" t="str">
+      <c r="AG15" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AF15" t="str">
+      <c r="AH15" t="str">
         <f t="shared" si="3"/>
         <v>poisExpXParamTransform</v>
       </c>
-      <c r="AG15" t="str">
+      <c r="AI15" t="str">
         <f t="shared" si="4"/>
         <v>poisExpXPDF</v>
       </c>
-      <c r="AH15" t="str">
+      <c r="AJ15" t="str">
         <f t="shared" si="14"/>
         <v>poisExpXPlotDistr</v>
       </c>
-      <c r="AI15" t="str">
+      <c r="AK15" t="str">
         <f t="shared" si="15"/>
         <v>poisExpXDraws</v>
       </c>
-      <c r="AJ15" t="str">
+      <c r="AL15" t="str">
         <f t="shared" si="16"/>
         <v>poisExpXLatex</v>
       </c>
-      <c r="AK15" t="str">
+      <c r="AM15" t="str">
         <f t="shared" si="5"/>
         <v>poisExpXChartDomain</v>
       </c>
-      <c r="AL15" t="str">
+      <c r="AN15" t="str">
         <f t="shared" si="6"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="7"/>
         <v>15</v>
@@ -2830,7 +2926,7 @@
         <v>76</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>0</v>
@@ -2848,19 +2944,19 @@
         <v>21</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>82</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>29</v>
@@ -2869,10 +2965,10 @@
         <v>30</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>36</v>
@@ -2892,63 +2988,69 @@
       <c r="W16" s="1">
         <v>1.5</v>
       </c>
-      <c r="X16" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y16" s="1" t="s">
-        <v>158</v>
+      <c r="X16" s="1">
+        <v>-1.25</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>2.5</v>
       </c>
       <c r="Z16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AA16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB16">
+      <c r="AC16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD16">
         <v>0.01</v>
       </c>
-      <c r="AC16" t="str">
+      <c r="AE16" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD16" t="str">
+      <c r="AF16" t="str">
         <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
-      <c r="AE16" t="str">
+      <c r="AG16" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 1.5, startVals = c(.25,.2,.25,0), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm", sigmaScale =c(1,2),</v>
       </c>
-      <c r="AF16" t="str">
+      <c r="AH16" t="str">
         <f>$B16&amp;"ParamTransform"</f>
         <v>negBinomXParamTransform</v>
       </c>
-      <c r="AG16" t="str">
+      <c r="AI16" t="str">
         <f>$B16&amp;"PDF"</f>
         <v>negBinomXPDF</v>
       </c>
-      <c r="AH16" t="str">
+      <c r="AJ16" t="str">
         <f t="shared" si="14"/>
         <v>negBinomXPlotDistr</v>
       </c>
-      <c r="AI16" t="str">
+      <c r="AK16" t="str">
         <f t="shared" si="15"/>
         <v>negBinomXDraws</v>
       </c>
-      <c r="AJ16" t="str">
+      <c r="AL16" t="str">
         <f t="shared" si="16"/>
         <v>negBinomXLatex</v>
       </c>
-      <c r="AK16" t="str">
+      <c r="AM16" t="str">
         <f>$B16&amp;"ChartDomain"</f>
         <v>negBinomXChartDomain</v>
       </c>
-      <c r="AL16" t="str">
+      <c r="AN16" t="str">
         <f>$B16&amp;"LikelihoodFun"</f>
         <v>negBinomXLikelihoodFun</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="7"/>
         <v>16</v>
@@ -2975,19 +3077,19 @@
         <v>21</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>30</v>
@@ -3019,63 +3121,69 @@
       <c r="W17" s="1">
         <v>1.5</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="X17" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="Z17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Y17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z17" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB17">
+      <c r="AB17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD17">
         <v>0.01</v>
       </c>
-      <c r="AC17" t="str">
+      <c r="AE17" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;lambda;"</v>
       </c>
-      <c r="AD17" t="str">
+      <c r="AF17" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AE17" t="str">
+      <c r="AG17" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AF17" t="str">
+      <c r="AH17" t="str">
         <f t="shared" si="3"/>
         <v>expParamTransform</v>
       </c>
-      <c r="AG17" t="str">
+      <c r="AI17" t="str">
         <f t="shared" si="4"/>
         <v>expPDF</v>
       </c>
-      <c r="AH17" t="str">
+      <c r="AJ17" t="str">
         <f t="shared" si="14"/>
         <v>expPlotDistr</v>
       </c>
-      <c r="AI17" t="str">
+      <c r="AK17" t="str">
         <f t="shared" si="15"/>
         <v>expDraws</v>
       </c>
-      <c r="AJ17" t="str">
+      <c r="AL17" t="str">
         <f t="shared" si="16"/>
         <v>expLatex</v>
       </c>
-      <c r="AK17" t="str">
+      <c r="AM17" t="str">
         <f t="shared" si="5"/>
         <v>expChartDomain</v>
       </c>
-      <c r="AL17" t="str">
+      <c r="AN17" t="str">
         <f t="shared" si="6"/>
         <v>expLikelihoodFun</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="7"/>
         <v>17</v>
@@ -3084,7 +3192,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -3102,19 +3210,19 @@
         <v>21</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>29</v>
@@ -3146,63 +3254,69 @@
       <c r="W18" s="1">
         <v>2</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="X18" s="1">
+        <v>-3</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Y18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z18" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB18">
+      <c r="AB18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD18">
         <v>0.01</v>
       </c>
-      <c r="AC18" t="str">
+      <c r="AE18" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD18" t="str">
+      <c r="AF18" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="AE18" t="str">
+      <c r="AG18" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none", sigmaScale =NA,</v>
       </c>
-      <c r="AF18" t="str">
+      <c r="AH18" t="str">
         <f t="shared" si="3"/>
         <v>expExpParamTransform</v>
       </c>
-      <c r="AG18" t="str">
+      <c r="AI18" t="str">
         <f t="shared" si="4"/>
         <v>expExpPDF</v>
       </c>
-      <c r="AH18" t="str">
+      <c r="AJ18" t="str">
         <f t="shared" si="14"/>
         <v>expExpPlotDistr</v>
       </c>
-      <c r="AI18" t="str">
+      <c r="AK18" t="str">
         <f t="shared" si="15"/>
         <v>expExpDraws</v>
       </c>
-      <c r="AJ18" t="str">
+      <c r="AL18" t="str">
         <f t="shared" si="16"/>
         <v>expExpLatex</v>
       </c>
-      <c r="AK18" t="str">
+      <c r="AM18" t="str">
         <f t="shared" si="5"/>
         <v>expExpChartDomain</v>
       </c>
-      <c r="AL18" t="str">
+      <c r="AN18" t="str">
         <f t="shared" si="6"/>
         <v>expExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="7"/>
         <v>18</v>
@@ -3211,7 +3325,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -3229,19 +3343,19 @@
         <v>21</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>29</v>
@@ -3273,58 +3387,64 @@
       <c r="W19" s="1">
         <v>0.5</v>
       </c>
-      <c r="X19" s="1" t="s">
+      <c r="X19" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Z19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Y19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z19" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB19">
+      <c r="AB19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD19">
         <v>0.01</v>
       </c>
-      <c r="AC19" t="str">
+      <c r="AE19" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="AD19" t="str">
+      <c r="AF19" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="AE19" t="str">
+      <c r="AG19" t="str">
         <f t="shared" si="2"/>
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas", sigmaScale =NA,</v>
       </c>
-      <c r="AF19" t="str">
+      <c r="AH19" t="str">
         <f t="shared" si="3"/>
         <v>expExpXParamTransform</v>
       </c>
-      <c r="AG19" t="str">
+      <c r="AI19" t="str">
         <f t="shared" si="4"/>
         <v>expExpXPDF</v>
       </c>
-      <c r="AH19" t="str">
+      <c r="AJ19" t="str">
         <f t="shared" si="14"/>
         <v>expExpXPlotDistr</v>
       </c>
-      <c r="AI19" t="str">
+      <c r="AK19" t="str">
         <f t="shared" si="15"/>
         <v>expExpXDraws</v>
       </c>
-      <c r="AJ19" t="str">
+      <c r="AL19" t="str">
         <f t="shared" si="16"/>
         <v>expExpXLatex</v>
       </c>
-      <c r="AK19" t="str">
+      <c r="AM19" t="str">
         <f t="shared" si="5"/>
         <v>expExpXChartDomain</v>
       </c>
-      <c r="AL19" t="str">
+      <c r="AN19" t="str">
         <f t="shared" si="6"/>
         <v>expExpXLikelihoodFun</v>
       </c>

</xml_diff>

<commit_message>
first round of MLE tutorial
</commit_message>
<xml_diff>
--- a/Config/DistrNames.xlsx
+++ b/Config/DistrNames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zagre\Documents\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B950AA94-1788-479E-BF2E-336F77789C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F01CAFB-A046-42D2-8C57-2934F879EDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="166">
   <si>
     <t>Poisson</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t>Bernoulli (Logit, X)</t>
-  </si>
-  <si>
-    <t>list("Normal (X)", "Stylized Normal (X)","Stylized Normal")</t>
   </si>
   <si>
     <t>Stylized Normal</t>
@@ -904,37 +901,37 @@
   <dimension ref="A1:AN19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="11" width="31.140625" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" customWidth="1"/>
+    <col min="10" max="11" width="31.1796875" customWidth="1"/>
+    <col min="13" max="13" width="15.54296875" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="20" max="21" width="9.42578125" customWidth="1"/>
-    <col min="22" max="22" width="6.140625" customWidth="1"/>
-    <col min="23" max="25" width="4.28515625" customWidth="1"/>
-    <col min="26" max="29" width="7.140625" customWidth="1"/>
+    <col min="20" max="21" width="9.453125" customWidth="1"/>
+    <col min="22" max="22" width="6.1796875" customWidth="1"/>
+    <col min="23" max="25" width="4.26953125" customWidth="1"/>
+    <col min="26" max="29" width="7.1796875" customWidth="1"/>
     <col min="30" max="30" width="6" customWidth="1"/>
-    <col min="31" max="32" width="4.28515625" customWidth="1"/>
+    <col min="31" max="32" width="4.26953125" customWidth="1"/>
     <col min="33" max="33" width="16" customWidth="1"/>
     <col min="34" max="35" width="26" customWidth="1"/>
-    <col min="36" max="36" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="15.5703125" customWidth="1"/>
+    <col min="36" max="36" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -945,16 +942,16 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
         <v>105</v>
       </c>
-      <c r="F1" t="s">
-        <v>106</v>
-      </c>
       <c r="G1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
@@ -966,25 +963,25 @@
         <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L1" t="s">
         <v>34</v>
       </c>
       <c r="M1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N1" t="s">
         <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R1" t="s">
         <v>32</v>
@@ -996,7 +993,7 @@
         <v>62</v>
       </c>
       <c r="U1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V1" t="s">
         <v>46</v>
@@ -1005,10 +1002,10 @@
         <v>47</v>
       </c>
       <c r="X1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y1" t="s">
         <v>155</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>156</v>
       </c>
       <c r="Z1" t="s">
         <v>48</v>
@@ -1017,10 +1014,10 @@
         <v>80</v>
       </c>
       <c r="AB1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AC1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AD1" t="s">
         <v>49</v>
@@ -1035,16 +1032,16 @@
         <v>52</v>
       </c>
       <c r="AH1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AI1" t="s">
         <v>65</v>
       </c>
       <c r="AJ1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AK1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AL1" t="s">
         <v>19</v>
@@ -1056,7 +1053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1082,19 +1079,19 @@
         <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>28</v>
@@ -1188,7 +1185,7 @@
         <v>bernLikelihoodFun</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1215,19 +1212,19 @@
         <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>29</v>
@@ -1321,7 +1318,7 @@
         <v>bernLogitLikelihoodFun</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A19" si="7">A3+1</f>
         <v>3</v>
@@ -1348,19 +1345,19 @@
         <v>20</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>29</v>
@@ -1399,7 +1396,7 @@
         <v>5</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>61</v>
@@ -1454,16 +1451,16 @@
         <v>bernLogitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -1481,19 +1478,19 @@
         <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>29</v>
@@ -1587,19 +1584,19 @@
         <v>bernProbitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -1614,19 +1611,19 @@
         <v>20</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>29</v>
@@ -1635,16 +1632,16 @@
         <v>31</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>61</v>
@@ -1665,16 +1662,16 @@
         <v>4</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AD6">
         <v>0.01</v>
@@ -1720,19 +1717,19 @@
         <v>orderedProbitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -1747,19 +1744,19 @@
         <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>29</v>
@@ -1768,16 +1765,16 @@
         <v>31</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>61</v>
@@ -1798,16 +1795,16 @@
         <v>4</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AD7">
         <v>0.01</v>
@@ -1853,7 +1850,7 @@
         <v>orderedLogitXLikelihoodFun</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="7"/>
         <v>7</v>
@@ -1862,7 +1859,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
@@ -1880,19 +1877,19 @@
         <v>21</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>29</v>
@@ -1916,7 +1913,7 @@
         <v>63</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V8" s="1">
         <v>-4</v>
@@ -1986,7 +1983,7 @@
         <v>styNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="7"/>
         <v>8</v>
@@ -1995,7 +1992,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
@@ -2013,19 +2010,19 @@
         <v>21</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>29</v>
@@ -2049,7 +2046,7 @@
         <v>63</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V9" s="1">
         <v>-3</v>
@@ -2064,7 +2061,7 @@
         <v>4</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA9" s="1" t="s">
         <v>61</v>
@@ -2119,7 +2116,7 @@
         <v>styNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="7"/>
         <v>9</v>
@@ -2128,7 +2125,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
@@ -2146,19 +2143,19 @@
         <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>29</v>
@@ -2167,10 +2164,10 @@
         <v>31</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>36</v>
@@ -2197,13 +2194,13 @@
         <v>4</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AC10" s="1" t="s">
         <v>61</v>
@@ -2252,7 +2249,7 @@
         <v>fullNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="7"/>
         <v>10</v>
@@ -2261,10 +2258,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -2279,19 +2276,19 @@
         <v>21</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>29</v>
@@ -2385,7 +2382,7 @@
         <v>logNormLikelihoodFun</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="7"/>
         <v>11</v>
@@ -2394,10 +2391,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -2412,19 +2409,19 @@
         <v>21</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>29</v>
@@ -2518,7 +2515,7 @@
         <v>logNormXLikelihoodFun</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="7"/>
         <v>12</v>
@@ -2545,19 +2542,19 @@
         <v>20</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>30</v>
@@ -2651,7 +2648,7 @@
         <v>poisLikelihoodFun</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="7"/>
         <v>13</v>
@@ -2660,7 +2657,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>0</v>
@@ -2678,19 +2675,19 @@
         <v>20</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>29</v>
@@ -2784,7 +2781,7 @@
         <v>poisExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="7"/>
         <v>14</v>
@@ -2793,7 +2790,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>0</v>
@@ -2811,19 +2808,19 @@
         <v>20</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>29</v>
@@ -2917,7 +2914,7 @@
         <v>poisExpXLikelihoodFun</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="7"/>
         <v>15</v>
@@ -2926,7 +2923,7 @@
         <v>76</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>0</v>
@@ -2944,19 +2941,19 @@
         <v>21</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>82</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>29</v>
@@ -2965,10 +2962,10 @@
         <v>30</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>36</v>
@@ -2995,10 +2992,10 @@
         <v>2.5</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AB16" s="1" t="s">
         <v>83</v>
@@ -3050,7 +3047,7 @@
         <v>negBinomXLikelihoodFun</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="7"/>
         <v>16</v>
@@ -3077,19 +3074,19 @@
         <v>21</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>30</v>
@@ -3183,7 +3180,7 @@
         <v>expLikelihoodFun</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="7"/>
         <v>17</v>
@@ -3192,7 +3189,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -3210,19 +3207,19 @@
         <v>21</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>77</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>29</v>
@@ -3316,7 +3313,7 @@
         <v>expExpLikelihoodFun</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="7"/>
         <v>18</v>
@@ -3325,7 +3322,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -3343,19 +3340,19 @@
         <v>21</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>29</v>

</xml_diff>